<commit_message>
Tests added to the report
</commit_message>
<xml_diff>
--- a/Doc/Tests/liste_de_tests.xlsx
+++ b/Doc/Tests/liste_de_tests.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE92126F-63FF-412B-A5E3-24BDFB390D76}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D3D91A6-22F1-4A36-9F01-90FD2E45E405}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="128">
   <si>
     <t>Client</t>
   </si>
@@ -407,17 +407,24 @@
  partagé</t>
   </si>
   <si>
-    <t>Champs de la partie connexion parfois plus accessibles avec le curseur</t>
-  </si>
-  <si>
     <t>Entité à 
 tester</t>
   </si>
   <si>
-    <t>Client pas supprimé si dépendances avec autres tables (conflit DB/BLL)</t>
-  </si>
-  <si>
-    <t>Erreur de connexion toujours présente si déconnexion du client</t>
+    <t>Erreur de connexion toujours 
+présente si déconnexion du client</t>
+  </si>
+  <si>
+    <t>Champs de la partie connexion
+plus accessibles avec le curseur</t>
+  </si>
+  <si>
+    <t>Champs de la partie connexion 
+plus accessibles avec le curseur</t>
+  </si>
+  <si>
+    <t>Client pas supprimé si dépendances 
+avec autres tables (conflit DB/BLL)</t>
   </si>
 </sst>
 </file>
@@ -558,7 +565,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -660,48 +667,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -760,7 +725,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -769,17 +733,74 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1101,7 +1122,7 @@
     <col min="2" max="2" width="22.77734375" customWidth="1"/>
     <col min="3" max="3" width="65.77734375" customWidth="1"/>
     <col min="4" max="5" width="7.77734375" style="19" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="32.33203125" style="78" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="32.33203125" style="64" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
@@ -1114,21 +1135,21 @@
       <c r="C1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="61" t="s">
+      <c r="D1" s="47" t="s">
         <v>97</v>
       </c>
-      <c r="E1" s="61" t="s">
+      <c r="E1" s="47" t="s">
         <v>98</v>
       </c>
-      <c r="F1" s="63" t="s">
+      <c r="F1" s="49" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="53" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="48" t="s">
+      <c r="A2" s="76" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="80" t="s">
         <v>14</v>
       </c>
       <c r="C2" s="20" t="s">
@@ -1140,11 +1161,11 @@
       <c r="E2" s="37">
         <v>0</v>
       </c>
-      <c r="F2" s="64"/>
+      <c r="F2" s="50"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="54"/>
-      <c r="B3" s="48"/>
+      <c r="A3" s="83"/>
+      <c r="B3" s="80"/>
       <c r="C3" s="22" t="s">
         <v>8</v>
       </c>
@@ -1154,7 +1175,7 @@
       <c r="E3" s="23">
         <v>0</v>
       </c>
-      <c r="F3" s="65"/>
+      <c r="F3" s="51"/>
       <c r="H3" s="8">
         <v>0</v>
       </c>
@@ -1163,8 +1184,8 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="54"/>
-      <c r="B4" s="48"/>
+      <c r="A4" s="83"/>
+      <c r="B4" s="80"/>
       <c r="C4" s="22" t="s">
         <v>9</v>
       </c>
@@ -1174,7 +1195,7 @@
       <c r="E4" s="23">
         <v>0</v>
       </c>
-      <c r="F4" s="65"/>
+      <c r="F4" s="51"/>
       <c r="H4" s="8">
         <v>1</v>
       </c>
@@ -1183,8 +1204,8 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="54"/>
-      <c r="B5" s="48"/>
+      <c r="A5" s="83"/>
+      <c r="B5" s="80"/>
       <c r="C5" s="22" t="s">
         <v>10</v>
       </c>
@@ -1194,11 +1215,11 @@
       <c r="E5" s="23">
         <v>0</v>
       </c>
-      <c r="F5" s="65"/>
+      <c r="F5" s="51"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="54"/>
-      <c r="B6" s="48"/>
+      <c r="A6" s="83"/>
+      <c r="B6" s="80"/>
       <c r="C6" s="24" t="s">
         <v>11</v>
       </c>
@@ -1208,11 +1229,11 @@
       <c r="E6" s="25">
         <v>0</v>
       </c>
-      <c r="F6" s="66"/>
+      <c r="F6" s="52"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="54"/>
-      <c r="B7" s="48"/>
+      <c r="A7" s="83"/>
+      <c r="B7" s="80"/>
       <c r="C7" s="24" t="s">
         <v>12</v>
       </c>
@@ -1222,11 +1243,11 @@
       <c r="E7" s="25">
         <v>1</v>
       </c>
-      <c r="F7" s="66"/>
+      <c r="F7" s="52"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="54"/>
-      <c r="B8" s="49"/>
+      <c r="A8" s="83"/>
+      <c r="B8" s="81"/>
       <c r="C8" s="29" t="s">
         <v>24</v>
       </c>
@@ -1236,11 +1257,11 @@
       <c r="E8" s="30">
         <v>1</v>
       </c>
-      <c r="F8" s="80"/>
+      <c r="F8" s="66"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="54"/>
-      <c r="B9" s="50" t="s">
+      <c r="A9" s="83"/>
+      <c r="B9" s="73" t="s">
         <v>15</v>
       </c>
       <c r="C9" s="31" t="s">
@@ -1252,11 +1273,11 @@
       <c r="E9" s="32">
         <v>0</v>
       </c>
-      <c r="F9" s="67"/>
+      <c r="F9" s="53"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="54"/>
-      <c r="B10" s="51"/>
+      <c r="A10" s="83"/>
+      <c r="B10" s="84"/>
       <c r="C10" s="33" t="s">
         <v>13</v>
       </c>
@@ -1266,11 +1287,11 @@
       <c r="E10" s="34">
         <v>0</v>
       </c>
-      <c r="F10" s="62"/>
+      <c r="F10" s="48"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="54"/>
-      <c r="B11" s="51"/>
+      <c r="A11" s="83"/>
+      <c r="B11" s="84"/>
       <c r="C11" s="33" t="s">
         <v>19</v>
       </c>
@@ -1280,11 +1301,11 @@
       <c r="E11" s="34">
         <v>0</v>
       </c>
-      <c r="F11" s="62"/>
+      <c r="F11" s="48"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="54"/>
-      <c r="B12" s="51"/>
+      <c r="A12" s="83"/>
+      <c r="B12" s="84"/>
       <c r="C12" s="33" t="s">
         <v>20</v>
       </c>
@@ -1294,11 +1315,11 @@
       <c r="E12" s="34">
         <v>0</v>
       </c>
-      <c r="F12" s="62"/>
+      <c r="F12" s="48"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="54"/>
-      <c r="B13" s="51"/>
+      <c r="A13" s="83"/>
+      <c r="B13" s="84"/>
       <c r="C13" s="33" t="s">
         <v>21</v>
       </c>
@@ -1308,11 +1329,11 @@
       <c r="E13" s="34">
         <v>0</v>
       </c>
-      <c r="F13" s="62"/>
+      <c r="F13" s="48"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="54"/>
-      <c r="B14" s="51"/>
+      <c r="A14" s="83"/>
+      <c r="B14" s="84"/>
       <c r="C14" s="33" t="s">
         <v>23</v>
       </c>
@@ -1322,11 +1343,11 @@
       <c r="E14" s="34">
         <v>1</v>
       </c>
-      <c r="F14" s="62"/>
+      <c r="F14" s="48"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="54"/>
-      <c r="B15" s="51"/>
+      <c r="A15" s="83"/>
+      <c r="B15" s="84"/>
       <c r="C15" s="33" t="s">
         <v>22</v>
       </c>
@@ -1336,11 +1357,11 @@
       <c r="E15" s="34">
         <v>1</v>
       </c>
-      <c r="F15" s="62"/>
+      <c r="F15" s="48"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="54"/>
-      <c r="B16" s="51"/>
+      <c r="A16" s="83"/>
+      <c r="B16" s="84"/>
       <c r="C16" s="27" t="s">
         <v>26</v>
       </c>
@@ -1350,11 +1371,11 @@
       <c r="E16" s="28">
         <v>1</v>
       </c>
-      <c r="F16" s="73"/>
+      <c r="F16" s="59"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="54"/>
-      <c r="B17" s="52"/>
+      <c r="A17" s="83"/>
+      <c r="B17" s="75"/>
       <c r="C17" s="3" t="s">
         <v>27</v>
       </c>
@@ -1364,11 +1385,11 @@
       <c r="E17" s="11">
         <v>1</v>
       </c>
-      <c r="F17" s="68"/>
+      <c r="F17" s="54"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="54"/>
-      <c r="B18" s="47" t="s">
+      <c r="A18" s="83"/>
+      <c r="B18" s="79" t="s">
         <v>28</v>
       </c>
       <c r="C18" s="20" t="s">
@@ -1380,11 +1401,11 @@
       <c r="E18" s="21">
         <v>0</v>
       </c>
-      <c r="F18" s="64"/>
+      <c r="F18" s="50"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" s="54"/>
-      <c r="B19" s="57"/>
+      <c r="A19" s="83"/>
+      <c r="B19" s="82"/>
       <c r="C19" s="22" t="s">
         <v>31</v>
       </c>
@@ -1394,11 +1415,11 @@
       <c r="E19" s="23">
         <v>1</v>
       </c>
-      <c r="F19" s="65"/>
+      <c r="F19" s="51"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="54"/>
-      <c r="B20" s="49"/>
+      <c r="A20" s="83"/>
+      <c r="B20" s="81"/>
       <c r="C20" s="7" t="s">
         <v>30</v>
       </c>
@@ -1408,10 +1429,10 @@
       <c r="E20" s="9">
         <v>1</v>
       </c>
-      <c r="F20" s="72"/>
+      <c r="F20" s="58"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" s="54"/>
+      <c r="A21" s="83"/>
       <c r="B21" s="4" t="s">
         <v>17</v>
       </c>
@@ -1424,13 +1445,13 @@
       <c r="E21" s="13">
         <v>1</v>
       </c>
-      <c r="F21" s="76" t="s">
+      <c r="F21" s="62" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" s="54"/>
-      <c r="B22" s="47" t="s">
+      <c r="A22" s="83"/>
+      <c r="B22" s="79" t="s">
         <v>16</v>
       </c>
       <c r="C22" s="20" t="s">
@@ -1442,13 +1463,13 @@
       <c r="E22" s="21">
         <v>1</v>
       </c>
-      <c r="F22" s="64" t="s">
+      <c r="F22" s="50" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23" s="54"/>
-      <c r="B23" s="57"/>
+      <c r="A23" s="83"/>
+      <c r="B23" s="82"/>
       <c r="C23" s="6" t="s">
         <v>34</v>
       </c>
@@ -1458,7 +1479,7 @@
       <c r="E23" s="12">
         <v>0</v>
       </c>
-      <c r="F23" s="74" t="s">
+      <c r="F23" s="60" t="s">
         <v>111</v>
       </c>
     </row>
@@ -1468,13 +1489,13 @@
       <c r="C24" s="14"/>
       <c r="D24" s="36"/>
       <c r="E24" s="36"/>
-      <c r="F24" s="71"/>
+      <c r="F24" s="57"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25" s="53" t="s">
-        <v>1</v>
-      </c>
-      <c r="B25" s="47" t="s">
+      <c r="A25" s="76" t="s">
+        <v>1</v>
+      </c>
+      <c r="B25" s="79" t="s">
         <v>35</v>
       </c>
       <c r="C25" s="20" t="s">
@@ -1486,11 +1507,11 @@
       <c r="E25" s="21">
         <v>1</v>
       </c>
-      <c r="F25" s="64"/>
+      <c r="F25" s="50"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26" s="60"/>
-      <c r="B26" s="48"/>
+      <c r="A26" s="77"/>
+      <c r="B26" s="80"/>
       <c r="C26" s="22" t="s">
         <v>50</v>
       </c>
@@ -1500,11 +1521,11 @@
       <c r="E26" s="23">
         <v>1</v>
       </c>
-      <c r="F26" s="65"/>
+      <c r="F26" s="51"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A27" s="54"/>
-      <c r="B27" s="49"/>
+      <c r="A27" s="83"/>
+      <c r="B27" s="81"/>
       <c r="C27" s="7" t="s">
         <v>37</v>
       </c>
@@ -1514,11 +1535,11 @@
       <c r="E27" s="9">
         <v>1</v>
       </c>
-      <c r="F27" s="72"/>
+      <c r="F27" s="58"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A28" s="54"/>
-      <c r="B28" s="50" t="s">
+      <c r="A28" s="83"/>
+      <c r="B28" s="73" t="s">
         <v>36</v>
       </c>
       <c r="C28" s="31" t="s">
@@ -1530,11 +1551,11 @@
       <c r="E28" s="32">
         <v>1</v>
       </c>
-      <c r="F28" s="67"/>
+      <c r="F28" s="53"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A29" s="54"/>
-      <c r="B29" s="56"/>
+      <c r="A29" s="83"/>
+      <c r="B29" s="74"/>
       <c r="C29" s="27" t="s">
         <v>102</v>
       </c>
@@ -1544,11 +1565,11 @@
       <c r="E29" s="28">
         <v>1</v>
       </c>
-      <c r="F29" s="73"/>
+      <c r="F29" s="59"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A30" s="54"/>
-      <c r="B30" s="52"/>
+      <c r="A30" s="83"/>
+      <c r="B30" s="75"/>
       <c r="C30" s="3" t="s">
         <v>103</v>
       </c>
@@ -1558,11 +1579,11 @@
       <c r="E30" s="11">
         <v>1</v>
       </c>
-      <c r="F30" s="68"/>
+      <c r="F30" s="54"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A31" s="54"/>
-      <c r="B31" s="57" t="s">
+      <c r="A31" s="83"/>
+      <c r="B31" s="82" t="s">
         <v>16</v>
       </c>
       <c r="C31" s="20" t="s">
@@ -1574,11 +1595,11 @@
       <c r="E31" s="21">
         <v>1</v>
       </c>
-      <c r="F31" s="64"/>
+      <c r="F31" s="50"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A32" s="54"/>
-      <c r="B32" s="57"/>
+      <c r="A32" s="83"/>
+      <c r="B32" s="82"/>
       <c r="C32" s="22" t="s">
         <v>112</v>
       </c>
@@ -1588,11 +1609,11 @@
       <c r="E32" s="23">
         <v>0</v>
       </c>
-      <c r="F32" s="65"/>
+      <c r="F32" s="51"/>
     </row>
     <row r="33" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A33" s="55"/>
-      <c r="B33" s="57"/>
+      <c r="A33" s="78"/>
+      <c r="B33" s="82"/>
       <c r="C33" s="15" t="s">
         <v>42</v>
       </c>
@@ -1602,7 +1623,7 @@
       <c r="E33" s="12">
         <v>1</v>
       </c>
-      <c r="F33" s="74"/>
+      <c r="F33" s="60"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="14"/>
@@ -1610,13 +1631,13 @@
       <c r="C34" s="14"/>
       <c r="D34" s="36"/>
       <c r="E34" s="36"/>
-      <c r="F34" s="71"/>
+      <c r="F34" s="57"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A35" s="58" t="s">
+      <c r="A35" s="85" t="s">
         <v>49</v>
       </c>
-      <c r="B35" s="47" t="s">
+      <c r="B35" s="79" t="s">
         <v>35</v>
       </c>
       <c r="C35" s="20" t="s">
@@ -1628,11 +1649,11 @@
       <c r="E35" s="21">
         <v>0</v>
       </c>
-      <c r="F35" s="64"/>
+      <c r="F35" s="50"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A36" s="59"/>
-      <c r="B36" s="48"/>
+      <c r="A36" s="86"/>
+      <c r="B36" s="80"/>
       <c r="C36" s="22" t="s">
         <v>43</v>
       </c>
@@ -1642,11 +1663,11 @@
       <c r="E36" s="23">
         <v>1</v>
       </c>
-      <c r="F36" s="65"/>
+      <c r="F36" s="51"/>
     </row>
     <row r="37" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A37" s="54"/>
-      <c r="B37" s="49"/>
+      <c r="A37" s="83"/>
+      <c r="B37" s="81"/>
       <c r="C37" s="17" t="s">
         <v>44</v>
       </c>
@@ -1656,11 +1677,11 @@
       <c r="E37" s="9">
         <v>1</v>
       </c>
-      <c r="F37" s="72"/>
+      <c r="F37" s="58"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A38" s="54"/>
-      <c r="B38" s="50" t="s">
+      <c r="A38" s="83"/>
+      <c r="B38" s="73" t="s">
         <v>48</v>
       </c>
       <c r="C38" s="38" t="s">
@@ -1672,11 +1693,11 @@
       <c r="E38" s="18">
         <v>1</v>
       </c>
-      <c r="F38" s="75"/>
+      <c r="F38" s="61"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A39" s="54"/>
-      <c r="B39" s="52"/>
+      <c r="A39" s="83"/>
+      <c r="B39" s="75"/>
       <c r="C39" s="2" t="s">
         <v>61</v>
       </c>
@@ -1686,11 +1707,11 @@
       <c r="E39" s="18">
         <v>1</v>
       </c>
-      <c r="F39" s="75"/>
+      <c r="F39" s="61"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A40" s="54"/>
-      <c r="B40" s="47" t="s">
+      <c r="A40" s="83"/>
+      <c r="B40" s="79" t="s">
         <v>36</v>
       </c>
       <c r="C40" s="20" t="s">
@@ -1702,11 +1723,11 @@
       <c r="E40" s="21">
         <v>0</v>
       </c>
-      <c r="F40" s="64"/>
+      <c r="F40" s="50"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A41" s="54"/>
-      <c r="B41" s="48"/>
+      <c r="A41" s="83"/>
+      <c r="B41" s="80"/>
       <c r="C41" s="22" t="s">
         <v>45</v>
       </c>
@@ -1716,11 +1737,11 @@
       <c r="E41" s="23">
         <v>1</v>
       </c>
-      <c r="F41" s="65"/>
+      <c r="F41" s="51"/>
     </row>
     <row r="42" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A42" s="54"/>
-      <c r="B42" s="49"/>
+      <c r="A42" s="83"/>
+      <c r="B42" s="81"/>
       <c r="C42" s="17" t="s">
         <v>46</v>
       </c>
@@ -1730,10 +1751,10 @@
       <c r="E42" s="9">
         <v>1</v>
       </c>
-      <c r="F42" s="72"/>
+      <c r="F42" s="58"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A43" s="55"/>
+      <c r="A43" s="78"/>
       <c r="B43" s="39" t="s">
         <v>16</v>
       </c>
@@ -1746,7 +1767,7 @@
       <c r="E43" s="10">
         <v>1</v>
       </c>
-      <c r="F43" s="70"/>
+      <c r="F43" s="56"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" s="14"/>
@@ -1754,13 +1775,13 @@
       <c r="C44" s="14"/>
       <c r="D44" s="36"/>
       <c r="E44" s="36"/>
-      <c r="F44" s="71"/>
+      <c r="F44" s="57"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A45" s="53" t="s">
+      <c r="A45" s="76" t="s">
         <v>4</v>
       </c>
-      <c r="B45" s="47" t="s">
+      <c r="B45" s="79" t="s">
         <v>35</v>
       </c>
       <c r="C45" s="20" t="s">
@@ -1772,11 +1793,11 @@
       <c r="E45" s="21">
         <v>0</v>
       </c>
-      <c r="F45" s="64"/>
+      <c r="F45" s="50"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A46" s="54"/>
-      <c r="B46" s="48"/>
+      <c r="A46" s="83"/>
+      <c r="B46" s="80"/>
       <c r="C46" s="22" t="s">
         <v>52</v>
       </c>
@@ -1786,11 +1807,11 @@
       <c r="E46" s="23">
         <v>1</v>
       </c>
-      <c r="F46" s="65"/>
+      <c r="F46" s="51"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A47" s="54"/>
-      <c r="B47" s="48"/>
+      <c r="A47" s="83"/>
+      <c r="B47" s="80"/>
       <c r="C47" s="22" t="s">
         <v>53</v>
       </c>
@@ -1800,11 +1821,11 @@
       <c r="E47" s="23">
         <v>1</v>
       </c>
-      <c r="F47" s="65"/>
+      <c r="F47" s="51"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A48" s="54"/>
-      <c r="B48" s="49"/>
+      <c r="A48" s="83"/>
+      <c r="B48" s="81"/>
       <c r="C48" s="7" t="s">
         <v>54</v>
       </c>
@@ -1814,11 +1835,11 @@
       <c r="E48" s="9">
         <v>1</v>
       </c>
-      <c r="F48" s="72"/>
+      <c r="F48" s="58"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A49" s="54"/>
-      <c r="B49" s="56" t="s">
+      <c r="A49" s="83"/>
+      <c r="B49" s="74" t="s">
         <v>36</v>
       </c>
       <c r="C49" s="27" t="s">
@@ -1830,11 +1851,11 @@
       <c r="E49" s="28">
         <v>0</v>
       </c>
-      <c r="F49" s="73"/>
+      <c r="F49" s="59"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A50" s="54"/>
-      <c r="B50" s="56"/>
+      <c r="A50" s="83"/>
+      <c r="B50" s="74"/>
       <c r="C50" s="33" t="s">
         <v>55</v>
       </c>
@@ -1844,11 +1865,11 @@
       <c r="E50" s="34">
         <v>1</v>
       </c>
-      <c r="F50" s="62"/>
+      <c r="F50" s="48"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A51" s="54"/>
-      <c r="B51" s="56"/>
+      <c r="A51" s="83"/>
+      <c r="B51" s="74"/>
       <c r="C51" s="33" t="s">
         <v>56</v>
       </c>
@@ -1858,11 +1879,11 @@
       <c r="E51" s="34">
         <v>1</v>
       </c>
-      <c r="F51" s="62"/>
+      <c r="F51" s="48"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A52" s="54"/>
-      <c r="B52" s="52"/>
+      <c r="A52" s="83"/>
+      <c r="B52" s="75"/>
       <c r="C52" s="3" t="s">
         <v>57</v>
       </c>
@@ -1872,11 +1893,11 @@
       <c r="E52" s="11">
         <v>1</v>
       </c>
-      <c r="F52" s="68"/>
+      <c r="F52" s="54"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A53" s="54"/>
-      <c r="B53" s="57" t="s">
+      <c r="A53" s="83"/>
+      <c r="B53" s="82" t="s">
         <v>16</v>
       </c>
       <c r="C53" s="24" t="s">
@@ -1888,11 +1909,11 @@
       <c r="E53" s="25">
         <v>1</v>
       </c>
-      <c r="F53" s="66"/>
+      <c r="F53" s="52"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A54" s="55"/>
-      <c r="B54" s="57"/>
+      <c r="A54" s="78"/>
+      <c r="B54" s="82"/>
       <c r="C54" s="16" t="s">
         <v>59</v>
       </c>
@@ -1902,7 +1923,7 @@
       <c r="E54" s="12">
         <v>1</v>
       </c>
-      <c r="F54" s="74"/>
+      <c r="F54" s="60"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" s="14"/>
@@ -1910,13 +1931,13 @@
       <c r="C55" s="14"/>
       <c r="D55" s="36"/>
       <c r="E55" s="36"/>
-      <c r="F55" s="71"/>
+      <c r="F55" s="57"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A56" s="53" t="s">
+      <c r="A56" s="76" t="s">
         <v>3</v>
       </c>
-      <c r="B56" s="47" t="s">
+      <c r="B56" s="79" t="s">
         <v>35</v>
       </c>
       <c r="C56" s="20" t="s">
@@ -1928,11 +1949,11 @@
       <c r="E56" s="21">
         <v>0</v>
       </c>
-      <c r="F56" s="64"/>
+      <c r="F56" s="50"/>
     </row>
     <row r="57" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A57" s="54"/>
-      <c r="B57" s="48"/>
+      <c r="A57" s="83"/>
+      <c r="B57" s="80"/>
       <c r="C57" s="43" t="s">
         <v>62</v>
       </c>
@@ -1942,13 +1963,13 @@
       <c r="E57" s="23">
         <v>0</v>
       </c>
-      <c r="F57" s="65" t="s">
+      <c r="F57" s="51" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A58" s="54"/>
-      <c r="B58" s="48"/>
+      <c r="A58" s="83"/>
+      <c r="B58" s="80"/>
       <c r="C58" s="22" t="s">
         <v>63</v>
       </c>
@@ -1958,11 +1979,11 @@
       <c r="E58" s="23">
         <v>0</v>
       </c>
-      <c r="F58" s="65"/>
+      <c r="F58" s="51"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A59" s="54"/>
-      <c r="B59" s="49"/>
+      <c r="A59" s="83"/>
+      <c r="B59" s="81"/>
       <c r="C59" s="7" t="s">
         <v>64</v>
       </c>
@@ -1972,11 +1993,11 @@
       <c r="E59" s="9">
         <v>1</v>
       </c>
-      <c r="F59" s="72"/>
+      <c r="F59" s="58"/>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A60" s="54"/>
-      <c r="B60" s="50" t="s">
+      <c r="A60" s="83"/>
+      <c r="B60" s="73" t="s">
         <v>36</v>
       </c>
       <c r="C60" s="31" t="s">
@@ -1988,11 +2009,11 @@
       <c r="E60" s="32">
         <v>0</v>
       </c>
-      <c r="F60" s="67"/>
+      <c r="F60" s="53"/>
     </row>
     <row r="61" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A61" s="54"/>
-      <c r="B61" s="56"/>
+      <c r="A61" s="83"/>
+      <c r="B61" s="74"/>
       <c r="C61" s="44" t="s">
         <v>65</v>
       </c>
@@ -2002,13 +2023,13 @@
       <c r="E61" s="34">
         <v>0</v>
       </c>
-      <c r="F61" s="62" t="s">
+      <c r="F61" s="48" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A62" s="54"/>
-      <c r="B62" s="56"/>
+      <c r="A62" s="83"/>
+      <c r="B62" s="74"/>
       <c r="C62" s="33" t="s">
         <v>66</v>
       </c>
@@ -2018,11 +2039,11 @@
       <c r="E62" s="34">
         <v>0</v>
       </c>
-      <c r="F62" s="62"/>
+      <c r="F62" s="48"/>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A63" s="54"/>
-      <c r="B63" s="52"/>
+      <c r="A63" s="83"/>
+      <c r="B63" s="75"/>
       <c r="C63" s="3" t="s">
         <v>67</v>
       </c>
@@ -2032,11 +2053,11 @@
       <c r="E63" s="11">
         <v>1</v>
       </c>
-      <c r="F63" s="68"/>
+      <c r="F63" s="54"/>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A64" s="54"/>
-      <c r="B64" s="47" t="s">
+      <c r="A64" s="83"/>
+      <c r="B64" s="79" t="s">
         <v>74</v>
       </c>
       <c r="C64" s="20" t="s">
@@ -2048,11 +2069,11 @@
       <c r="E64" s="21">
         <v>1</v>
       </c>
-      <c r="F64" s="64"/>
+      <c r="F64" s="50"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A65" s="54"/>
-      <c r="B65" s="48"/>
+      <c r="A65" s="83"/>
+      <c r="B65" s="80"/>
       <c r="C65" s="22" t="s">
         <v>69</v>
       </c>
@@ -2062,11 +2083,11 @@
       <c r="E65" s="23">
         <v>1</v>
       </c>
-      <c r="F65" s="65"/>
+      <c r="F65" s="51"/>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A66" s="54"/>
-      <c r="B66" s="49"/>
+      <c r="A66" s="83"/>
+      <c r="B66" s="81"/>
       <c r="C66" s="7" t="s">
         <v>70</v>
       </c>
@@ -2076,11 +2097,11 @@
       <c r="E66" s="9">
         <v>1</v>
       </c>
-      <c r="F66" s="72"/>
+      <c r="F66" s="58"/>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A67" s="54"/>
-      <c r="B67" s="50" t="s">
+      <c r="A67" s="83"/>
+      <c r="B67" s="73" t="s">
         <v>96</v>
       </c>
       <c r="C67" s="31" t="s">
@@ -2092,11 +2113,11 @@
       <c r="E67" s="32">
         <v>1</v>
       </c>
-      <c r="F67" s="67"/>
+      <c r="F67" s="53"/>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A68" s="54"/>
-      <c r="B68" s="51"/>
+      <c r="A68" s="83"/>
+      <c r="B68" s="84"/>
       <c r="C68" s="33" t="s">
         <v>72</v>
       </c>
@@ -2106,11 +2127,11 @@
       <c r="E68" s="34">
         <v>1</v>
       </c>
-      <c r="F68" s="62"/>
+      <c r="F68" s="48"/>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A69" s="54"/>
-      <c r="B69" s="56"/>
+      <c r="A69" s="83"/>
+      <c r="B69" s="74"/>
       <c r="C69" s="40" t="s">
         <v>73</v>
       </c>
@@ -2120,11 +2141,11 @@
       <c r="E69" s="18">
         <v>1</v>
       </c>
-      <c r="F69" s="75"/>
+      <c r="F69" s="61"/>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A70" s="54"/>
-      <c r="B70" s="47" t="s">
+      <c r="A70" s="83"/>
+      <c r="B70" s="79" t="s">
         <v>16</v>
       </c>
       <c r="C70" s="20" t="s">
@@ -2136,11 +2157,11 @@
       <c r="E70" s="21">
         <v>1</v>
       </c>
-      <c r="F70" s="64"/>
+      <c r="F70" s="50"/>
     </row>
     <row r="71" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A71" s="54"/>
-      <c r="B71" s="48"/>
+      <c r="A71" s="83"/>
+      <c r="B71" s="80"/>
       <c r="C71" s="43" t="s">
         <v>76</v>
       </c>
@@ -2150,11 +2171,11 @@
       <c r="E71" s="23">
         <v>1</v>
       </c>
-      <c r="F71" s="65"/>
+      <c r="F71" s="51"/>
     </row>
     <row r="72" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A72" s="55"/>
-      <c r="B72" s="49"/>
+      <c r="A72" s="78"/>
+      <c r="B72" s="81"/>
       <c r="C72" s="17" t="s">
         <v>77</v>
       </c>
@@ -2164,7 +2185,7 @@
       <c r="E72" s="9">
         <v>1</v>
       </c>
-      <c r="F72" s="72"/>
+      <c r="F72" s="58"/>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73" s="14"/>
@@ -2172,13 +2193,13 @@
       <c r="C73" s="14"/>
       <c r="D73" s="36"/>
       <c r="E73" s="36"/>
-      <c r="F73" s="71"/>
+      <c r="F73" s="57"/>
     </row>
     <row r="74" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="53" t="s">
+      <c r="A74" s="76" t="s">
         <v>2</v>
       </c>
-      <c r="B74" s="47" t="s">
+      <c r="B74" s="79" t="s">
         <v>35</v>
       </c>
       <c r="C74" s="20" t="s">
@@ -2190,13 +2211,13 @@
       <c r="E74" s="21">
         <v>0</v>
       </c>
-      <c r="F74" s="64" t="s">
+      <c r="F74" s="50" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A75" s="60"/>
-      <c r="B75" s="48"/>
+      <c r="A75" s="77"/>
+      <c r="B75" s="80"/>
       <c r="C75" s="22" t="s">
         <v>79</v>
       </c>
@@ -2206,13 +2227,13 @@
       <c r="E75" s="23">
         <v>0</v>
       </c>
-      <c r="F75" s="65" t="s">
+      <c r="F75" s="51" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A76" s="60"/>
-      <c r="B76" s="48"/>
+      <c r="A76" s="77"/>
+      <c r="B76" s="80"/>
       <c r="C76" s="22" t="s">
         <v>80</v>
       </c>
@@ -2222,11 +2243,11 @@
       <c r="E76" s="23">
         <v>1</v>
       </c>
-      <c r="F76" s="65"/>
+      <c r="F76" s="51"/>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A77" s="60"/>
-      <c r="B77" s="48"/>
+      <c r="A77" s="77"/>
+      <c r="B77" s="80"/>
       <c r="C77" s="22" t="s">
         <v>81</v>
       </c>
@@ -2236,11 +2257,11 @@
       <c r="E77" s="23">
         <v>1</v>
       </c>
-      <c r="F77" s="65"/>
+      <c r="F77" s="51"/>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A78" s="60"/>
-      <c r="B78" s="48"/>
+      <c r="A78" s="77"/>
+      <c r="B78" s="80"/>
       <c r="C78" s="22" t="s">
         <v>83</v>
       </c>
@@ -2250,13 +2271,13 @@
       <c r="E78" s="23">
         <v>0</v>
       </c>
-      <c r="F78" s="65" t="s">
+      <c r="F78" s="51" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A79" s="60"/>
-      <c r="B79" s="48"/>
+      <c r="A79" s="77"/>
+      <c r="B79" s="80"/>
       <c r="C79" s="22" t="s">
         <v>84</v>
       </c>
@@ -2266,13 +2287,13 @@
       <c r="E79" s="23">
         <v>0</v>
       </c>
-      <c r="F79" s="65" t="s">
+      <c r="F79" s="51" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A80" s="60"/>
-      <c r="B80" s="48"/>
+      <c r="A80" s="77"/>
+      <c r="B80" s="80"/>
       <c r="C80" s="22" t="s">
         <v>85</v>
       </c>
@@ -2282,11 +2303,11 @@
       <c r="E80" s="23">
         <v>1</v>
       </c>
-      <c r="F80" s="65"/>
+      <c r="F80" s="51"/>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A81" s="60"/>
-      <c r="B81" s="49"/>
+      <c r="A81" s="77"/>
+      <c r="B81" s="81"/>
       <c r="C81" s="7" t="s">
         <v>82</v>
       </c>
@@ -2296,11 +2317,11 @@
       <c r="E81" s="9">
         <v>1</v>
       </c>
-      <c r="F81" s="72"/>
+      <c r="F81" s="58"/>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A82" s="60"/>
-      <c r="B82" s="50" t="s">
+      <c r="A82" s="77"/>
+      <c r="B82" s="73" t="s">
         <v>36</v>
       </c>
       <c r="C82" s="31" t="s">
@@ -2312,13 +2333,13 @@
       <c r="E82" s="32">
         <v>0</v>
       </c>
-      <c r="F82" s="67" t="s">
+      <c r="F82" s="53" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A83" s="60"/>
-      <c r="B83" s="51"/>
+      <c r="A83" s="77"/>
+      <c r="B83" s="84"/>
       <c r="C83" s="27" t="s">
         <v>87</v>
       </c>
@@ -2328,13 +2349,13 @@
       <c r="E83" s="28">
         <v>0</v>
       </c>
-      <c r="F83" s="73" t="s">
+      <c r="F83" s="59" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A84" s="60"/>
-      <c r="B84" s="51"/>
+      <c r="A84" s="77"/>
+      <c r="B84" s="84"/>
       <c r="C84" s="27" t="s">
         <v>88</v>
       </c>
@@ -2344,11 +2365,11 @@
       <c r="E84" s="28">
         <v>1</v>
       </c>
-      <c r="F84" s="73"/>
+      <c r="F84" s="59"/>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A85" s="60"/>
-      <c r="B85" s="51"/>
+      <c r="A85" s="77"/>
+      <c r="B85" s="84"/>
       <c r="C85" s="27" t="s">
         <v>89</v>
       </c>
@@ -2358,11 +2379,11 @@
       <c r="E85" s="28">
         <v>1</v>
       </c>
-      <c r="F85" s="73"/>
+      <c r="F85" s="59"/>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A86" s="60"/>
-      <c r="B86" s="51"/>
+      <c r="A86" s="77"/>
+      <c r="B86" s="84"/>
       <c r="C86" s="27" t="s">
         <v>90</v>
       </c>
@@ -2372,13 +2393,13 @@
       <c r="E86" s="28">
         <v>0</v>
       </c>
-      <c r="F86" s="73" t="s">
+      <c r="F86" s="59" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A87" s="60"/>
-      <c r="B87" s="51"/>
+      <c r="A87" s="77"/>
+      <c r="B87" s="84"/>
       <c r="C87" s="27" t="s">
         <v>91</v>
       </c>
@@ -2388,13 +2409,13 @@
       <c r="E87" s="28">
         <v>0</v>
       </c>
-      <c r="F87" s="73" t="s">
+      <c r="F87" s="59" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A88" s="60"/>
-      <c r="B88" s="51"/>
+      <c r="A88" s="77"/>
+      <c r="B88" s="84"/>
       <c r="C88" s="27" t="s">
         <v>92</v>
       </c>
@@ -2404,11 +2425,11 @@
       <c r="E88" s="28">
         <v>1</v>
       </c>
-      <c r="F88" s="73"/>
+      <c r="F88" s="59"/>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A89" s="60"/>
-      <c r="B89" s="52"/>
+      <c r="A89" s="77"/>
+      <c r="B89" s="75"/>
       <c r="C89" s="3" t="s">
         <v>93</v>
       </c>
@@ -2418,11 +2439,11 @@
       <c r="E89" s="11">
         <v>1</v>
       </c>
-      <c r="F89" s="68"/>
+      <c r="F89" s="54"/>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A90" s="60"/>
-      <c r="B90" s="47" t="s">
+      <c r="A90" s="77"/>
+      <c r="B90" s="79" t="s">
         <v>16</v>
       </c>
       <c r="C90" s="20" t="s">
@@ -2434,11 +2455,11 @@
       <c r="E90" s="21">
         <v>1</v>
       </c>
-      <c r="F90" s="64"/>
+      <c r="F90" s="50"/>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A91" s="60"/>
-      <c r="B91" s="49"/>
+      <c r="A91" s="77"/>
+      <c r="B91" s="81"/>
       <c r="C91" s="6" t="s">
         <v>95</v>
       </c>
@@ -2448,11 +2469,11 @@
       <c r="E91" s="12">
         <v>1</v>
       </c>
-      <c r="F91" s="74"/>
+      <c r="F91" s="60"/>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A92" s="60"/>
-      <c r="B92" s="50" t="s">
+      <c r="A92" s="77"/>
+      <c r="B92" s="73" t="s">
         <v>107</v>
       </c>
       <c r="C92" s="31" t="s">
@@ -2464,11 +2485,11 @@
       <c r="E92" s="32">
         <v>1</v>
       </c>
-      <c r="F92" s="67"/>
+      <c r="F92" s="53"/>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A93" s="60"/>
-      <c r="B93" s="56"/>
+      <c r="A93" s="77"/>
+      <c r="B93" s="74"/>
       <c r="C93" s="33" t="s">
         <v>113</v>
       </c>
@@ -2478,11 +2499,11 @@
       <c r="E93" s="34">
         <v>1</v>
       </c>
-      <c r="F93" s="62"/>
+      <c r="F93" s="48"/>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A94" s="60"/>
-      <c r="B94" s="56"/>
+      <c r="A94" s="77"/>
+      <c r="B94" s="74"/>
       <c r="C94" s="33" t="s">
         <v>109</v>
       </c>
@@ -2492,11 +2513,11 @@
       <c r="E94" s="34">
         <v>1</v>
       </c>
-      <c r="F94" s="62"/>
+      <c r="F94" s="48"/>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A95" s="55"/>
-      <c r="B95" s="52"/>
+      <c r="A95" s="78"/>
+      <c r="B95" s="75"/>
       <c r="C95" s="40" t="s">
         <v>114</v>
       </c>
@@ -2506,7 +2527,7 @@
       <c r="E95" s="18">
         <v>1</v>
       </c>
-      <c r="F95" s="75"/>
+      <c r="F95" s="61"/>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A96" s="14"/>
@@ -2514,20 +2535,27 @@
       <c r="C96" s="14"/>
       <c r="D96" s="36"/>
       <c r="E96" s="36"/>
-      <c r="F96" s="71"/>
+      <c r="F96" s="57"/>
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="B45:B48"/>
+    <mergeCell ref="A56:A72"/>
+    <mergeCell ref="B56:B59"/>
+    <mergeCell ref="B60:B63"/>
+    <mergeCell ref="B64:B66"/>
+    <mergeCell ref="B67:B69"/>
+    <mergeCell ref="B70:B72"/>
+    <mergeCell ref="B2:B8"/>
+    <mergeCell ref="B9:B17"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="A2:A23"/>
     <mergeCell ref="B92:B95"/>
     <mergeCell ref="A74:A95"/>
     <mergeCell ref="B25:B27"/>
     <mergeCell ref="B31:B33"/>
     <mergeCell ref="A25:A33"/>
-    <mergeCell ref="B2:B8"/>
-    <mergeCell ref="B9:B17"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="A2:A23"/>
     <mergeCell ref="B38:B39"/>
     <mergeCell ref="B35:B37"/>
     <mergeCell ref="B40:B42"/>
@@ -2539,13 +2567,6 @@
     <mergeCell ref="B49:B52"/>
     <mergeCell ref="B53:B54"/>
     <mergeCell ref="A45:A54"/>
-    <mergeCell ref="B45:B48"/>
-    <mergeCell ref="A56:A72"/>
-    <mergeCell ref="B56:B59"/>
-    <mergeCell ref="B60:B63"/>
-    <mergeCell ref="B64:B66"/>
-    <mergeCell ref="B67:B69"/>
-    <mergeCell ref="B70:B72"/>
   </mergeCells>
   <conditionalFormatting sqref="D97:E1048576 D56:E72 D1:E54 D74:E91">
     <cfRule type="iconSet" priority="12">
@@ -2620,7 +2641,7 @@
     <col min="2" max="2" width="22.77734375" customWidth="1"/>
     <col min="3" max="3" width="70.33203125" customWidth="1"/>
     <col min="4" max="5" width="7.77734375" style="19" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="32.33203125" style="78" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="32.33203125" style="64" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
@@ -2633,21 +2654,21 @@
       <c r="C1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="61" t="s">
+      <c r="D1" s="47" t="s">
         <v>97</v>
       </c>
-      <c r="E1" s="61" t="s">
+      <c r="E1" s="47" t="s">
         <v>98</v>
       </c>
-      <c r="F1" s="63" t="s">
+      <c r="F1" s="49" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="53" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="48" t="s">
+      <c r="A2" s="76" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="80" t="s">
         <v>14</v>
       </c>
       <c r="C2" s="20" t="s">
@@ -2659,11 +2680,11 @@
       <c r="E2" s="37">
         <v>0</v>
       </c>
-      <c r="F2" s="64"/>
+      <c r="F2" s="50"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="54"/>
-      <c r="B3" s="48"/>
+      <c r="A3" s="83"/>
+      <c r="B3" s="80"/>
       <c r="C3" s="22" t="s">
         <v>8</v>
       </c>
@@ -2673,7 +2694,7 @@
       <c r="E3" s="23">
         <v>0</v>
       </c>
-      <c r="F3" s="65"/>
+      <c r="F3" s="51"/>
       <c r="H3" s="8">
         <v>0</v>
       </c>
@@ -2682,8 +2703,8 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="54"/>
-      <c r="B4" s="48"/>
+      <c r="A4" s="83"/>
+      <c r="B4" s="80"/>
       <c r="C4" s="22" t="s">
         <v>9</v>
       </c>
@@ -2693,7 +2714,7 @@
       <c r="E4" s="23">
         <v>0</v>
       </c>
-      <c r="F4" s="65"/>
+      <c r="F4" s="51"/>
       <c r="H4" s="8">
         <v>1</v>
       </c>
@@ -2702,8 +2723,8 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="54"/>
-      <c r="B5" s="48"/>
+      <c r="A5" s="83"/>
+      <c r="B5" s="80"/>
       <c r="C5" s="22" t="s">
         <v>10</v>
       </c>
@@ -2713,11 +2734,11 @@
       <c r="E5" s="23">
         <v>0</v>
       </c>
-      <c r="F5" s="65"/>
+      <c r="F5" s="51"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="54"/>
-      <c r="B6" s="48"/>
+      <c r="A6" s="83"/>
+      <c r="B6" s="80"/>
       <c r="C6" s="24" t="s">
         <v>11</v>
       </c>
@@ -2727,11 +2748,11 @@
       <c r="E6" s="25">
         <v>0</v>
       </c>
-      <c r="F6" s="66"/>
+      <c r="F6" s="52"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="54"/>
-      <c r="B7" s="48"/>
+      <c r="A7" s="83"/>
+      <c r="B7" s="80"/>
       <c r="C7" s="24" t="s">
         <v>12</v>
       </c>
@@ -2741,11 +2762,11 @@
       <c r="E7" s="25">
         <v>1</v>
       </c>
-      <c r="F7" s="66"/>
+      <c r="F7" s="52"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="54"/>
-      <c r="B8" s="50" t="s">
+      <c r="A8" s="83"/>
+      <c r="B8" s="73" t="s">
         <v>15</v>
       </c>
       <c r="C8" s="31" t="s">
@@ -2757,11 +2778,11 @@
       <c r="E8" s="32">
         <v>0</v>
       </c>
-      <c r="F8" s="67"/>
+      <c r="F8" s="53"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="54"/>
-      <c r="B9" s="51"/>
+      <c r="A9" s="83"/>
+      <c r="B9" s="84"/>
       <c r="C9" s="33" t="s">
         <v>13</v>
       </c>
@@ -2771,11 +2792,11 @@
       <c r="E9" s="34">
         <v>0</v>
       </c>
-      <c r="F9" s="62"/>
+      <c r="F9" s="48"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="54"/>
-      <c r="B10" s="51"/>
+      <c r="A10" s="83"/>
+      <c r="B10" s="84"/>
       <c r="C10" s="33" t="s">
         <v>19</v>
       </c>
@@ -2785,13 +2806,13 @@
       <c r="E10" s="34">
         <v>0</v>
       </c>
-      <c r="F10" s="62" t="s">
+      <c r="F10" s="48" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="54"/>
-      <c r="B11" s="51"/>
+      <c r="A11" s="83"/>
+      <c r="B11" s="84"/>
       <c r="C11" s="33" t="s">
         <v>20</v>
       </c>
@@ -2801,11 +2822,11 @@
       <c r="E11" s="34">
         <v>0</v>
       </c>
-      <c r="F11" s="62"/>
+      <c r="F11" s="48"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="54"/>
-      <c r="B12" s="51"/>
+      <c r="A12" s="83"/>
+      <c r="B12" s="84"/>
       <c r="C12" s="33" t="s">
         <v>21</v>
       </c>
@@ -2815,11 +2836,11 @@
       <c r="E12" s="34">
         <v>0</v>
       </c>
-      <c r="F12" s="62"/>
+      <c r="F12" s="48"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="54"/>
-      <c r="B13" s="51"/>
+      <c r="A13" s="83"/>
+      <c r="B13" s="84"/>
       <c r="C13" s="33" t="s">
         <v>23</v>
       </c>
@@ -2829,11 +2850,11 @@
       <c r="E13" s="34">
         <v>1</v>
       </c>
-      <c r="F13" s="62"/>
+      <c r="F13" s="48"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="54"/>
-      <c r="B14" s="51"/>
+      <c r="A14" s="83"/>
+      <c r="B14" s="84"/>
       <c r="C14" s="33" t="s">
         <v>22</v>
       </c>
@@ -2843,11 +2864,11 @@
       <c r="E14" s="34">
         <v>1</v>
       </c>
-      <c r="F14" s="62"/>
+      <c r="F14" s="48"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="54"/>
-      <c r="B15" s="52"/>
+      <c r="A15" s="83"/>
+      <c r="B15" s="75"/>
       <c r="C15" s="3" t="s">
         <v>100</v>
       </c>
@@ -2857,10 +2878,10 @@
       <c r="E15" s="11">
         <v>1</v>
       </c>
-      <c r="F15" s="68"/>
+      <c r="F15" s="54"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="54"/>
+      <c r="A16" s="83"/>
       <c r="B16" s="41" t="s">
         <v>17</v>
       </c>
@@ -2873,11 +2894,11 @@
       <c r="E16" s="42">
         <v>1</v>
       </c>
-      <c r="F16" s="69"/>
+      <c r="F16" s="55"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="54"/>
-      <c r="B17" s="50" t="s">
+      <c r="A17" s="83"/>
+      <c r="B17" s="73" t="s">
         <v>16</v>
       </c>
       <c r="C17" s="31" t="s">
@@ -2889,11 +2910,11 @@
       <c r="E17" s="32">
         <v>1</v>
       </c>
-      <c r="F17" s="67"/>
+      <c r="F17" s="53"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="54"/>
-      <c r="B18" s="51"/>
+      <c r="A18" s="83"/>
+      <c r="B18" s="84"/>
       <c r="C18" s="40" t="s">
         <v>34</v>
       </c>
@@ -2903,7 +2924,7 @@
       <c r="E18" s="10">
         <v>0</v>
       </c>
-      <c r="F18" s="70" t="s">
+      <c r="F18" s="56" t="s">
         <v>111</v>
       </c>
     </row>
@@ -2913,13 +2934,13 @@
       <c r="C19" s="14"/>
       <c r="D19" s="36"/>
       <c r="E19" s="36"/>
-      <c r="F19" s="71"/>
+      <c r="F19" s="57"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="53" t="s">
-        <v>1</v>
-      </c>
-      <c r="B20" s="47" t="s">
+      <c r="A20" s="76" t="s">
+        <v>1</v>
+      </c>
+      <c r="B20" s="79" t="s">
         <v>35</v>
       </c>
       <c r="C20" s="20" t="s">
@@ -2931,11 +2952,11 @@
       <c r="E20" s="21">
         <v>1</v>
       </c>
-      <c r="F20" s="64"/>
+      <c r="F20" s="50"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" s="60"/>
-      <c r="B21" s="48"/>
+      <c r="A21" s="77"/>
+      <c r="B21" s="80"/>
       <c r="C21" s="22" t="s">
         <v>50</v>
       </c>
@@ -2945,13 +2966,13 @@
       <c r="E21" s="23">
         <v>1</v>
       </c>
-      <c r="F21" s="65" t="s">
+      <c r="F21" s="51" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" s="54"/>
-      <c r="B22" s="49"/>
+      <c r="A22" s="83"/>
+      <c r="B22" s="81"/>
       <c r="C22" s="7" t="s">
         <v>37</v>
       </c>
@@ -2961,11 +2982,11 @@
       <c r="E22" s="9">
         <v>1</v>
       </c>
-      <c r="F22" s="72"/>
+      <c r="F22" s="58"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23" s="54"/>
-      <c r="B23" s="50" t="s">
+      <c r="A23" s="83"/>
+      <c r="B23" s="73" t="s">
         <v>36</v>
       </c>
       <c r="C23" s="31" t="s">
@@ -2977,13 +2998,13 @@
       <c r="E23" s="32">
         <v>1</v>
       </c>
-      <c r="F23" s="67" t="s">
+      <c r="F23" s="53" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24" s="54"/>
-      <c r="B24" s="56"/>
+      <c r="A24" s="83"/>
+      <c r="B24" s="74"/>
       <c r="C24" s="27" t="s">
         <v>102</v>
       </c>
@@ -2993,11 +3014,11 @@
       <c r="E24" s="28">
         <v>1</v>
       </c>
-      <c r="F24" s="73"/>
+      <c r="F24" s="59"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25" s="54"/>
-      <c r="B25" s="52"/>
+      <c r="A25" s="83"/>
+      <c r="B25" s="75"/>
       <c r="C25" s="3" t="s">
         <v>103</v>
       </c>
@@ -3007,11 +3028,11 @@
       <c r="E25" s="11">
         <v>1</v>
       </c>
-      <c r="F25" s="68"/>
+      <c r="F25" s="54"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26" s="54"/>
-      <c r="B26" s="57" t="s">
+      <c r="A26" s="83"/>
+      <c r="B26" s="82" t="s">
         <v>16</v>
       </c>
       <c r="C26" s="20" t="s">
@@ -3023,11 +3044,11 @@
       <c r="E26" s="21">
         <v>1</v>
       </c>
-      <c r="F26" s="64"/>
+      <c r="F26" s="50"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A27" s="54"/>
-      <c r="B27" s="57"/>
+      <c r="A27" s="83"/>
+      <c r="B27" s="82"/>
       <c r="C27" s="22" t="s">
         <v>112</v>
       </c>
@@ -3037,11 +3058,11 @@
       <c r="E27" s="23">
         <v>0</v>
       </c>
-      <c r="F27" s="65"/>
+      <c r="F27" s="51"/>
     </row>
     <row r="28" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A28" s="55"/>
-      <c r="B28" s="57"/>
+      <c r="A28" s="78"/>
+      <c r="B28" s="82"/>
       <c r="C28" s="15" t="s">
         <v>42</v>
       </c>
@@ -3051,7 +3072,7 @@
       <c r="E28" s="12">
         <v>1</v>
       </c>
-      <c r="F28" s="74"/>
+      <c r="F28" s="60"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="14"/>
@@ -3059,13 +3080,13 @@
       <c r="C29" s="14"/>
       <c r="D29" s="36"/>
       <c r="E29" s="36"/>
-      <c r="F29" s="71"/>
+      <c r="F29" s="57"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A30" s="58" t="s">
+      <c r="A30" s="85" t="s">
         <v>49</v>
       </c>
-      <c r="B30" s="47" t="s">
+      <c r="B30" s="79" t="s">
         <v>35</v>
       </c>
       <c r="C30" s="20" t="s">
@@ -3077,11 +3098,11 @@
       <c r="E30" s="21">
         <v>0</v>
       </c>
-      <c r="F30" s="64"/>
+      <c r="F30" s="50"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A31" s="59"/>
-      <c r="B31" s="48"/>
+      <c r="A31" s="86"/>
+      <c r="B31" s="80"/>
       <c r="C31" s="22" t="s">
         <v>43</v>
       </c>
@@ -3091,11 +3112,11 @@
       <c r="E31" s="23">
         <v>1</v>
       </c>
-      <c r="F31" s="65"/>
+      <c r="F31" s="51"/>
     </row>
     <row r="32" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A32" s="54"/>
-      <c r="B32" s="49"/>
+      <c r="A32" s="83"/>
+      <c r="B32" s="81"/>
       <c r="C32" s="17" t="s">
         <v>44</v>
       </c>
@@ -3105,11 +3126,11 @@
       <c r="E32" s="9">
         <v>1</v>
       </c>
-      <c r="F32" s="72"/>
+      <c r="F32" s="58"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A33" s="54"/>
-      <c r="B33" s="50" t="s">
+      <c r="A33" s="83"/>
+      <c r="B33" s="73" t="s">
         <v>48</v>
       </c>
       <c r="C33" s="38" t="s">
@@ -3121,11 +3142,11 @@
       <c r="E33" s="18">
         <v>1</v>
       </c>
-      <c r="F33" s="75"/>
+      <c r="F33" s="61"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A34" s="54"/>
-      <c r="B34" s="52"/>
+      <c r="A34" s="83"/>
+      <c r="B34" s="75"/>
       <c r="C34" s="2" t="s">
         <v>61</v>
       </c>
@@ -3135,11 +3156,11 @@
       <c r="E34" s="18">
         <v>1</v>
       </c>
-      <c r="F34" s="75"/>
+      <c r="F34" s="61"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A35" s="54"/>
-      <c r="B35" s="47" t="s">
+      <c r="A35" s="83"/>
+      <c r="B35" s="79" t="s">
         <v>36</v>
       </c>
       <c r="C35" s="20" t="s">
@@ -3151,11 +3172,11 @@
       <c r="E35" s="21">
         <v>0</v>
       </c>
-      <c r="F35" s="64"/>
+      <c r="F35" s="50"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A36" s="54"/>
-      <c r="B36" s="48"/>
+      <c r="A36" s="83"/>
+      <c r="B36" s="80"/>
       <c r="C36" s="22" t="s">
         <v>45</v>
       </c>
@@ -3165,11 +3186,11 @@
       <c r="E36" s="23">
         <v>1</v>
       </c>
-      <c r="F36" s="65"/>
+      <c r="F36" s="51"/>
     </row>
     <row r="37" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A37" s="54"/>
-      <c r="B37" s="49"/>
+      <c r="A37" s="83"/>
+      <c r="B37" s="81"/>
       <c r="C37" s="17" t="s">
         <v>46</v>
       </c>
@@ -3179,10 +3200,10 @@
       <c r="E37" s="9">
         <v>1</v>
       </c>
-      <c r="F37" s="72"/>
+      <c r="F37" s="58"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A38" s="55"/>
+      <c r="A38" s="78"/>
       <c r="B38" s="39" t="s">
         <v>16</v>
       </c>
@@ -3195,7 +3216,7 @@
       <c r="E38" s="10">
         <v>1</v>
       </c>
-      <c r="F38" s="70"/>
+      <c r="F38" s="56"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="14"/>
@@ -3203,13 +3224,13 @@
       <c r="C39" s="14"/>
       <c r="D39" s="36"/>
       <c r="E39" s="36"/>
-      <c r="F39" s="71"/>
+      <c r="F39" s="57"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A40" s="53" t="s">
+      <c r="A40" s="76" t="s">
         <v>4</v>
       </c>
-      <c r="B40" s="47" t="s">
+      <c r="B40" s="79" t="s">
         <v>35</v>
       </c>
       <c r="C40" s="20" t="s">
@@ -3221,11 +3242,11 @@
       <c r="E40" s="21">
         <v>0</v>
       </c>
-      <c r="F40" s="64"/>
+      <c r="F40" s="50"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A41" s="54"/>
-      <c r="B41" s="48"/>
+      <c r="A41" s="83"/>
+      <c r="B41" s="80"/>
       <c r="C41" s="22" t="s">
         <v>52</v>
       </c>
@@ -3235,11 +3256,11 @@
       <c r="E41" s="23">
         <v>1</v>
       </c>
-      <c r="F41" s="65"/>
+      <c r="F41" s="51"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A42" s="54"/>
-      <c r="B42" s="48"/>
+      <c r="A42" s="83"/>
+      <c r="B42" s="80"/>
       <c r="C42" s="22" t="s">
         <v>53</v>
       </c>
@@ -3249,11 +3270,11 @@
       <c r="E42" s="23">
         <v>1</v>
       </c>
-      <c r="F42" s="65"/>
+      <c r="F42" s="51"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A43" s="54"/>
-      <c r="B43" s="49"/>
+      <c r="A43" s="83"/>
+      <c r="B43" s="81"/>
       <c r="C43" s="7" t="s">
         <v>54</v>
       </c>
@@ -3263,11 +3284,11 @@
       <c r="E43" s="9">
         <v>1</v>
       </c>
-      <c r="F43" s="72"/>
+      <c r="F43" s="58"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A44" s="54"/>
-      <c r="B44" s="56" t="s">
+      <c r="A44" s="83"/>
+      <c r="B44" s="74" t="s">
         <v>36</v>
       </c>
       <c r="C44" s="27" t="s">
@@ -3279,11 +3300,11 @@
       <c r="E44" s="28">
         <v>0</v>
       </c>
-      <c r="F44" s="73"/>
+      <c r="F44" s="59"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A45" s="54"/>
-      <c r="B45" s="56"/>
+      <c r="A45" s="83"/>
+      <c r="B45" s="74"/>
       <c r="C45" s="33" t="s">
         <v>55</v>
       </c>
@@ -3293,11 +3314,11 @@
       <c r="E45" s="34">
         <v>1</v>
       </c>
-      <c r="F45" s="62"/>
+      <c r="F45" s="48"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A46" s="54"/>
-      <c r="B46" s="56"/>
+      <c r="A46" s="83"/>
+      <c r="B46" s="74"/>
       <c r="C46" s="33" t="s">
         <v>56</v>
       </c>
@@ -3307,11 +3328,11 @@
       <c r="E46" s="34">
         <v>1</v>
       </c>
-      <c r="F46" s="62"/>
+      <c r="F46" s="48"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A47" s="54"/>
-      <c r="B47" s="52"/>
+      <c r="A47" s="83"/>
+      <c r="B47" s="75"/>
       <c r="C47" s="3" t="s">
         <v>57</v>
       </c>
@@ -3321,11 +3342,11 @@
       <c r="E47" s="11">
         <v>1</v>
       </c>
-      <c r="F47" s="68"/>
+      <c r="F47" s="54"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A48" s="54"/>
-      <c r="B48" s="57" t="s">
+      <c r="A48" s="83"/>
+      <c r="B48" s="82" t="s">
         <v>16</v>
       </c>
       <c r="C48" s="24" t="s">
@@ -3337,11 +3358,11 @@
       <c r="E48" s="25">
         <v>1</v>
       </c>
-      <c r="F48" s="66"/>
+      <c r="F48" s="52"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A49" s="55"/>
-      <c r="B49" s="57"/>
+      <c r="A49" s="78"/>
+      <c r="B49" s="82"/>
       <c r="C49" s="16" t="s">
         <v>59</v>
       </c>
@@ -3351,7 +3372,7 @@
       <c r="E49" s="12">
         <v>1</v>
       </c>
-      <c r="F49" s="74"/>
+      <c r="F49" s="60"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" s="14"/>
@@ -3359,13 +3380,13 @@
       <c r="C50" s="14"/>
       <c r="D50" s="36"/>
       <c r="E50" s="36"/>
-      <c r="F50" s="71"/>
+      <c r="F50" s="57"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A51" s="53" t="s">
+      <c r="A51" s="76" t="s">
         <v>3</v>
       </c>
-      <c r="B51" s="47" t="s">
+      <c r="B51" s="79" t="s">
         <v>35</v>
       </c>
       <c r="C51" s="20" t="s">
@@ -3377,11 +3398,11 @@
       <c r="E51" s="21">
         <v>0</v>
       </c>
-      <c r="F51" s="64"/>
+      <c r="F51" s="50"/>
     </row>
     <row r="52" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A52" s="54"/>
-      <c r="B52" s="48"/>
+      <c r="A52" s="83"/>
+      <c r="B52" s="80"/>
       <c r="C52" s="43" t="s">
         <v>62</v>
       </c>
@@ -3391,13 +3412,13 @@
       <c r="E52" s="23">
         <v>0</v>
       </c>
-      <c r="F52" s="65" t="s">
+      <c r="F52" s="51" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A53" s="54"/>
-      <c r="B53" s="48"/>
+      <c r="A53" s="83"/>
+      <c r="B53" s="80"/>
       <c r="C53" s="22" t="s">
         <v>63</v>
       </c>
@@ -3407,11 +3428,11 @@
       <c r="E53" s="23">
         <v>0</v>
       </c>
-      <c r="F53" s="65"/>
+      <c r="F53" s="51"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A54" s="54"/>
-      <c r="B54" s="49"/>
+      <c r="A54" s="83"/>
+      <c r="B54" s="81"/>
       <c r="C54" s="7" t="s">
         <v>64</v>
       </c>
@@ -3421,11 +3442,11 @@
       <c r="E54" s="9">
         <v>1</v>
       </c>
-      <c r="F54" s="72"/>
+      <c r="F54" s="58"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A55" s="54"/>
-      <c r="B55" s="50" t="s">
+      <c r="A55" s="83"/>
+      <c r="B55" s="73" t="s">
         <v>36</v>
       </c>
       <c r="C55" s="31" t="s">
@@ -3437,11 +3458,11 @@
       <c r="E55" s="32">
         <v>0</v>
       </c>
-      <c r="F55" s="67"/>
+      <c r="F55" s="53"/>
     </row>
     <row r="56" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A56" s="54"/>
-      <c r="B56" s="56"/>
+      <c r="A56" s="83"/>
+      <c r="B56" s="74"/>
       <c r="C56" s="44" t="s">
         <v>65</v>
       </c>
@@ -3451,13 +3472,13 @@
       <c r="E56" s="34">
         <v>0</v>
       </c>
-      <c r="F56" s="62" t="s">
+      <c r="F56" s="48" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A57" s="54"/>
-      <c r="B57" s="56"/>
+      <c r="A57" s="83"/>
+      <c r="B57" s="74"/>
       <c r="C57" s="33" t="s">
         <v>66</v>
       </c>
@@ -3467,11 +3488,11 @@
       <c r="E57" s="34">
         <v>0</v>
       </c>
-      <c r="F57" s="62"/>
+      <c r="F57" s="48"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A58" s="54"/>
-      <c r="B58" s="52"/>
+      <c r="A58" s="83"/>
+      <c r="B58" s="75"/>
       <c r="C58" s="3" t="s">
         <v>67</v>
       </c>
@@ -3481,11 +3502,11 @@
       <c r="E58" s="11">
         <v>1</v>
       </c>
-      <c r="F58" s="68"/>
+      <c r="F58" s="54"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A59" s="54"/>
-      <c r="B59" s="47" t="s">
+      <c r="A59" s="83"/>
+      <c r="B59" s="79" t="s">
         <v>74</v>
       </c>
       <c r="C59" s="20" t="s">
@@ -3497,11 +3518,11 @@
       <c r="E59" s="21">
         <v>1</v>
       </c>
-      <c r="F59" s="64"/>
+      <c r="F59" s="50"/>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A60" s="54"/>
-      <c r="B60" s="48"/>
+      <c r="A60" s="83"/>
+      <c r="B60" s="80"/>
       <c r="C60" s="22" t="s">
         <v>69</v>
       </c>
@@ -3511,11 +3532,11 @@
       <c r="E60" s="23">
         <v>1</v>
       </c>
-      <c r="F60" s="65"/>
+      <c r="F60" s="51"/>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A61" s="54"/>
-      <c r="B61" s="49"/>
+      <c r="A61" s="83"/>
+      <c r="B61" s="81"/>
       <c r="C61" s="7" t="s">
         <v>70</v>
       </c>
@@ -3525,10 +3546,10 @@
       <c r="E61" s="9">
         <v>1</v>
       </c>
-      <c r="F61" s="72"/>
+      <c r="F61" s="58"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A62" s="54"/>
+      <c r="A62" s="83"/>
       <c r="B62" s="45" t="s">
         <v>16</v>
       </c>
@@ -3541,7 +3562,7 @@
       <c r="E62" s="32">
         <v>1</v>
       </c>
-      <c r="F62" s="67" t="s">
+      <c r="F62" s="53" t="s">
         <v>106</v>
       </c>
     </row>
@@ -3551,13 +3572,13 @@
       <c r="C63" s="14"/>
       <c r="D63" s="36"/>
       <c r="E63" s="36"/>
-      <c r="F63" s="71"/>
+      <c r="F63" s="57"/>
     </row>
     <row r="64" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="53" t="s">
+      <c r="A64" s="76" t="s">
         <v>2</v>
       </c>
-      <c r="B64" s="47" t="s">
+      <c r="B64" s="79" t="s">
         <v>35</v>
       </c>
       <c r="C64" s="20" t="s">
@@ -3569,13 +3590,13 @@
       <c r="E64" s="21">
         <v>0</v>
       </c>
-      <c r="F64" s="64" t="s">
+      <c r="F64" s="50" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A65" s="60"/>
-      <c r="B65" s="48"/>
+      <c r="A65" s="77"/>
+      <c r="B65" s="80"/>
       <c r="C65" s="22" t="s">
         <v>79</v>
       </c>
@@ -3585,13 +3606,13 @@
       <c r="E65" s="23">
         <v>0</v>
       </c>
-      <c r="F65" s="65" t="s">
+      <c r="F65" s="51" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A66" s="60"/>
-      <c r="B66" s="48"/>
+      <c r="A66" s="77"/>
+      <c r="B66" s="80"/>
       <c r="C66" s="24" t="s">
         <v>80</v>
       </c>
@@ -3601,11 +3622,11 @@
       <c r="E66" s="25">
         <v>1</v>
       </c>
-      <c r="F66" s="66"/>
+      <c r="F66" s="52"/>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A67" s="60"/>
-      <c r="B67" s="48"/>
+      <c r="A67" s="77"/>
+      <c r="B67" s="80"/>
       <c r="C67" s="24" t="s">
         <v>81</v>
       </c>
@@ -3615,11 +3636,11 @@
       <c r="E67" s="25">
         <v>1</v>
       </c>
-      <c r="F67" s="66"/>
+      <c r="F67" s="52"/>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A68" s="60"/>
-      <c r="B68" s="48"/>
+      <c r="A68" s="77"/>
+      <c r="B68" s="80"/>
       <c r="C68" s="24" t="s">
         <v>83</v>
       </c>
@@ -3629,13 +3650,13 @@
       <c r="E68" s="25">
         <v>0</v>
       </c>
-      <c r="F68" s="66" t="s">
+      <c r="F68" s="52" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A69" s="60"/>
-      <c r="B69" s="48"/>
+      <c r="A69" s="77"/>
+      <c r="B69" s="80"/>
       <c r="C69" s="24" t="s">
         <v>84</v>
       </c>
@@ -3645,13 +3666,13 @@
       <c r="E69" s="25">
         <v>0</v>
       </c>
-      <c r="F69" s="66" t="s">
+      <c r="F69" s="52" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A70" s="60"/>
-      <c r="B70" s="48"/>
+      <c r="A70" s="77"/>
+      <c r="B70" s="80"/>
       <c r="C70" s="24" t="s">
         <v>85</v>
       </c>
@@ -3661,11 +3682,11 @@
       <c r="E70" s="25">
         <v>1</v>
       </c>
-      <c r="F70" s="66"/>
+      <c r="F70" s="52"/>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A71" s="60"/>
-      <c r="B71" s="49"/>
+      <c r="A71" s="77"/>
+      <c r="B71" s="81"/>
       <c r="C71" s="7" t="s">
         <v>82</v>
       </c>
@@ -3675,11 +3696,11 @@
       <c r="E71" s="9">
         <v>1</v>
       </c>
-      <c r="F71" s="72"/>
+      <c r="F71" s="58"/>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A72" s="60"/>
-      <c r="B72" s="50" t="s">
+      <c r="A72" s="77"/>
+      <c r="B72" s="73" t="s">
         <v>36</v>
       </c>
       <c r="C72" s="31" t="s">
@@ -3691,13 +3712,13 @@
       <c r="E72" s="32">
         <v>0</v>
       </c>
-      <c r="F72" s="67" t="s">
+      <c r="F72" s="53" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A73" s="60"/>
-      <c r="B73" s="51"/>
+      <c r="A73" s="77"/>
+      <c r="B73" s="84"/>
       <c r="C73" s="33" t="s">
         <v>87</v>
       </c>
@@ -3707,13 +3728,13 @@
       <c r="E73" s="34">
         <v>0</v>
       </c>
-      <c r="F73" s="62" t="s">
+      <c r="F73" s="48" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A74" s="60"/>
-      <c r="B74" s="51"/>
+      <c r="A74" s="77"/>
+      <c r="B74" s="84"/>
       <c r="C74" s="27" t="s">
         <v>88</v>
       </c>
@@ -3723,11 +3744,11 @@
       <c r="E74" s="28">
         <v>1</v>
       </c>
-      <c r="F74" s="73"/>
+      <c r="F74" s="59"/>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A75" s="60"/>
-      <c r="B75" s="51"/>
+      <c r="A75" s="77"/>
+      <c r="B75" s="84"/>
       <c r="C75" s="33" t="s">
         <v>89</v>
       </c>
@@ -3737,11 +3758,11 @@
       <c r="E75" s="34">
         <v>1</v>
       </c>
-      <c r="F75" s="62"/>
+      <c r="F75" s="48"/>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A76" s="60"/>
-      <c r="B76" s="51"/>
+      <c r="A76" s="77"/>
+      <c r="B76" s="84"/>
       <c r="C76" s="33" t="s">
         <v>90</v>
       </c>
@@ -3751,13 +3772,13 @@
       <c r="E76" s="34">
         <v>0</v>
       </c>
-      <c r="F76" s="62" t="s">
+      <c r="F76" s="48" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A77" s="60"/>
-      <c r="B77" s="51"/>
+      <c r="A77" s="77"/>
+      <c r="B77" s="84"/>
       <c r="C77" s="33" t="s">
         <v>91</v>
       </c>
@@ -3767,13 +3788,13 @@
       <c r="E77" s="34">
         <v>0</v>
       </c>
-      <c r="F77" s="62" t="s">
+      <c r="F77" s="48" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A78" s="60"/>
-      <c r="B78" s="51"/>
+      <c r="A78" s="77"/>
+      <c r="B78" s="84"/>
       <c r="C78" s="33" t="s">
         <v>92</v>
       </c>
@@ -3783,11 +3804,11 @@
       <c r="E78" s="34">
         <v>1</v>
       </c>
-      <c r="F78" s="62"/>
+      <c r="F78" s="48"/>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A79" s="60"/>
-      <c r="B79" s="52"/>
+      <c r="A79" s="77"/>
+      <c r="B79" s="75"/>
       <c r="C79" s="3" t="s">
         <v>93</v>
       </c>
@@ -3797,11 +3818,11 @@
       <c r="E79" s="11">
         <v>1</v>
       </c>
-      <c r="F79" s="68"/>
+      <c r="F79" s="54"/>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A80" s="60"/>
-      <c r="B80" s="47" t="s">
+      <c r="A80" s="77"/>
+      <c r="B80" s="79" t="s">
         <v>16</v>
       </c>
       <c r="C80" s="20" t="s">
@@ -3813,11 +3834,11 @@
       <c r="E80" s="21">
         <v>1</v>
       </c>
-      <c r="F80" s="64"/>
+      <c r="F80" s="50"/>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A81" s="60"/>
-      <c r="B81" s="49"/>
+      <c r="A81" s="77"/>
+      <c r="B81" s="81"/>
       <c r="C81" s="6" t="s">
         <v>95</v>
       </c>
@@ -3827,11 +3848,11 @@
       <c r="E81" s="12">
         <v>1</v>
       </c>
-      <c r="F81" s="74"/>
+      <c r="F81" s="60"/>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A82" s="60"/>
-      <c r="B82" s="50" t="s">
+      <c r="A82" s="77"/>
+      <c r="B82" s="73" t="s">
         <v>107</v>
       </c>
       <c r="C82" s="31" t="s">
@@ -3843,11 +3864,11 @@
       <c r="E82" s="32">
         <v>1</v>
       </c>
-      <c r="F82" s="67"/>
+      <c r="F82" s="53"/>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A83" s="55"/>
-      <c r="B83" s="52"/>
+      <c r="A83" s="78"/>
+      <c r="B83" s="75"/>
       <c r="C83" s="40" t="s">
         <v>109</v>
       </c>
@@ -3857,23 +3878,26 @@
       <c r="E83" s="18">
         <v>1</v>
       </c>
-      <c r="F83" s="75"/>
+      <c r="F83" s="61"/>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A84" s="79"/>
+      <c r="A84" s="65"/>
       <c r="B84" s="14"/>
       <c r="C84" s="14"/>
       <c r="D84" s="36"/>
       <c r="E84" s="36"/>
-      <c r="F84" s="71"/>
+      <c r="F84" s="57"/>
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="B64:B71"/>
-    <mergeCell ref="B72:B79"/>
-    <mergeCell ref="B80:B81"/>
-    <mergeCell ref="A64:A83"/>
-    <mergeCell ref="B82:B83"/>
+    <mergeCell ref="A2:A18"/>
+    <mergeCell ref="B2:B7"/>
+    <mergeCell ref="B8:B15"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="A20:A28"/>
+    <mergeCell ref="B20:B22"/>
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="B26:B28"/>
     <mergeCell ref="A51:A62"/>
     <mergeCell ref="B51:B54"/>
     <mergeCell ref="B55:B58"/>
@@ -3886,14 +3910,11 @@
     <mergeCell ref="B40:B43"/>
     <mergeCell ref="B44:B47"/>
     <mergeCell ref="B48:B49"/>
-    <mergeCell ref="A2:A18"/>
-    <mergeCell ref="B2:B7"/>
-    <mergeCell ref="B8:B15"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="A20:A28"/>
-    <mergeCell ref="B20:B22"/>
-    <mergeCell ref="B23:B25"/>
-    <mergeCell ref="B26:B28"/>
+    <mergeCell ref="B64:B71"/>
+    <mergeCell ref="B72:B79"/>
+    <mergeCell ref="B80:B81"/>
+    <mergeCell ref="A64:A83"/>
+    <mergeCell ref="B82:B83"/>
   </mergeCells>
   <conditionalFormatting sqref="D85:E1048576 D64:E81 D51:E62 D1:E49">
     <cfRule type="iconSet" priority="7">
@@ -3958,8 +3979,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E11F7609-0A7A-46D7-A44A-76050598E181}">
   <dimension ref="A1:J98"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3969,12 +3990,12 @@
     <col min="3" max="3" width="65.77734375" customWidth="1"/>
     <col min="4" max="4" width="8.5546875" style="19" customWidth="1"/>
     <col min="5" max="6" width="9" style="19" customWidth="1"/>
-    <col min="7" max="7" width="60.77734375" style="78" customWidth="1"/>
+    <col min="7" max="7" width="31.5546875" style="64" customWidth="1"/>
     <col min="9" max="9" width="9.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" s="82"/>
+      <c r="A1" s="6"/>
       <c r="B1" s="8">
         <v>0</v>
       </c>
@@ -3984,10 +4005,10 @@
       <c r="D1" s="8"/>
       <c r="E1" s="8"/>
       <c r="F1" s="8"/>
-      <c r="G1" s="77"/>
+      <c r="G1" s="63"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="81"/>
+      <c r="A2" s="7"/>
       <c r="B2" s="9">
         <v>1</v>
       </c>
@@ -3997,13 +4018,13 @@
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
       <c r="F2" s="9"/>
-      <c r="G2" s="72"/>
-      <c r="H2" s="83"/>
-      <c r="I2" s="83"/>
+      <c r="G2" s="58"/>
+      <c r="H2" s="68"/>
+      <c r="I2" s="68"/>
     </row>
     <row r="3" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="61" t="s">
-        <v>124</v>
+      <c r="A3" s="47" t="s">
+        <v>123</v>
       </c>
       <c r="B3" s="35" t="s">
         <v>6</v>
@@ -4011,27 +4032,27 @@
       <c r="C3" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="61" t="s">
+      <c r="D3" s="47" t="s">
         <v>97</v>
       </c>
-      <c r="E3" s="61" t="s">
+      <c r="E3" s="47" t="s">
         <v>117</v>
       </c>
-      <c r="F3" s="61" t="s">
+      <c r="F3" s="47" t="s">
         <v>118</v>
       </c>
       <c r="G3" s="35" t="s">
         <v>104</v>
       </c>
-      <c r="H3" s="82"/>
-      <c r="I3" s="82"/>
-      <c r="J3" s="82"/>
+      <c r="H3" s="67"/>
+      <c r="I3" s="67"/>
+      <c r="J3" s="67"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="53" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="48" t="s">
+      <c r="A4" s="76" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="80" t="s">
         <v>14</v>
       </c>
       <c r="C4" s="20" t="s">
@@ -4046,14 +4067,14 @@
       <c r="F4" s="37">
         <v>0</v>
       </c>
-      <c r="G4" s="64"/>
-      <c r="H4" s="82"/>
-      <c r="I4" s="89"/>
-      <c r="J4" s="82"/>
+      <c r="G4" s="50"/>
+      <c r="H4" s="67"/>
+      <c r="I4" s="72"/>
+      <c r="J4" s="67"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="54"/>
-      <c r="B5" s="48"/>
+      <c r="A5" s="83"/>
+      <c r="B5" s="80"/>
       <c r="C5" s="22" t="s">
         <v>8</v>
       </c>
@@ -4066,14 +4087,14 @@
       <c r="F5" s="23">
         <v>0</v>
       </c>
-      <c r="G5" s="65"/>
-      <c r="H5" s="82"/>
-      <c r="I5" s="88"/>
-      <c r="J5" s="82"/>
+      <c r="G5" s="51"/>
+      <c r="H5" s="67"/>
+      <c r="I5" s="71"/>
+      <c r="J5" s="67"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" s="54"/>
-      <c r="B6" s="48"/>
+      <c r="A6" s="83"/>
+      <c r="B6" s="80"/>
       <c r="C6" s="22" t="s">
         <v>9</v>
       </c>
@@ -4086,14 +4107,14 @@
       <c r="F6" s="23">
         <v>0</v>
       </c>
-      <c r="G6" s="65"/>
-      <c r="H6" s="82"/>
-      <c r="I6" s="88"/>
-      <c r="J6" s="82"/>
+      <c r="G6" s="51"/>
+      <c r="H6" s="67"/>
+      <c r="I6" s="71"/>
+      <c r="J6" s="67"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" s="54"/>
-      <c r="B7" s="48"/>
+      <c r="A7" s="83"/>
+      <c r="B7" s="80"/>
       <c r="C7" s="22" t="s">
         <v>10</v>
       </c>
@@ -4106,14 +4127,14 @@
       <c r="F7" s="23">
         <v>0</v>
       </c>
-      <c r="G7" s="65"/>
-      <c r="H7" s="82"/>
-      <c r="I7" s="88"/>
-      <c r="J7" s="82"/>
+      <c r="G7" s="51"/>
+      <c r="H7" s="67"/>
+      <c r="I7" s="71"/>
+      <c r="J7" s="67"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" s="54"/>
-      <c r="B8" s="48"/>
+      <c r="A8" s="83"/>
+      <c r="B8" s="80"/>
       <c r="C8" s="24" t="s">
         <v>11</v>
       </c>
@@ -4126,14 +4147,14 @@
       <c r="F8" s="25">
         <v>0</v>
       </c>
-      <c r="G8" s="66"/>
-      <c r="H8" s="82"/>
-      <c r="I8" s="85"/>
-      <c r="J8" s="82"/>
+      <c r="G8" s="52"/>
+      <c r="H8" s="67"/>
+      <c r="I8" s="70"/>
+      <c r="J8" s="67"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" s="54"/>
-      <c r="B9" s="48"/>
+      <c r="A9" s="83"/>
+      <c r="B9" s="80"/>
       <c r="C9" s="24" t="s">
         <v>12</v>
       </c>
@@ -4146,13 +4167,13 @@
       <c r="F9" s="25">
         <v>1</v>
       </c>
-      <c r="G9" s="66"/>
-      <c r="H9" s="83"/>
-      <c r="I9" s="84"/>
+      <c r="G9" s="52"/>
+      <c r="H9" s="68"/>
+      <c r="I9" s="69"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" s="54"/>
-      <c r="B10" s="49"/>
+      <c r="A10" s="83"/>
+      <c r="B10" s="81"/>
       <c r="C10" s="29" t="s">
         <v>24</v>
       </c>
@@ -4165,13 +4186,13 @@
       <c r="F10" s="30" t="s">
         <v>119</v>
       </c>
-      <c r="G10" s="80"/>
-      <c r="H10" s="83"/>
-      <c r="I10" s="84"/>
+      <c r="G10" s="66"/>
+      <c r="H10" s="68"/>
+      <c r="I10" s="69"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" s="54"/>
-      <c r="B11" s="50" t="s">
+      <c r="A11" s="83"/>
+      <c r="B11" s="73" t="s">
         <v>15</v>
       </c>
       <c r="C11" s="31" t="s">
@@ -4186,14 +4207,14 @@
       <c r="F11" s="32">
         <v>0</v>
       </c>
-      <c r="G11" s="67"/>
-      <c r="H11" s="83"/>
-      <c r="I11" s="84"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A12" s="54"/>
-      <c r="B12" s="51"/>
-      <c r="C12" s="33" t="s">
+      <c r="G11" s="53"/>
+      <c r="H11" s="68"/>
+      <c r="I11" s="69"/>
+    </row>
+    <row r="12" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="83"/>
+      <c r="B12" s="84"/>
+      <c r="C12" s="90" t="s">
         <v>13</v>
       </c>
       <c r="D12" s="34">
@@ -4205,16 +4226,16 @@
       <c r="F12" s="34">
         <v>0</v>
       </c>
-      <c r="G12" s="62" t="s">
-        <v>126</v>
-      </c>
-      <c r="H12" s="83"/>
-      <c r="I12" s="84"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A13" s="54"/>
-      <c r="B13" s="51"/>
-      <c r="C13" s="33" t="s">
+      <c r="G12" s="89" t="s">
+        <v>124</v>
+      </c>
+      <c r="H12" s="68"/>
+      <c r="I12" s="69"/>
+    </row>
+    <row r="13" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="83"/>
+      <c r="B13" s="84"/>
+      <c r="C13" s="90" t="s">
         <v>19</v>
       </c>
       <c r="D13" s="34">
@@ -4226,15 +4247,15 @@
       <c r="F13" s="34">
         <v>0</v>
       </c>
-      <c r="G13" s="62" t="s">
-        <v>126</v>
-      </c>
-      <c r="I13" s="84"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14" s="54"/>
-      <c r="B14" s="51"/>
-      <c r="C14" s="33" t="s">
+      <c r="G13" s="89" t="s">
+        <v>124</v>
+      </c>
+      <c r="I13" s="69"/>
+    </row>
+    <row r="14" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A14" s="83"/>
+      <c r="B14" s="84"/>
+      <c r="C14" s="90" t="s">
         <v>20</v>
       </c>
       <c r="D14" s="34">
@@ -4246,15 +4267,15 @@
       <c r="F14" s="34">
         <v>0</v>
       </c>
-      <c r="G14" s="62" t="s">
-        <v>126</v>
-      </c>
-      <c r="I14" s="84"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A15" s="54"/>
-      <c r="B15" s="51"/>
-      <c r="C15" s="33" t="s">
+      <c r="G14" s="89" t="s">
+        <v>124</v>
+      </c>
+      <c r="I14" s="69"/>
+    </row>
+    <row r="15" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="83"/>
+      <c r="B15" s="84"/>
+      <c r="C15" s="90" t="s">
         <v>21</v>
       </c>
       <c r="D15" s="34">
@@ -4266,14 +4287,14 @@
       <c r="F15" s="34">
         <v>0</v>
       </c>
-      <c r="G15" s="62" t="s">
-        <v>126</v>
-      </c>
-      <c r="I15" s="84"/>
+      <c r="G15" s="89" t="s">
+        <v>124</v>
+      </c>
+      <c r="I15" s="69"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A16" s="54"/>
-      <c r="B16" s="51"/>
+      <c r="A16" s="83"/>
+      <c r="B16" s="84"/>
       <c r="C16" s="33" t="s">
         <v>23</v>
       </c>
@@ -4286,12 +4307,12 @@
       <c r="F16" s="34">
         <v>1</v>
       </c>
-      <c r="G16" s="62"/>
-      <c r="I16" s="84"/>
+      <c r="G16" s="48"/>
+      <c r="I16" s="69"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" s="54"/>
-      <c r="B17" s="51"/>
+      <c r="A17" s="83"/>
+      <c r="B17" s="84"/>
       <c r="C17" s="33" t="s">
         <v>22</v>
       </c>
@@ -4304,12 +4325,12 @@
       <c r="F17" s="34">
         <v>1</v>
       </c>
-      <c r="G17" s="62"/>
-      <c r="I17" s="84"/>
+      <c r="G17" s="48"/>
+      <c r="I17" s="69"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" s="54"/>
-      <c r="B18" s="51"/>
+      <c r="A18" s="83"/>
+      <c r="B18" s="84"/>
       <c r="C18" s="27" t="s">
         <v>26</v>
       </c>
@@ -4322,12 +4343,12 @@
       <c r="F18" s="28" t="s">
         <v>119</v>
       </c>
-      <c r="G18" s="73"/>
-      <c r="I18" s="84"/>
+      <c r="G18" s="59"/>
+      <c r="I18" s="69"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="54"/>
-      <c r="B19" s="52"/>
+      <c r="A19" s="83"/>
+      <c r="B19" s="75"/>
       <c r="C19" s="3" t="s">
         <v>27</v>
       </c>
@@ -4340,12 +4361,12 @@
       <c r="F19" s="11">
         <v>1</v>
       </c>
-      <c r="G19" s="68"/>
-      <c r="I19" s="84"/>
+      <c r="G19" s="54"/>
+      <c r="I19" s="69"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A20" s="54"/>
-      <c r="B20" s="47" t="s">
+      <c r="A20" s="83"/>
+      <c r="B20" s="79" t="s">
         <v>28</v>
       </c>
       <c r="C20" s="20" t="s">
@@ -4360,12 +4381,12 @@
       <c r="F20" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="G20" s="64"/>
-      <c r="I20" s="84"/>
+      <c r="G20" s="50"/>
+      <c r="I20" s="69"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21" s="54"/>
-      <c r="B21" s="57"/>
+      <c r="A21" s="83"/>
+      <c r="B21" s="82"/>
       <c r="C21" s="22" t="s">
         <v>31</v>
       </c>
@@ -4378,12 +4399,12 @@
       <c r="F21" s="23" t="s">
         <v>119</v>
       </c>
-      <c r="G21" s="65"/>
-      <c r="I21" s="84"/>
+      <c r="G21" s="51"/>
+      <c r="I21" s="69"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A22" s="54"/>
-      <c r="B22" s="49"/>
+      <c r="A22" s="83"/>
+      <c r="B22" s="81"/>
       <c r="C22" s="7" t="s">
         <v>30</v>
       </c>
@@ -4396,10 +4417,10 @@
       <c r="F22" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="G22" s="72"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A23" s="54"/>
+      <c r="G22" s="58"/>
+    </row>
+    <row r="23" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A23" s="83"/>
       <c r="B23" s="4" t="s">
         <v>17</v>
       </c>
@@ -4415,13 +4436,13 @@
       <c r="F23" s="13">
         <v>1</v>
       </c>
-      <c r="G23" s="76" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A24" s="54"/>
-      <c r="B24" s="47" t="s">
+      <c r="G23" s="91" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A24" s="83"/>
+      <c r="B24" s="79" t="s">
         <v>16</v>
       </c>
       <c r="C24" s="20" t="s">
@@ -4436,13 +4457,13 @@
       <c r="F24" s="21">
         <v>1</v>
       </c>
-      <c r="G24" s="64" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A25" s="54"/>
-      <c r="B25" s="57"/>
+      <c r="G24" s="92" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A25" s="83"/>
+      <c r="B25" s="82"/>
       <c r="C25" s="6" t="s">
         <v>34</v>
       </c>
@@ -4455,8 +4476,8 @@
       <c r="F25" s="12">
         <v>0</v>
       </c>
-      <c r="G25" s="74" t="s">
-        <v>125</v>
+      <c r="G25" s="93" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
@@ -4466,13 +4487,13 @@
       <c r="D26" s="36"/>
       <c r="E26" s="36"/>
       <c r="F26" s="36"/>
-      <c r="G26" s="71"/>
+      <c r="G26" s="57"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A27" s="53" t="s">
-        <v>1</v>
-      </c>
-      <c r="B27" s="47" t="s">
+      <c r="A27" s="76" t="s">
+        <v>1</v>
+      </c>
+      <c r="B27" s="79" t="s">
         <v>35</v>
       </c>
       <c r="C27" s="20" t="s">
@@ -4487,12 +4508,12 @@
       <c r="F27" s="25">
         <v>1</v>
       </c>
-      <c r="G27" s="64"/>
-      <c r="I27" s="84"/>
+      <c r="G27" s="50"/>
+      <c r="I27" s="69"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A28" s="60"/>
-      <c r="B28" s="48"/>
+      <c r="A28" s="77"/>
+      <c r="B28" s="80"/>
       <c r="C28" s="22" t="s">
         <v>50</v>
       </c>
@@ -4505,14 +4526,14 @@
       <c r="F28" s="23">
         <v>1</v>
       </c>
-      <c r="G28" s="65" t="s">
+      <c r="G28" s="51" t="s">
         <v>101</v>
       </c>
-      <c r="I28" s="84"/>
+      <c r="I28" s="69"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A29" s="54"/>
-      <c r="B29" s="49"/>
+      <c r="A29" s="83"/>
+      <c r="B29" s="81"/>
       <c r="C29" s="7" t="s">
         <v>37</v>
       </c>
@@ -4525,12 +4546,12 @@
       <c r="F29" s="9">
         <v>1</v>
       </c>
-      <c r="G29" s="72"/>
-      <c r="I29" s="84"/>
+      <c r="G29" s="58"/>
+      <c r="I29" s="69"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A30" s="54"/>
-      <c r="B30" s="50" t="s">
+      <c r="A30" s="83"/>
+      <c r="B30" s="73" t="s">
         <v>36</v>
       </c>
       <c r="C30" s="31" t="s">
@@ -4545,12 +4566,12 @@
       <c r="F30" s="32">
         <v>1</v>
       </c>
-      <c r="G30" s="67"/>
-      <c r="I30" s="84"/>
+      <c r="G30" s="53"/>
+      <c r="I30" s="69"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A31" s="54"/>
-      <c r="B31" s="56"/>
+      <c r="A31" s="83"/>
+      <c r="B31" s="74"/>
       <c r="C31" s="27" t="s">
         <v>102</v>
       </c>
@@ -4563,12 +4584,12 @@
       <c r="F31" s="28">
         <v>1</v>
       </c>
-      <c r="G31" s="73"/>
-      <c r="I31" s="84"/>
+      <c r="G31" s="59"/>
+      <c r="I31" s="69"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A32" s="54"/>
-      <c r="B32" s="52"/>
+      <c r="A32" s="83"/>
+      <c r="B32" s="75"/>
       <c r="C32" s="3" t="s">
         <v>103</v>
       </c>
@@ -4581,12 +4602,12 @@
       <c r="F32" s="11">
         <v>1</v>
       </c>
-      <c r="G32" s="68"/>
-      <c r="I32" s="84"/>
+      <c r="G32" s="54"/>
+      <c r="I32" s="69"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A33" s="54"/>
-      <c r="B33" s="57" t="s">
+      <c r="A33" s="83"/>
+      <c r="B33" s="82" t="s">
         <v>16</v>
       </c>
       <c r="C33" s="20" t="s">
@@ -4601,12 +4622,12 @@
       <c r="F33" s="21">
         <v>1</v>
       </c>
-      <c r="G33" s="64"/>
-      <c r="I33" s="84"/>
+      <c r="G33" s="50"/>
+      <c r="I33" s="69"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A34" s="54"/>
-      <c r="B34" s="57"/>
+      <c r="A34" s="83"/>
+      <c r="B34" s="82"/>
       <c r="C34" s="22" t="s">
         <v>112</v>
       </c>
@@ -4619,12 +4640,12 @@
       <c r="F34" s="23">
         <v>0</v>
       </c>
-      <c r="G34" s="65"/>
-      <c r="I34" s="84"/>
+      <c r="G34" s="51"/>
+      <c r="I34" s="69"/>
     </row>
     <row r="35" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A35" s="55"/>
-      <c r="B35" s="57"/>
+      <c r="A35" s="78"/>
+      <c r="B35" s="82"/>
       <c r="C35" s="15" t="s">
         <v>42</v>
       </c>
@@ -4637,8 +4658,8 @@
       <c r="F35" s="12">
         <v>1</v>
       </c>
-      <c r="G35" s="74"/>
-      <c r="I35" s="84"/>
+      <c r="G35" s="60"/>
+      <c r="I35" s="69"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" s="14"/>
@@ -4647,14 +4668,14 @@
       <c r="D36" s="36"/>
       <c r="E36" s="36"/>
       <c r="F36" s="36"/>
-      <c r="G36" s="71"/>
-      <c r="I36" s="84"/>
+      <c r="G36" s="57"/>
+      <c r="I36" s="69"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A37" s="58" t="s">
+      <c r="A37" s="85" t="s">
         <v>49</v>
       </c>
-      <c r="B37" s="47" t="s">
+      <c r="B37" s="79" t="s">
         <v>35</v>
       </c>
       <c r="C37" s="20" t="s">
@@ -4669,12 +4690,12 @@
       <c r="F37" s="25">
         <v>0</v>
       </c>
-      <c r="G37" s="64"/>
-      <c r="I37" s="84"/>
+      <c r="G37" s="50"/>
+      <c r="I37" s="69"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A38" s="59"/>
-      <c r="B38" s="48"/>
+      <c r="A38" s="86"/>
+      <c r="B38" s="80"/>
       <c r="C38" s="22" t="s">
         <v>43</v>
       </c>
@@ -4687,12 +4708,12 @@
       <c r="F38" s="23">
         <v>1</v>
       </c>
-      <c r="G38" s="65"/>
-      <c r="I38" s="84"/>
+      <c r="G38" s="51"/>
+      <c r="I38" s="69"/>
     </row>
     <row r="39" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A39" s="54"/>
-      <c r="B39" s="49"/>
+      <c r="A39" s="83"/>
+      <c r="B39" s="81"/>
       <c r="C39" s="17" t="s">
         <v>44</v>
       </c>
@@ -4705,12 +4726,12 @@
       <c r="F39" s="9">
         <v>1</v>
       </c>
-      <c r="G39" s="72"/>
-      <c r="I39" s="84"/>
+      <c r="G39" s="58"/>
+      <c r="I39" s="69"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A40" s="54"/>
-      <c r="B40" s="50" t="s">
+      <c r="A40" s="83"/>
+      <c r="B40" s="73" t="s">
         <v>48</v>
       </c>
       <c r="C40" s="38" t="s">
@@ -4725,12 +4746,12 @@
       <c r="F40" s="18">
         <v>1</v>
       </c>
-      <c r="G40" s="75"/>
-      <c r="I40" s="84"/>
+      <c r="G40" s="61"/>
+      <c r="I40" s="69"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A41" s="54"/>
-      <c r="B41" s="52"/>
+      <c r="A41" s="83"/>
+      <c r="B41" s="75"/>
       <c r="C41" s="2" t="s">
         <v>61</v>
       </c>
@@ -4743,12 +4764,12 @@
       <c r="F41" s="18">
         <v>1</v>
       </c>
-      <c r="G41" s="75"/>
-      <c r="I41" s="84"/>
+      <c r="G41" s="61"/>
+      <c r="I41" s="69"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A42" s="54"/>
-      <c r="B42" s="47" t="s">
+      <c r="A42" s="83"/>
+      <c r="B42" s="79" t="s">
         <v>36</v>
       </c>
       <c r="C42" s="20" t="s">
@@ -4763,12 +4784,12 @@
       <c r="F42" s="21">
         <v>0</v>
       </c>
-      <c r="G42" s="64"/>
-      <c r="I42" s="84"/>
+      <c r="G42" s="50"/>
+      <c r="I42" s="69"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A43" s="54"/>
-      <c r="B43" s="48"/>
+      <c r="A43" s="83"/>
+      <c r="B43" s="80"/>
       <c r="C43" s="22" t="s">
         <v>45</v>
       </c>
@@ -4781,12 +4802,12 @@
       <c r="F43" s="23">
         <v>1</v>
       </c>
-      <c r="G43" s="65"/>
-      <c r="I43" s="84"/>
+      <c r="G43" s="51"/>
+      <c r="I43" s="69"/>
     </row>
     <row r="44" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A44" s="54"/>
-      <c r="B44" s="49"/>
+      <c r="A44" s="83"/>
+      <c r="B44" s="81"/>
       <c r="C44" s="17" t="s">
         <v>46</v>
       </c>
@@ -4799,11 +4820,11 @@
       <c r="F44" s="9">
         <v>1</v>
       </c>
-      <c r="G44" s="72"/>
-      <c r="I44" s="84"/>
+      <c r="G44" s="58"/>
+      <c r="I44" s="69"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A45" s="55"/>
+      <c r="A45" s="78"/>
       <c r="B45" s="39" t="s">
         <v>16</v>
       </c>
@@ -4819,8 +4840,8 @@
       <c r="F45" s="10">
         <v>1</v>
       </c>
-      <c r="G45" s="70"/>
-      <c r="I45" s="84"/>
+      <c r="G45" s="56"/>
+      <c r="I45" s="69"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" s="14"/>
@@ -4829,14 +4850,14 @@
       <c r="D46" s="36"/>
       <c r="E46" s="36"/>
       <c r="F46" s="36"/>
-      <c r="G46" s="71"/>
-      <c r="I46" s="84"/>
+      <c r="G46" s="57"/>
+      <c r="I46" s="69"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A47" s="53" t="s">
+      <c r="A47" s="76" t="s">
         <v>4</v>
       </c>
-      <c r="B47" s="47" t="s">
+      <c r="B47" s="79" t="s">
         <v>35</v>
       </c>
       <c r="C47" s="20" t="s">
@@ -4851,12 +4872,12 @@
       <c r="F47" s="25">
         <v>0</v>
       </c>
-      <c r="G47" s="64"/>
-      <c r="I47" s="84"/>
+      <c r="G47" s="50"/>
+      <c r="I47" s="69"/>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A48" s="54"/>
-      <c r="B48" s="48"/>
+      <c r="A48" s="83"/>
+      <c r="B48" s="80"/>
       <c r="C48" s="22" t="s">
         <v>52</v>
       </c>
@@ -4869,12 +4890,12 @@
       <c r="F48" s="23">
         <v>1</v>
       </c>
-      <c r="G48" s="65"/>
-      <c r="I48" s="84"/>
+      <c r="G48" s="51"/>
+      <c r="I48" s="69"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A49" s="54"/>
-      <c r="B49" s="48"/>
+      <c r="A49" s="83"/>
+      <c r="B49" s="80"/>
       <c r="C49" s="22" t="s">
         <v>53</v>
       </c>
@@ -4887,12 +4908,12 @@
       <c r="F49" s="23">
         <v>1</v>
       </c>
-      <c r="G49" s="65"/>
-      <c r="I49" s="84"/>
+      <c r="G49" s="51"/>
+      <c r="I49" s="69"/>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A50" s="54"/>
-      <c r="B50" s="49"/>
+      <c r="A50" s="83"/>
+      <c r="B50" s="81"/>
       <c r="C50" s="7" t="s">
         <v>54</v>
       </c>
@@ -4905,12 +4926,12 @@
       <c r="F50" s="9">
         <v>1</v>
       </c>
-      <c r="G50" s="72"/>
-      <c r="I50" s="84"/>
+      <c r="G50" s="58"/>
+      <c r="I50" s="69"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A51" s="54"/>
-      <c r="B51" s="56" t="s">
+      <c r="A51" s="83"/>
+      <c r="B51" s="74" t="s">
         <v>36</v>
       </c>
       <c r="C51" s="27" t="s">
@@ -4925,12 +4946,12 @@
       <c r="F51" s="28">
         <v>0</v>
       </c>
-      <c r="G51" s="73"/>
-      <c r="I51" s="84"/>
+      <c r="G51" s="59"/>
+      <c r="I51" s="69"/>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A52" s="54"/>
-      <c r="B52" s="56"/>
+      <c r="A52" s="83"/>
+      <c r="B52" s="74"/>
       <c r="C52" s="33" t="s">
         <v>55</v>
       </c>
@@ -4943,12 +4964,12 @@
       <c r="F52" s="34">
         <v>1</v>
       </c>
-      <c r="G52" s="62"/>
-      <c r="I52" s="84"/>
+      <c r="G52" s="48"/>
+      <c r="I52" s="69"/>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A53" s="54"/>
-      <c r="B53" s="56"/>
+      <c r="A53" s="83"/>
+      <c r="B53" s="74"/>
       <c r="C53" s="33" t="s">
         <v>56</v>
       </c>
@@ -4961,12 +4982,12 @@
       <c r="F53" s="34">
         <v>1</v>
       </c>
-      <c r="G53" s="62"/>
-      <c r="I53" s="84"/>
+      <c r="G53" s="48"/>
+      <c r="I53" s="69"/>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A54" s="54"/>
-      <c r="B54" s="52"/>
+      <c r="A54" s="83"/>
+      <c r="B54" s="75"/>
       <c r="C54" s="3" t="s">
         <v>57</v>
       </c>
@@ -4979,12 +5000,12 @@
       <c r="F54" s="11">
         <v>1</v>
       </c>
-      <c r="G54" s="68"/>
-      <c r="I54" s="84"/>
+      <c r="G54" s="54"/>
+      <c r="I54" s="69"/>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A55" s="54"/>
-      <c r="B55" s="57" t="s">
+      <c r="A55" s="83"/>
+      <c r="B55" s="82" t="s">
         <v>16</v>
       </c>
       <c r="C55" s="24" t="s">
@@ -4999,12 +5020,12 @@
       <c r="F55" s="25">
         <v>1</v>
       </c>
-      <c r="G55" s="66"/>
-      <c r="I55" s="84"/>
+      <c r="G55" s="52"/>
+      <c r="I55" s="69"/>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A56" s="55"/>
-      <c r="B56" s="57"/>
+      <c r="A56" s="78"/>
+      <c r="B56" s="82"/>
       <c r="C56" s="16" t="s">
         <v>59</v>
       </c>
@@ -5017,8 +5038,8 @@
       <c r="F56" s="12">
         <v>1</v>
       </c>
-      <c r="G56" s="74"/>
-      <c r="I56" s="84"/>
+      <c r="G56" s="60"/>
+      <c r="I56" s="69"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57" s="14"/>
@@ -5027,14 +5048,14 @@
       <c r="D57" s="36"/>
       <c r="E57" s="36"/>
       <c r="F57" s="36"/>
-      <c r="G57" s="71"/>
-      <c r="I57" s="84"/>
+      <c r="G57" s="57"/>
+      <c r="I57" s="69"/>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A58" s="53" t="s">
+      <c r="A58" s="76" t="s">
         <v>3</v>
       </c>
-      <c r="B58" s="47" t="s">
+      <c r="B58" s="79" t="s">
         <v>35</v>
       </c>
       <c r="C58" s="20" t="s">
@@ -5049,12 +5070,12 @@
       <c r="F58" s="25">
         <v>0</v>
       </c>
-      <c r="G58" s="64"/>
-      <c r="I58" s="84"/>
+      <c r="G58" s="50"/>
+      <c r="I58" s="69"/>
     </row>
     <row r="59" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A59" s="54"/>
-      <c r="B59" s="48"/>
+      <c r="A59" s="83"/>
+      <c r="B59" s="80"/>
       <c r="C59" s="43" t="s">
         <v>62</v>
       </c>
@@ -5067,14 +5088,14 @@
       <c r="F59" s="23">
         <v>0</v>
       </c>
-      <c r="G59" s="65" t="s">
+      <c r="G59" s="51" t="s">
         <v>101</v>
       </c>
-      <c r="I59" s="84"/>
+      <c r="I59" s="69"/>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A60" s="54"/>
-      <c r="B60" s="48"/>
+      <c r="A60" s="83"/>
+      <c r="B60" s="80"/>
       <c r="C60" s="22" t="s">
         <v>63</v>
       </c>
@@ -5087,12 +5108,12 @@
       <c r="F60" s="23">
         <v>0</v>
       </c>
-      <c r="G60" s="65"/>
-      <c r="I60" s="84"/>
+      <c r="G60" s="51"/>
+      <c r="I60" s="69"/>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A61" s="54"/>
-      <c r="B61" s="49"/>
+      <c r="A61" s="83"/>
+      <c r="B61" s="81"/>
       <c r="C61" s="7" t="s">
         <v>64</v>
       </c>
@@ -5105,12 +5126,12 @@
       <c r="F61" s="9">
         <v>1</v>
       </c>
-      <c r="G61" s="72"/>
-      <c r="I61" s="84"/>
+      <c r="G61" s="58"/>
+      <c r="I61" s="69"/>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A62" s="54"/>
-      <c r="B62" s="50" t="s">
+      <c r="A62" s="83"/>
+      <c r="B62" s="73" t="s">
         <v>36</v>
       </c>
       <c r="C62" s="31" t="s">
@@ -5125,12 +5146,12 @@
       <c r="F62" s="32">
         <v>0</v>
       </c>
-      <c r="G62" s="67"/>
-      <c r="I62" s="84"/>
+      <c r="G62" s="53"/>
+      <c r="I62" s="69"/>
     </row>
     <row r="63" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A63" s="54"/>
-      <c r="B63" s="56"/>
+      <c r="A63" s="83"/>
+      <c r="B63" s="74"/>
       <c r="C63" s="44" t="s">
         <v>65</v>
       </c>
@@ -5143,14 +5164,14 @@
       <c r="F63" s="34">
         <v>0</v>
       </c>
-      <c r="G63" s="62" t="s">
+      <c r="G63" s="48" t="s">
         <v>101</v>
       </c>
-      <c r="I63" s="84"/>
+      <c r="I63" s="69"/>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A64" s="54"/>
-      <c r="B64" s="56"/>
+      <c r="A64" s="83"/>
+      <c r="B64" s="74"/>
       <c r="C64" s="33" t="s">
         <v>66</v>
       </c>
@@ -5163,12 +5184,12 @@
       <c r="F64" s="34">
         <v>0</v>
       </c>
-      <c r="G64" s="62"/>
-      <c r="I64" s="84"/>
+      <c r="G64" s="48"/>
+      <c r="I64" s="69"/>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A65" s="54"/>
-      <c r="B65" s="52"/>
+      <c r="A65" s="83"/>
+      <c r="B65" s="75"/>
       <c r="C65" s="3" t="s">
         <v>67</v>
       </c>
@@ -5181,12 +5202,12 @@
       <c r="F65" s="11">
         <v>1</v>
       </c>
-      <c r="G65" s="68"/>
-      <c r="I65" s="84"/>
+      <c r="G65" s="54"/>
+      <c r="I65" s="69"/>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A66" s="54"/>
-      <c r="B66" s="86" t="s">
+      <c r="A66" s="83"/>
+      <c r="B66" s="87" t="s">
         <v>121</v>
       </c>
       <c r="C66" s="20" t="s">
@@ -5201,12 +5222,12 @@
       <c r="F66" s="21">
         <v>1</v>
       </c>
-      <c r="G66" s="64"/>
-      <c r="I66" s="84"/>
+      <c r="G66" s="50"/>
+      <c r="I66" s="69"/>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A67" s="54"/>
-      <c r="B67" s="48"/>
+      <c r="A67" s="83"/>
+      <c r="B67" s="80"/>
       <c r="C67" s="22" t="s">
         <v>69</v>
       </c>
@@ -5219,12 +5240,12 @@
       <c r="F67" s="23">
         <v>1</v>
       </c>
-      <c r="G67" s="65"/>
-      <c r="I67" s="84"/>
+      <c r="G67" s="51"/>
+      <c r="I67" s="69"/>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A68" s="54"/>
-      <c r="B68" s="49"/>
+      <c r="A68" s="83"/>
+      <c r="B68" s="81"/>
       <c r="C68" s="7" t="s">
         <v>70</v>
       </c>
@@ -5237,12 +5258,12 @@
       <c r="F68" s="9">
         <v>1</v>
       </c>
-      <c r="G68" s="72"/>
-      <c r="I68" s="84"/>
+      <c r="G68" s="58"/>
+      <c r="I68" s="69"/>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A69" s="54"/>
-      <c r="B69" s="87" t="s">
+      <c r="A69" s="83"/>
+      <c r="B69" s="88" t="s">
         <v>122</v>
       </c>
       <c r="C69" s="31" t="s">
@@ -5257,12 +5278,12 @@
       <c r="F69" s="32" t="s">
         <v>119</v>
       </c>
-      <c r="G69" s="67"/>
-      <c r="I69" s="84"/>
+      <c r="G69" s="53"/>
+      <c r="I69" s="69"/>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A70" s="54"/>
-      <c r="B70" s="51"/>
+      <c r="A70" s="83"/>
+      <c r="B70" s="84"/>
       <c r="C70" s="33" t="s">
         <v>72</v>
       </c>
@@ -5275,12 +5296,12 @@
       <c r="F70" s="34" t="s">
         <v>119</v>
       </c>
-      <c r="G70" s="62"/>
-      <c r="I70" s="84"/>
+      <c r="G70" s="48"/>
+      <c r="I70" s="69"/>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A71" s="54"/>
-      <c r="B71" s="56"/>
+      <c r="A71" s="83"/>
+      <c r="B71" s="74"/>
       <c r="C71" s="40" t="s">
         <v>73</v>
       </c>
@@ -5293,12 +5314,12 @@
       <c r="F71" s="18" t="s">
         <v>119</v>
       </c>
-      <c r="G71" s="75"/>
-      <c r="I71" s="84"/>
+      <c r="G71" s="61"/>
+      <c r="I71" s="69"/>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A72" s="54"/>
-      <c r="B72" s="47" t="s">
+      <c r="A72" s="83"/>
+      <c r="B72" s="79" t="s">
         <v>16</v>
       </c>
       <c r="C72" s="20" t="s">
@@ -5313,12 +5334,12 @@
       <c r="F72" s="21">
         <v>1</v>
       </c>
-      <c r="G72" s="64"/>
-      <c r="I72" s="84"/>
+      <c r="G72" s="50"/>
+      <c r="I72" s="69"/>
     </row>
     <row r="73" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A73" s="54"/>
-      <c r="B73" s="48"/>
+      <c r="A73" s="83"/>
+      <c r="B73" s="80"/>
       <c r="C73" s="43" t="s">
         <v>76</v>
       </c>
@@ -5331,12 +5352,12 @@
       <c r="F73" s="23" t="s">
         <v>119</v>
       </c>
-      <c r="G73" s="65"/>
-      <c r="I73" s="84"/>
+      <c r="G73" s="51"/>
+      <c r="I73" s="69"/>
     </row>
     <row r="74" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A74" s="55"/>
-      <c r="B74" s="49"/>
+      <c r="A74" s="78"/>
+      <c r="B74" s="81"/>
       <c r="C74" s="17" t="s">
         <v>77</v>
       </c>
@@ -5349,8 +5370,8 @@
       <c r="F74" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="G74" s="72"/>
-      <c r="I74" s="84"/>
+      <c r="G74" s="58"/>
+      <c r="I74" s="69"/>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A75" s="14"/>
@@ -5359,14 +5380,14 @@
       <c r="D75" s="36"/>
       <c r="E75" s="36"/>
       <c r="F75" s="36"/>
-      <c r="G75" s="71"/>
-      <c r="I75" s="84"/>
+      <c r="G75" s="57"/>
+      <c r="I75" s="69"/>
     </row>
     <row r="76" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A76" s="53" t="s">
+      <c r="A76" s="76" t="s">
         <v>2</v>
       </c>
-      <c r="B76" s="47" t="s">
+      <c r="B76" s="79" t="s">
         <v>35</v>
       </c>
       <c r="C76" s="20" t="s">
@@ -5381,14 +5402,14 @@
       <c r="F76" s="25">
         <v>0</v>
       </c>
-      <c r="G76" s="64" t="s">
+      <c r="G76" s="50" t="s">
         <v>115</v>
       </c>
-      <c r="I76" s="84"/>
+      <c r="I76" s="69"/>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A77" s="60"/>
-      <c r="B77" s="48"/>
+      <c r="A77" s="77"/>
+      <c r="B77" s="80"/>
       <c r="C77" s="22" t="s">
         <v>79</v>
       </c>
@@ -5401,14 +5422,14 @@
       <c r="F77" s="23">
         <v>0</v>
       </c>
-      <c r="G77" s="65" t="s">
+      <c r="G77" s="51" t="s">
         <v>115</v>
       </c>
-      <c r="I77" s="84"/>
+      <c r="I77" s="69"/>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A78" s="60"/>
-      <c r="B78" s="48"/>
+      <c r="A78" s="77"/>
+      <c r="B78" s="80"/>
       <c r="C78" s="22" t="s">
         <v>80</v>
       </c>
@@ -5421,12 +5442,12 @@
       <c r="F78" s="25">
         <v>1</v>
       </c>
-      <c r="G78" s="65"/>
-      <c r="I78" s="84"/>
+      <c r="G78" s="51"/>
+      <c r="I78" s="69"/>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A79" s="60"/>
-      <c r="B79" s="48"/>
+      <c r="A79" s="77"/>
+      <c r="B79" s="80"/>
       <c r="C79" s="22" t="s">
         <v>81</v>
       </c>
@@ -5439,12 +5460,12 @@
       <c r="F79" s="25">
         <v>1</v>
       </c>
-      <c r="G79" s="65"/>
-      <c r="I79" s="84"/>
+      <c r="G79" s="51"/>
+      <c r="I79" s="69"/>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A80" s="60"/>
-      <c r="B80" s="48"/>
+      <c r="A80" s="77"/>
+      <c r="B80" s="80"/>
       <c r="C80" s="22" t="s">
         <v>83</v>
       </c>
@@ -5457,14 +5478,14 @@
       <c r="F80" s="25">
         <v>0</v>
       </c>
-      <c r="G80" s="65" t="s">
+      <c r="G80" s="51" t="s">
         <v>115</v>
       </c>
-      <c r="I80" s="84"/>
+      <c r="I80" s="69"/>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A81" s="60"/>
-      <c r="B81" s="48"/>
+      <c r="A81" s="77"/>
+      <c r="B81" s="80"/>
       <c r="C81" s="22" t="s">
         <v>84</v>
       </c>
@@ -5477,14 +5498,14 @@
       <c r="F81" s="25">
         <v>0</v>
       </c>
-      <c r="G81" s="65" t="s">
+      <c r="G81" s="51" t="s">
         <v>115</v>
       </c>
-      <c r="I81" s="84"/>
+      <c r="I81" s="69"/>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A82" s="60"/>
-      <c r="B82" s="48"/>
+      <c r="A82" s="77"/>
+      <c r="B82" s="80"/>
       <c r="C82" s="22" t="s">
         <v>85</v>
       </c>
@@ -5497,12 +5518,12 @@
       <c r="F82" s="25">
         <v>1</v>
       </c>
-      <c r="G82" s="65"/>
-      <c r="I82" s="84"/>
+      <c r="G82" s="51"/>
+      <c r="I82" s="69"/>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A83" s="60"/>
-      <c r="B83" s="49"/>
+      <c r="A83" s="77"/>
+      <c r="B83" s="81"/>
       <c r="C83" s="7" t="s">
         <v>82</v>
       </c>
@@ -5515,12 +5536,12 @@
       <c r="F83" s="9">
         <v>1</v>
       </c>
-      <c r="G83" s="72"/>
-      <c r="I83" s="84"/>
+      <c r="G83" s="58"/>
+      <c r="I83" s="69"/>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A84" s="60"/>
-      <c r="B84" s="50" t="s">
+      <c r="A84" s="77"/>
+      <c r="B84" s="73" t="s">
         <v>36</v>
       </c>
       <c r="C84" s="31" t="s">
@@ -5535,14 +5556,14 @@
       <c r="F84" s="32">
         <v>0</v>
       </c>
-      <c r="G84" s="67" t="s">
+      <c r="G84" s="53" t="s">
         <v>115</v>
       </c>
-      <c r="I84" s="84"/>
+      <c r="I84" s="69"/>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A85" s="60"/>
-      <c r="B85" s="51"/>
+      <c r="A85" s="77"/>
+      <c r="B85" s="84"/>
       <c r="C85" s="27" t="s">
         <v>87</v>
       </c>
@@ -5555,14 +5576,14 @@
       <c r="F85" s="34">
         <v>0</v>
       </c>
-      <c r="G85" s="73" t="s">
+      <c r="G85" s="59" t="s">
         <v>115</v>
       </c>
-      <c r="I85" s="84"/>
+      <c r="I85" s="69"/>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A86" s="60"/>
-      <c r="B86" s="51"/>
+      <c r="A86" s="77"/>
+      <c r="B86" s="84"/>
       <c r="C86" s="27" t="s">
         <v>88</v>
       </c>
@@ -5575,12 +5596,12 @@
       <c r="F86" s="28">
         <v>1</v>
       </c>
-      <c r="G86" s="73"/>
-      <c r="I86" s="84"/>
+      <c r="G86" s="59"/>
+      <c r="I86" s="69"/>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A87" s="60"/>
-      <c r="B87" s="51"/>
+      <c r="A87" s="77"/>
+      <c r="B87" s="84"/>
       <c r="C87" s="27" t="s">
         <v>89</v>
       </c>
@@ -5593,12 +5614,12 @@
       <c r="F87" s="34">
         <v>1</v>
       </c>
-      <c r="G87" s="73"/>
-      <c r="I87" s="84"/>
+      <c r="G87" s="59"/>
+      <c r="I87" s="69"/>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A88" s="60"/>
-      <c r="B88" s="51"/>
+      <c r="A88" s="77"/>
+      <c r="B88" s="84"/>
       <c r="C88" s="27" t="s">
         <v>90</v>
       </c>
@@ -5611,14 +5632,14 @@
       <c r="F88" s="34">
         <v>0</v>
       </c>
-      <c r="G88" s="73" t="s">
+      <c r="G88" s="59" t="s">
         <v>115</v>
       </c>
-      <c r="I88" s="84"/>
+      <c r="I88" s="69"/>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A89" s="60"/>
-      <c r="B89" s="51"/>
+      <c r="A89" s="77"/>
+      <c r="B89" s="84"/>
       <c r="C89" s="27" t="s">
         <v>91</v>
       </c>
@@ -5631,14 +5652,14 @@
       <c r="F89" s="34">
         <v>0</v>
       </c>
-      <c r="G89" s="73" t="s">
+      <c r="G89" s="59" t="s">
         <v>115</v>
       </c>
-      <c r="I89" s="84"/>
+      <c r="I89" s="69"/>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A90" s="60"/>
-      <c r="B90" s="51"/>
+      <c r="A90" s="77"/>
+      <c r="B90" s="84"/>
       <c r="C90" s="27" t="s">
         <v>92</v>
       </c>
@@ -5651,12 +5672,12 @@
       <c r="F90" s="34">
         <v>1</v>
       </c>
-      <c r="G90" s="73"/>
-      <c r="I90" s="84"/>
+      <c r="G90" s="59"/>
+      <c r="I90" s="69"/>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A91" s="60"/>
-      <c r="B91" s="52"/>
+      <c r="A91" s="77"/>
+      <c r="B91" s="75"/>
       <c r="C91" s="3" t="s">
         <v>93</v>
       </c>
@@ -5669,12 +5690,12 @@
       <c r="F91" s="11">
         <v>1</v>
       </c>
-      <c r="G91" s="68"/>
-      <c r="I91" s="82"/>
+      <c r="G91" s="54"/>
+      <c r="I91" s="67"/>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A92" s="60"/>
-      <c r="B92" s="47" t="s">
+      <c r="A92" s="77"/>
+      <c r="B92" s="79" t="s">
         <v>16</v>
       </c>
       <c r="C92" s="20" t="s">
@@ -5689,12 +5710,12 @@
       <c r="F92" s="21">
         <v>1</v>
       </c>
-      <c r="G92" s="64"/>
-      <c r="I92" s="82"/>
+      <c r="G92" s="50"/>
+      <c r="I92" s="67"/>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A93" s="60"/>
-      <c r="B93" s="49"/>
+      <c r="A93" s="77"/>
+      <c r="B93" s="81"/>
       <c r="C93" s="6" t="s">
         <v>95</v>
       </c>
@@ -5707,12 +5728,12 @@
       <c r="F93" s="12">
         <v>1</v>
       </c>
-      <c r="G93" s="74"/>
-      <c r="I93" s="82"/>
+      <c r="G93" s="60"/>
+      <c r="I93" s="67"/>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A94" s="60"/>
-      <c r="B94" s="50" t="s">
+      <c r="A94" s="77"/>
+      <c r="B94" s="73" t="s">
         <v>107</v>
       </c>
       <c r="C94" s="31" t="s">
@@ -5727,12 +5748,12 @@
       <c r="F94" s="32">
         <v>1</v>
       </c>
-      <c r="G94" s="67"/>
-      <c r="I94" s="82"/>
+      <c r="G94" s="53"/>
+      <c r="I94" s="67"/>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A95" s="60"/>
-      <c r="B95" s="56"/>
+      <c r="A95" s="77"/>
+      <c r="B95" s="74"/>
       <c r="C95" s="33" t="s">
         <v>113</v>
       </c>
@@ -5745,12 +5766,12 @@
       <c r="F95" s="34" t="s">
         <v>119</v>
       </c>
-      <c r="G95" s="62"/>
-      <c r="I95" s="82"/>
+      <c r="G95" s="48"/>
+      <c r="I95" s="67"/>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A96" s="60"/>
-      <c r="B96" s="56"/>
+      <c r="A96" s="77"/>
+      <c r="B96" s="74"/>
       <c r="C96" s="33" t="s">
         <v>109</v>
       </c>
@@ -5763,11 +5784,11 @@
       <c r="F96" s="34">
         <v>1</v>
       </c>
-      <c r="G96" s="62"/>
+      <c r="G96" s="48"/>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A97" s="55"/>
-      <c r="B97" s="52"/>
+      <c r="A97" s="78"/>
+      <c r="B97" s="75"/>
       <c r="C97" s="40" t="s">
         <v>114</v>
       </c>
@@ -5780,7 +5801,7 @@
       <c r="F97" s="18" t="s">
         <v>119</v>
       </c>
-      <c r="G97" s="75"/>
+      <c r="G97" s="61"/>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A98" s="14"/>
@@ -5789,21 +5810,19 @@
       <c r="D98" s="36"/>
       <c r="E98" s="36"/>
       <c r="F98" s="36"/>
-      <c r="G98" s="71"/>
+      <c r="G98" s="57"/>
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="A76:A97"/>
-    <mergeCell ref="B76:B83"/>
-    <mergeCell ref="B84:B91"/>
-    <mergeCell ref="B92:B93"/>
-    <mergeCell ref="B94:B97"/>
-    <mergeCell ref="A58:A74"/>
-    <mergeCell ref="B58:B61"/>
-    <mergeCell ref="B62:B65"/>
-    <mergeCell ref="B66:B68"/>
-    <mergeCell ref="B69:B71"/>
-    <mergeCell ref="B72:B74"/>
+    <mergeCell ref="A27:A35"/>
+    <mergeCell ref="B27:B29"/>
+    <mergeCell ref="B30:B32"/>
+    <mergeCell ref="B33:B35"/>
+    <mergeCell ref="A4:A25"/>
+    <mergeCell ref="B4:B10"/>
+    <mergeCell ref="B11:B19"/>
+    <mergeCell ref="B20:B22"/>
+    <mergeCell ref="B24:B25"/>
     <mergeCell ref="A37:A45"/>
     <mergeCell ref="B37:B39"/>
     <mergeCell ref="B40:B41"/>
@@ -5812,15 +5831,17 @@
     <mergeCell ref="B47:B50"/>
     <mergeCell ref="B51:B54"/>
     <mergeCell ref="B55:B56"/>
-    <mergeCell ref="A4:A25"/>
-    <mergeCell ref="B4:B10"/>
-    <mergeCell ref="B11:B19"/>
-    <mergeCell ref="B20:B22"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="A27:A35"/>
-    <mergeCell ref="B27:B29"/>
-    <mergeCell ref="B30:B32"/>
-    <mergeCell ref="B33:B35"/>
+    <mergeCell ref="A58:A74"/>
+    <mergeCell ref="B58:B61"/>
+    <mergeCell ref="B62:B65"/>
+    <mergeCell ref="B66:B68"/>
+    <mergeCell ref="B69:B71"/>
+    <mergeCell ref="B72:B74"/>
+    <mergeCell ref="A76:A97"/>
+    <mergeCell ref="B76:B83"/>
+    <mergeCell ref="B84:B91"/>
+    <mergeCell ref="B92:B93"/>
+    <mergeCell ref="B94:B97"/>
   </mergeCells>
   <conditionalFormatting sqref="D99:F1048576 D69:F74 D3:F3 D76:E93 D10:F10 D4:E9 D18:F26 D11:E17 D36:F36 D27:E35 D46:F46 D37:E45 D47:E56 D58:E68">
     <cfRule type="iconSet" priority="17">

</xml_diff>

<commit_message>
Report and tests updated
</commit_message>
<xml_diff>
--- a/Doc/Tests/liste_de_tests.xlsx
+++ b/Doc/Tests/liste_de_tests.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D3D91A6-22F1-4A36-9F01-90FD2E45E405}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F558BB1-DE3E-4D19-8FB8-56DB2DB74271}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="132">
   <si>
     <t>Client</t>
   </si>
@@ -396,9 +396,6 @@
     <t>-</t>
   </si>
   <si>
-    <t>(application refuse / ça ne marche pas)</t>
-  </si>
-  <si>
     <t>Catégories du 
 budget</t>
   </si>
@@ -425,6 +422,21 @@
   <si>
     <t>Client pas supprimé si dépendances 
 avec autres tables (conflit DB/BLL)</t>
+  </si>
+  <si>
+    <t>(l'application doit accepter)</t>
+  </si>
+  <si>
+    <t>(l'application doit refuser)</t>
+  </si>
+  <si>
+    <t>Connexion</t>
+  </si>
+  <si>
+    <t>Tableau de bord</t>
+  </si>
+  <si>
+    <t>Le résumé du compte par défaut s'affiche sur le tableau de bord</t>
   </si>
 </sst>
 </file>
@@ -739,6 +751,21 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -772,34 +799,19 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1146,10 +1158,10 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="76" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="80" t="s">
+      <c r="A2" s="81" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="85" t="s">
         <v>14</v>
       </c>
       <c r="C2" s="20" t="s">
@@ -1164,8 +1176,8 @@
       <c r="F2" s="50"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="83"/>
-      <c r="B3" s="80"/>
+      <c r="A3" s="88"/>
+      <c r="B3" s="85"/>
       <c r="C3" s="22" t="s">
         <v>8</v>
       </c>
@@ -1184,8 +1196,8 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="83"/>
-      <c r="B4" s="80"/>
+      <c r="A4" s="88"/>
+      <c r="B4" s="85"/>
       <c r="C4" s="22" t="s">
         <v>9</v>
       </c>
@@ -1204,8 +1216,8 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="83"/>
-      <c r="B5" s="80"/>
+      <c r="A5" s="88"/>
+      <c r="B5" s="85"/>
       <c r="C5" s="22" t="s">
         <v>10</v>
       </c>
@@ -1218,8 +1230,8 @@
       <c r="F5" s="51"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="83"/>
-      <c r="B6" s="80"/>
+      <c r="A6" s="88"/>
+      <c r="B6" s="85"/>
       <c r="C6" s="24" t="s">
         <v>11</v>
       </c>
@@ -1232,8 +1244,8 @@
       <c r="F6" s="52"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="83"/>
-      <c r="B7" s="80"/>
+      <c r="A7" s="88"/>
+      <c r="B7" s="85"/>
       <c r="C7" s="24" t="s">
         <v>12</v>
       </c>
@@ -1246,8 +1258,8 @@
       <c r="F7" s="52"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="83"/>
-      <c r="B8" s="81"/>
+      <c r="A8" s="88"/>
+      <c r="B8" s="86"/>
       <c r="C8" s="29" t="s">
         <v>24</v>
       </c>
@@ -1260,8 +1272,8 @@
       <c r="F8" s="66"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="83"/>
-      <c r="B9" s="73" t="s">
+      <c r="A9" s="88"/>
+      <c r="B9" s="78" t="s">
         <v>15</v>
       </c>
       <c r="C9" s="31" t="s">
@@ -1276,8 +1288,8 @@
       <c r="F9" s="53"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="83"/>
-      <c r="B10" s="84"/>
+      <c r="A10" s="88"/>
+      <c r="B10" s="91"/>
       <c r="C10" s="33" t="s">
         <v>13</v>
       </c>
@@ -1290,8 +1302,8 @@
       <c r="F10" s="48"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="83"/>
-      <c r="B11" s="84"/>
+      <c r="A11" s="88"/>
+      <c r="B11" s="91"/>
       <c r="C11" s="33" t="s">
         <v>19</v>
       </c>
@@ -1304,8 +1316,8 @@
       <c r="F11" s="48"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="83"/>
-      <c r="B12" s="84"/>
+      <c r="A12" s="88"/>
+      <c r="B12" s="91"/>
       <c r="C12" s="33" t="s">
         <v>20</v>
       </c>
@@ -1318,8 +1330,8 @@
       <c r="F12" s="48"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="83"/>
-      <c r="B13" s="84"/>
+      <c r="A13" s="88"/>
+      <c r="B13" s="91"/>
       <c r="C13" s="33" t="s">
         <v>21</v>
       </c>
@@ -1332,8 +1344,8 @@
       <c r="F13" s="48"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="83"/>
-      <c r="B14" s="84"/>
+      <c r="A14" s="88"/>
+      <c r="B14" s="91"/>
       <c r="C14" s="33" t="s">
         <v>23</v>
       </c>
@@ -1346,8 +1358,8 @@
       <c r="F14" s="48"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="83"/>
-      <c r="B15" s="84"/>
+      <c r="A15" s="88"/>
+      <c r="B15" s="91"/>
       <c r="C15" s="33" t="s">
         <v>22</v>
       </c>
@@ -1360,8 +1372,8 @@
       <c r="F15" s="48"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="83"/>
-      <c r="B16" s="84"/>
+      <c r="A16" s="88"/>
+      <c r="B16" s="91"/>
       <c r="C16" s="27" t="s">
         <v>26</v>
       </c>
@@ -1374,8 +1386,8 @@
       <c r="F16" s="59"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="83"/>
-      <c r="B17" s="75"/>
+      <c r="A17" s="88"/>
+      <c r="B17" s="80"/>
       <c r="C17" s="3" t="s">
         <v>27</v>
       </c>
@@ -1388,8 +1400,8 @@
       <c r="F17" s="54"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="83"/>
-      <c r="B18" s="79" t="s">
+      <c r="A18" s="88"/>
+      <c r="B18" s="84" t="s">
         <v>28</v>
       </c>
       <c r="C18" s="20" t="s">
@@ -1404,8 +1416,8 @@
       <c r="F18" s="50"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" s="83"/>
-      <c r="B19" s="82"/>
+      <c r="A19" s="88"/>
+      <c r="B19" s="87"/>
       <c r="C19" s="22" t="s">
         <v>31</v>
       </c>
@@ -1418,8 +1430,8 @@
       <c r="F19" s="51"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="83"/>
-      <c r="B20" s="81"/>
+      <c r="A20" s="88"/>
+      <c r="B20" s="86"/>
       <c r="C20" s="7" t="s">
         <v>30</v>
       </c>
@@ -1432,7 +1444,7 @@
       <c r="F20" s="58"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" s="83"/>
+      <c r="A21" s="88"/>
       <c r="B21" s="4" t="s">
         <v>17</v>
       </c>
@@ -1450,8 +1462,8 @@
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" s="83"/>
-      <c r="B22" s="79" t="s">
+      <c r="A22" s="88"/>
+      <c r="B22" s="84" t="s">
         <v>16</v>
       </c>
       <c r="C22" s="20" t="s">
@@ -1468,8 +1480,8 @@
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23" s="83"/>
-      <c r="B23" s="82"/>
+      <c r="A23" s="88"/>
+      <c r="B23" s="87"/>
       <c r="C23" s="6" t="s">
         <v>34</v>
       </c>
@@ -1492,10 +1504,10 @@
       <c r="F24" s="57"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25" s="76" t="s">
-        <v>1</v>
-      </c>
-      <c r="B25" s="79" t="s">
+      <c r="A25" s="81" t="s">
+        <v>1</v>
+      </c>
+      <c r="B25" s="84" t="s">
         <v>35</v>
       </c>
       <c r="C25" s="20" t="s">
@@ -1510,8 +1522,8 @@
       <c r="F25" s="50"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26" s="77"/>
-      <c r="B26" s="80"/>
+      <c r="A26" s="82"/>
+      <c r="B26" s="85"/>
       <c r="C26" s="22" t="s">
         <v>50</v>
       </c>
@@ -1524,8 +1536,8 @@
       <c r="F26" s="51"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A27" s="83"/>
-      <c r="B27" s="81"/>
+      <c r="A27" s="88"/>
+      <c r="B27" s="86"/>
       <c r="C27" s="7" t="s">
         <v>37</v>
       </c>
@@ -1538,8 +1550,8 @@
       <c r="F27" s="58"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A28" s="83"/>
-      <c r="B28" s="73" t="s">
+      <c r="A28" s="88"/>
+      <c r="B28" s="78" t="s">
         <v>36</v>
       </c>
       <c r="C28" s="31" t="s">
@@ -1554,8 +1566,8 @@
       <c r="F28" s="53"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A29" s="83"/>
-      <c r="B29" s="74"/>
+      <c r="A29" s="88"/>
+      <c r="B29" s="79"/>
       <c r="C29" s="27" t="s">
         <v>102</v>
       </c>
@@ -1568,8 +1580,8 @@
       <c r="F29" s="59"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A30" s="83"/>
-      <c r="B30" s="75"/>
+      <c r="A30" s="88"/>
+      <c r="B30" s="80"/>
       <c r="C30" s="3" t="s">
         <v>103</v>
       </c>
@@ -1582,8 +1594,8 @@
       <c r="F30" s="54"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A31" s="83"/>
-      <c r="B31" s="82" t="s">
+      <c r="A31" s="88"/>
+      <c r="B31" s="87" t="s">
         <v>16</v>
       </c>
       <c r="C31" s="20" t="s">
@@ -1598,8 +1610,8 @@
       <c r="F31" s="50"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A32" s="83"/>
-      <c r="B32" s="82"/>
+      <c r="A32" s="88"/>
+      <c r="B32" s="87"/>
       <c r="C32" s="22" t="s">
         <v>112</v>
       </c>
@@ -1612,8 +1624,8 @@
       <c r="F32" s="51"/>
     </row>
     <row r="33" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A33" s="78"/>
-      <c r="B33" s="82"/>
+      <c r="A33" s="83"/>
+      <c r="B33" s="87"/>
       <c r="C33" s="15" t="s">
         <v>42</v>
       </c>
@@ -1634,10 +1646,10 @@
       <c r="F34" s="57"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A35" s="85" t="s">
+      <c r="A35" s="89" t="s">
         <v>49</v>
       </c>
-      <c r="B35" s="79" t="s">
+      <c r="B35" s="84" t="s">
         <v>35</v>
       </c>
       <c r="C35" s="20" t="s">
@@ -1652,8 +1664,8 @@
       <c r="F35" s="50"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A36" s="86"/>
-      <c r="B36" s="80"/>
+      <c r="A36" s="90"/>
+      <c r="B36" s="85"/>
       <c r="C36" s="22" t="s">
         <v>43</v>
       </c>
@@ -1666,8 +1678,8 @@
       <c r="F36" s="51"/>
     </row>
     <row r="37" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A37" s="83"/>
-      <c r="B37" s="81"/>
+      <c r="A37" s="88"/>
+      <c r="B37" s="86"/>
       <c r="C37" s="17" t="s">
         <v>44</v>
       </c>
@@ -1680,8 +1692,8 @@
       <c r="F37" s="58"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A38" s="83"/>
-      <c r="B38" s="73" t="s">
+      <c r="A38" s="88"/>
+      <c r="B38" s="78" t="s">
         <v>48</v>
       </c>
       <c r="C38" s="38" t="s">
@@ -1696,8 +1708,8 @@
       <c r="F38" s="61"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A39" s="83"/>
-      <c r="B39" s="75"/>
+      <c r="A39" s="88"/>
+      <c r="B39" s="80"/>
       <c r="C39" s="2" t="s">
         <v>61</v>
       </c>
@@ -1710,8 +1722,8 @@
       <c r="F39" s="61"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A40" s="83"/>
-      <c r="B40" s="79" t="s">
+      <c r="A40" s="88"/>
+      <c r="B40" s="84" t="s">
         <v>36</v>
       </c>
       <c r="C40" s="20" t="s">
@@ -1726,8 +1738,8 @@
       <c r="F40" s="50"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A41" s="83"/>
-      <c r="B41" s="80"/>
+      <c r="A41" s="88"/>
+      <c r="B41" s="85"/>
       <c r="C41" s="22" t="s">
         <v>45</v>
       </c>
@@ -1740,8 +1752,8 @@
       <c r="F41" s="51"/>
     </row>
     <row r="42" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A42" s="83"/>
-      <c r="B42" s="81"/>
+      <c r="A42" s="88"/>
+      <c r="B42" s="86"/>
       <c r="C42" s="17" t="s">
         <v>46</v>
       </c>
@@ -1754,7 +1766,7 @@
       <c r="F42" s="58"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A43" s="78"/>
+      <c r="A43" s="83"/>
       <c r="B43" s="39" t="s">
         <v>16</v>
       </c>
@@ -1778,10 +1790,10 @@
       <c r="F44" s="57"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A45" s="76" t="s">
+      <c r="A45" s="81" t="s">
         <v>4</v>
       </c>
-      <c r="B45" s="79" t="s">
+      <c r="B45" s="84" t="s">
         <v>35</v>
       </c>
       <c r="C45" s="20" t="s">
@@ -1796,8 +1808,8 @@
       <c r="F45" s="50"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A46" s="83"/>
-      <c r="B46" s="80"/>
+      <c r="A46" s="88"/>
+      <c r="B46" s="85"/>
       <c r="C46" s="22" t="s">
         <v>52</v>
       </c>
@@ -1810,8 +1822,8 @@
       <c r="F46" s="51"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A47" s="83"/>
-      <c r="B47" s="80"/>
+      <c r="A47" s="88"/>
+      <c r="B47" s="85"/>
       <c r="C47" s="22" t="s">
         <v>53</v>
       </c>
@@ -1824,8 +1836,8 @@
       <c r="F47" s="51"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A48" s="83"/>
-      <c r="B48" s="81"/>
+      <c r="A48" s="88"/>
+      <c r="B48" s="86"/>
       <c r="C48" s="7" t="s">
         <v>54</v>
       </c>
@@ -1838,8 +1850,8 @@
       <c r="F48" s="58"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A49" s="83"/>
-      <c r="B49" s="74" t="s">
+      <c r="A49" s="88"/>
+      <c r="B49" s="79" t="s">
         <v>36</v>
       </c>
       <c r="C49" s="27" t="s">
@@ -1854,8 +1866,8 @@
       <c r="F49" s="59"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A50" s="83"/>
-      <c r="B50" s="74"/>
+      <c r="A50" s="88"/>
+      <c r="B50" s="79"/>
       <c r="C50" s="33" t="s">
         <v>55</v>
       </c>
@@ -1868,8 +1880,8 @@
       <c r="F50" s="48"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A51" s="83"/>
-      <c r="B51" s="74"/>
+      <c r="A51" s="88"/>
+      <c r="B51" s="79"/>
       <c r="C51" s="33" t="s">
         <v>56</v>
       </c>
@@ -1882,8 +1894,8 @@
       <c r="F51" s="48"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A52" s="83"/>
-      <c r="B52" s="75"/>
+      <c r="A52" s="88"/>
+      <c r="B52" s="80"/>
       <c r="C52" s="3" t="s">
         <v>57</v>
       </c>
@@ -1896,8 +1908,8 @@
       <c r="F52" s="54"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A53" s="83"/>
-      <c r="B53" s="82" t="s">
+      <c r="A53" s="88"/>
+      <c r="B53" s="87" t="s">
         <v>16</v>
       </c>
       <c r="C53" s="24" t="s">
@@ -1912,8 +1924,8 @@
       <c r="F53" s="52"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A54" s="78"/>
-      <c r="B54" s="82"/>
+      <c r="A54" s="83"/>
+      <c r="B54" s="87"/>
       <c r="C54" s="16" t="s">
         <v>59</v>
       </c>
@@ -1934,10 +1946,10 @@
       <c r="F55" s="57"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A56" s="76" t="s">
+      <c r="A56" s="81" t="s">
         <v>3</v>
       </c>
-      <c r="B56" s="79" t="s">
+      <c r="B56" s="84" t="s">
         <v>35</v>
       </c>
       <c r="C56" s="20" t="s">
@@ -1952,8 +1964,8 @@
       <c r="F56" s="50"/>
     </row>
     <row r="57" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A57" s="83"/>
-      <c r="B57" s="80"/>
+      <c r="A57" s="88"/>
+      <c r="B57" s="85"/>
       <c r="C57" s="43" t="s">
         <v>62</v>
       </c>
@@ -1968,8 +1980,8 @@
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A58" s="83"/>
-      <c r="B58" s="80"/>
+      <c r="A58" s="88"/>
+      <c r="B58" s="85"/>
       <c r="C58" s="22" t="s">
         <v>63</v>
       </c>
@@ -1982,8 +1994,8 @@
       <c r="F58" s="51"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A59" s="83"/>
-      <c r="B59" s="81"/>
+      <c r="A59" s="88"/>
+      <c r="B59" s="86"/>
       <c r="C59" s="7" t="s">
         <v>64</v>
       </c>
@@ -1996,8 +2008,8 @@
       <c r="F59" s="58"/>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A60" s="83"/>
-      <c r="B60" s="73" t="s">
+      <c r="A60" s="88"/>
+      <c r="B60" s="78" t="s">
         <v>36</v>
       </c>
       <c r="C60" s="31" t="s">
@@ -2012,8 +2024,8 @@
       <c r="F60" s="53"/>
     </row>
     <row r="61" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A61" s="83"/>
-      <c r="B61" s="74"/>
+      <c r="A61" s="88"/>
+      <c r="B61" s="79"/>
       <c r="C61" s="44" t="s">
         <v>65</v>
       </c>
@@ -2028,8 +2040,8 @@
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A62" s="83"/>
-      <c r="B62" s="74"/>
+      <c r="A62" s="88"/>
+      <c r="B62" s="79"/>
       <c r="C62" s="33" t="s">
         <v>66</v>
       </c>
@@ -2042,8 +2054,8 @@
       <c r="F62" s="48"/>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A63" s="83"/>
-      <c r="B63" s="75"/>
+      <c r="A63" s="88"/>
+      <c r="B63" s="80"/>
       <c r="C63" s="3" t="s">
         <v>67</v>
       </c>
@@ -2056,8 +2068,8 @@
       <c r="F63" s="54"/>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A64" s="83"/>
-      <c r="B64" s="79" t="s">
+      <c r="A64" s="88"/>
+      <c r="B64" s="84" t="s">
         <v>74</v>
       </c>
       <c r="C64" s="20" t="s">
@@ -2072,8 +2084,8 @@
       <c r="F64" s="50"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A65" s="83"/>
-      <c r="B65" s="80"/>
+      <c r="A65" s="88"/>
+      <c r="B65" s="85"/>
       <c r="C65" s="22" t="s">
         <v>69</v>
       </c>
@@ -2086,8 +2098,8 @@
       <c r="F65" s="51"/>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A66" s="83"/>
-      <c r="B66" s="81"/>
+      <c r="A66" s="88"/>
+      <c r="B66" s="86"/>
       <c r="C66" s="7" t="s">
         <v>70</v>
       </c>
@@ -2100,8 +2112,8 @@
       <c r="F66" s="58"/>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A67" s="83"/>
-      <c r="B67" s="73" t="s">
+      <c r="A67" s="88"/>
+      <c r="B67" s="78" t="s">
         <v>96</v>
       </c>
       <c r="C67" s="31" t="s">
@@ -2116,8 +2128,8 @@
       <c r="F67" s="53"/>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A68" s="83"/>
-      <c r="B68" s="84"/>
+      <c r="A68" s="88"/>
+      <c r="B68" s="91"/>
       <c r="C68" s="33" t="s">
         <v>72</v>
       </c>
@@ -2130,8 +2142,8 @@
       <c r="F68" s="48"/>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A69" s="83"/>
-      <c r="B69" s="74"/>
+      <c r="A69" s="88"/>
+      <c r="B69" s="79"/>
       <c r="C69" s="40" t="s">
         <v>73</v>
       </c>
@@ -2144,8 +2156,8 @@
       <c r="F69" s="61"/>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A70" s="83"/>
-      <c r="B70" s="79" t="s">
+      <c r="A70" s="88"/>
+      <c r="B70" s="84" t="s">
         <v>16</v>
       </c>
       <c r="C70" s="20" t="s">
@@ -2160,8 +2172,8 @@
       <c r="F70" s="50"/>
     </row>
     <row r="71" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A71" s="83"/>
-      <c r="B71" s="80"/>
+      <c r="A71" s="88"/>
+      <c r="B71" s="85"/>
       <c r="C71" s="43" t="s">
         <v>76</v>
       </c>
@@ -2174,8 +2186,8 @@
       <c r="F71" s="51"/>
     </row>
     <row r="72" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A72" s="78"/>
-      <c r="B72" s="81"/>
+      <c r="A72" s="83"/>
+      <c r="B72" s="86"/>
       <c r="C72" s="17" t="s">
         <v>77</v>
       </c>
@@ -2196,10 +2208,10 @@
       <c r="F73" s="57"/>
     </row>
     <row r="74" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="76" t="s">
+      <c r="A74" s="81" t="s">
         <v>2</v>
       </c>
-      <c r="B74" s="79" t="s">
+      <c r="B74" s="84" t="s">
         <v>35</v>
       </c>
       <c r="C74" s="20" t="s">
@@ -2216,8 +2228,8 @@
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A75" s="77"/>
-      <c r="B75" s="80"/>
+      <c r="A75" s="82"/>
+      <c r="B75" s="85"/>
       <c r="C75" s="22" t="s">
         <v>79</v>
       </c>
@@ -2232,8 +2244,8 @@
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A76" s="77"/>
-      <c r="B76" s="80"/>
+      <c r="A76" s="82"/>
+      <c r="B76" s="85"/>
       <c r="C76" s="22" t="s">
         <v>80</v>
       </c>
@@ -2246,8 +2258,8 @@
       <c r="F76" s="51"/>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A77" s="77"/>
-      <c r="B77" s="80"/>
+      <c r="A77" s="82"/>
+      <c r="B77" s="85"/>
       <c r="C77" s="22" t="s">
         <v>81</v>
       </c>
@@ -2260,8 +2272,8 @@
       <c r="F77" s="51"/>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A78" s="77"/>
-      <c r="B78" s="80"/>
+      <c r="A78" s="82"/>
+      <c r="B78" s="85"/>
       <c r="C78" s="22" t="s">
         <v>83</v>
       </c>
@@ -2276,8 +2288,8 @@
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A79" s="77"/>
-      <c r="B79" s="80"/>
+      <c r="A79" s="82"/>
+      <c r="B79" s="85"/>
       <c r="C79" s="22" t="s">
         <v>84</v>
       </c>
@@ -2292,8 +2304,8 @@
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A80" s="77"/>
-      <c r="B80" s="80"/>
+      <c r="A80" s="82"/>
+      <c r="B80" s="85"/>
       <c r="C80" s="22" t="s">
         <v>85</v>
       </c>
@@ -2306,8 +2318,8 @@
       <c r="F80" s="51"/>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A81" s="77"/>
-      <c r="B81" s="81"/>
+      <c r="A81" s="82"/>
+      <c r="B81" s="86"/>
       <c r="C81" s="7" t="s">
         <v>82</v>
       </c>
@@ -2320,8 +2332,8 @@
       <c r="F81" s="58"/>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A82" s="77"/>
-      <c r="B82" s="73" t="s">
+      <c r="A82" s="82"/>
+      <c r="B82" s="78" t="s">
         <v>36</v>
       </c>
       <c r="C82" s="31" t="s">
@@ -2338,8 +2350,8 @@
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A83" s="77"/>
-      <c r="B83" s="84"/>
+      <c r="A83" s="82"/>
+      <c r="B83" s="91"/>
       <c r="C83" s="27" t="s">
         <v>87</v>
       </c>
@@ -2354,8 +2366,8 @@
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A84" s="77"/>
-      <c r="B84" s="84"/>
+      <c r="A84" s="82"/>
+      <c r="B84" s="91"/>
       <c r="C84" s="27" t="s">
         <v>88</v>
       </c>
@@ -2368,8 +2380,8 @@
       <c r="F84" s="59"/>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A85" s="77"/>
-      <c r="B85" s="84"/>
+      <c r="A85" s="82"/>
+      <c r="B85" s="91"/>
       <c r="C85" s="27" t="s">
         <v>89</v>
       </c>
@@ -2382,8 +2394,8 @@
       <c r="F85" s="59"/>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A86" s="77"/>
-      <c r="B86" s="84"/>
+      <c r="A86" s="82"/>
+      <c r="B86" s="91"/>
       <c r="C86" s="27" t="s">
         <v>90</v>
       </c>
@@ -2398,8 +2410,8 @@
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A87" s="77"/>
-      <c r="B87" s="84"/>
+      <c r="A87" s="82"/>
+      <c r="B87" s="91"/>
       <c r="C87" s="27" t="s">
         <v>91</v>
       </c>
@@ -2414,8 +2426,8 @@
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A88" s="77"/>
-      <c r="B88" s="84"/>
+      <c r="A88" s="82"/>
+      <c r="B88" s="91"/>
       <c r="C88" s="27" t="s">
         <v>92</v>
       </c>
@@ -2428,8 +2440,8 @@
       <c r="F88" s="59"/>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A89" s="77"/>
-      <c r="B89" s="75"/>
+      <c r="A89" s="82"/>
+      <c r="B89" s="80"/>
       <c r="C89" s="3" t="s">
         <v>93</v>
       </c>
@@ -2442,8 +2454,8 @@
       <c r="F89" s="54"/>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A90" s="77"/>
-      <c r="B90" s="79" t="s">
+      <c r="A90" s="82"/>
+      <c r="B90" s="84" t="s">
         <v>16</v>
       </c>
       <c r="C90" s="20" t="s">
@@ -2458,8 +2470,8 @@
       <c r="F90" s="50"/>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A91" s="77"/>
-      <c r="B91" s="81"/>
+      <c r="A91" s="82"/>
+      <c r="B91" s="86"/>
       <c r="C91" s="6" t="s">
         <v>95</v>
       </c>
@@ -2472,8 +2484,8 @@
       <c r="F91" s="60"/>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A92" s="77"/>
-      <c r="B92" s="73" t="s">
+      <c r="A92" s="82"/>
+      <c r="B92" s="78" t="s">
         <v>107</v>
       </c>
       <c r="C92" s="31" t="s">
@@ -2488,8 +2500,8 @@
       <c r="F92" s="53"/>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A93" s="77"/>
-      <c r="B93" s="74"/>
+      <c r="A93" s="82"/>
+      <c r="B93" s="79"/>
       <c r="C93" s="33" t="s">
         <v>113</v>
       </c>
@@ -2502,8 +2514,8 @@
       <c r="F93" s="48"/>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A94" s="77"/>
-      <c r="B94" s="74"/>
+      <c r="A94" s="82"/>
+      <c r="B94" s="79"/>
       <c r="C94" s="33" t="s">
         <v>109</v>
       </c>
@@ -2516,8 +2528,8 @@
       <c r="F94" s="48"/>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A95" s="78"/>
-      <c r="B95" s="75"/>
+      <c r="A95" s="83"/>
+      <c r="B95" s="80"/>
       <c r="C95" s="40" t="s">
         <v>114</v>
       </c>
@@ -2665,10 +2677,10 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="76" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="80" t="s">
+      <c r="A2" s="81" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="85" t="s">
         <v>14</v>
       </c>
       <c r="C2" s="20" t="s">
@@ -2683,8 +2695,8 @@
       <c r="F2" s="50"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="83"/>
-      <c r="B3" s="80"/>
+      <c r="A3" s="88"/>
+      <c r="B3" s="85"/>
       <c r="C3" s="22" t="s">
         <v>8</v>
       </c>
@@ -2703,8 +2715,8 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="83"/>
-      <c r="B4" s="80"/>
+      <c r="A4" s="88"/>
+      <c r="B4" s="85"/>
       <c r="C4" s="22" t="s">
         <v>9</v>
       </c>
@@ -2723,8 +2735,8 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="83"/>
-      <c r="B5" s="80"/>
+      <c r="A5" s="88"/>
+      <c r="B5" s="85"/>
       <c r="C5" s="22" t="s">
         <v>10</v>
       </c>
@@ -2737,8 +2749,8 @@
       <c r="F5" s="51"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="83"/>
-      <c r="B6" s="80"/>
+      <c r="A6" s="88"/>
+      <c r="B6" s="85"/>
       <c r="C6" s="24" t="s">
         <v>11</v>
       </c>
@@ -2751,8 +2763,8 @@
       <c r="F6" s="52"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="83"/>
-      <c r="B7" s="80"/>
+      <c r="A7" s="88"/>
+      <c r="B7" s="85"/>
       <c r="C7" s="24" t="s">
         <v>12</v>
       </c>
@@ -2765,8 +2777,8 @@
       <c r="F7" s="52"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="83"/>
-      <c r="B8" s="73" t="s">
+      <c r="A8" s="88"/>
+      <c r="B8" s="78" t="s">
         <v>15</v>
       </c>
       <c r="C8" s="31" t="s">
@@ -2781,8 +2793,8 @@
       <c r="F8" s="53"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="83"/>
-      <c r="B9" s="84"/>
+      <c r="A9" s="88"/>
+      <c r="B9" s="91"/>
       <c r="C9" s="33" t="s">
         <v>13</v>
       </c>
@@ -2795,8 +2807,8 @@
       <c r="F9" s="48"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="83"/>
-      <c r="B10" s="84"/>
+      <c r="A10" s="88"/>
+      <c r="B10" s="91"/>
       <c r="C10" s="33" t="s">
         <v>19</v>
       </c>
@@ -2811,8 +2823,8 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="83"/>
-      <c r="B11" s="84"/>
+      <c r="A11" s="88"/>
+      <c r="B11" s="91"/>
       <c r="C11" s="33" t="s">
         <v>20</v>
       </c>
@@ -2825,8 +2837,8 @@
       <c r="F11" s="48"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="83"/>
-      <c r="B12" s="84"/>
+      <c r="A12" s="88"/>
+      <c r="B12" s="91"/>
       <c r="C12" s="33" t="s">
         <v>21</v>
       </c>
@@ -2839,8 +2851,8 @@
       <c r="F12" s="48"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="83"/>
-      <c r="B13" s="84"/>
+      <c r="A13" s="88"/>
+      <c r="B13" s="91"/>
       <c r="C13" s="33" t="s">
         <v>23</v>
       </c>
@@ -2853,8 +2865,8 @@
       <c r="F13" s="48"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="83"/>
-      <c r="B14" s="84"/>
+      <c r="A14" s="88"/>
+      <c r="B14" s="91"/>
       <c r="C14" s="33" t="s">
         <v>22</v>
       </c>
@@ -2867,8 +2879,8 @@
       <c r="F14" s="48"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="83"/>
-      <c r="B15" s="75"/>
+      <c r="A15" s="88"/>
+      <c r="B15" s="80"/>
       <c r="C15" s="3" t="s">
         <v>100</v>
       </c>
@@ -2881,7 +2893,7 @@
       <c r="F15" s="54"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="83"/>
+      <c r="A16" s="88"/>
       <c r="B16" s="41" t="s">
         <v>17</v>
       </c>
@@ -2897,8 +2909,8 @@
       <c r="F16" s="55"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="83"/>
-      <c r="B17" s="73" t="s">
+      <c r="A17" s="88"/>
+      <c r="B17" s="78" t="s">
         <v>16</v>
       </c>
       <c r="C17" s="31" t="s">
@@ -2913,8 +2925,8 @@
       <c r="F17" s="53"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="83"/>
-      <c r="B18" s="84"/>
+      <c r="A18" s="88"/>
+      <c r="B18" s="91"/>
       <c r="C18" s="40" t="s">
         <v>34</v>
       </c>
@@ -2937,10 +2949,10 @@
       <c r="F19" s="57"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="76" t="s">
-        <v>1</v>
-      </c>
-      <c r="B20" s="79" t="s">
+      <c r="A20" s="81" t="s">
+        <v>1</v>
+      </c>
+      <c r="B20" s="84" t="s">
         <v>35</v>
       </c>
       <c r="C20" s="20" t="s">
@@ -2955,8 +2967,8 @@
       <c r="F20" s="50"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" s="77"/>
-      <c r="B21" s="80"/>
+      <c r="A21" s="82"/>
+      <c r="B21" s="85"/>
       <c r="C21" s="22" t="s">
         <v>50</v>
       </c>
@@ -2971,8 +2983,8 @@
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" s="83"/>
-      <c r="B22" s="81"/>
+      <c r="A22" s="88"/>
+      <c r="B22" s="86"/>
       <c r="C22" s="7" t="s">
         <v>37</v>
       </c>
@@ -2985,8 +2997,8 @@
       <c r="F22" s="58"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23" s="83"/>
-      <c r="B23" s="73" t="s">
+      <c r="A23" s="88"/>
+      <c r="B23" s="78" t="s">
         <v>36</v>
       </c>
       <c r="C23" s="31" t="s">
@@ -3003,8 +3015,8 @@
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24" s="83"/>
-      <c r="B24" s="74"/>
+      <c r="A24" s="88"/>
+      <c r="B24" s="79"/>
       <c r="C24" s="27" t="s">
         <v>102</v>
       </c>
@@ -3017,8 +3029,8 @@
       <c r="F24" s="59"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25" s="83"/>
-      <c r="B25" s="75"/>
+      <c r="A25" s="88"/>
+      <c r="B25" s="80"/>
       <c r="C25" s="3" t="s">
         <v>103</v>
       </c>
@@ -3031,8 +3043,8 @@
       <c r="F25" s="54"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26" s="83"/>
-      <c r="B26" s="82" t="s">
+      <c r="A26" s="88"/>
+      <c r="B26" s="87" t="s">
         <v>16</v>
       </c>
       <c r="C26" s="20" t="s">
@@ -3047,8 +3059,8 @@
       <c r="F26" s="50"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A27" s="83"/>
-      <c r="B27" s="82"/>
+      <c r="A27" s="88"/>
+      <c r="B27" s="87"/>
       <c r="C27" s="22" t="s">
         <v>112</v>
       </c>
@@ -3061,8 +3073,8 @@
       <c r="F27" s="51"/>
     </row>
     <row r="28" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A28" s="78"/>
-      <c r="B28" s="82"/>
+      <c r="A28" s="83"/>
+      <c r="B28" s="87"/>
       <c r="C28" s="15" t="s">
         <v>42</v>
       </c>
@@ -3083,10 +3095,10 @@
       <c r="F29" s="57"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A30" s="85" t="s">
+      <c r="A30" s="89" t="s">
         <v>49</v>
       </c>
-      <c r="B30" s="79" t="s">
+      <c r="B30" s="84" t="s">
         <v>35</v>
       </c>
       <c r="C30" s="20" t="s">
@@ -3101,8 +3113,8 @@
       <c r="F30" s="50"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A31" s="86"/>
-      <c r="B31" s="80"/>
+      <c r="A31" s="90"/>
+      <c r="B31" s="85"/>
       <c r="C31" s="22" t="s">
         <v>43</v>
       </c>
@@ -3115,8 +3127,8 @@
       <c r="F31" s="51"/>
     </row>
     <row r="32" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A32" s="83"/>
-      <c r="B32" s="81"/>
+      <c r="A32" s="88"/>
+      <c r="B32" s="86"/>
       <c r="C32" s="17" t="s">
         <v>44</v>
       </c>
@@ -3129,8 +3141,8 @@
       <c r="F32" s="58"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A33" s="83"/>
-      <c r="B33" s="73" t="s">
+      <c r="A33" s="88"/>
+      <c r="B33" s="78" t="s">
         <v>48</v>
       </c>
       <c r="C33" s="38" t="s">
@@ -3145,8 +3157,8 @@
       <c r="F33" s="61"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A34" s="83"/>
-      <c r="B34" s="75"/>
+      <c r="A34" s="88"/>
+      <c r="B34" s="80"/>
       <c r="C34" s="2" t="s">
         <v>61</v>
       </c>
@@ -3159,8 +3171,8 @@
       <c r="F34" s="61"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A35" s="83"/>
-      <c r="B35" s="79" t="s">
+      <c r="A35" s="88"/>
+      <c r="B35" s="84" t="s">
         <v>36</v>
       </c>
       <c r="C35" s="20" t="s">
@@ -3175,8 +3187,8 @@
       <c r="F35" s="50"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A36" s="83"/>
-      <c r="B36" s="80"/>
+      <c r="A36" s="88"/>
+      <c r="B36" s="85"/>
       <c r="C36" s="22" t="s">
         <v>45</v>
       </c>
@@ -3189,8 +3201,8 @@
       <c r="F36" s="51"/>
     </row>
     <row r="37" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A37" s="83"/>
-      <c r="B37" s="81"/>
+      <c r="A37" s="88"/>
+      <c r="B37" s="86"/>
       <c r="C37" s="17" t="s">
         <v>46</v>
       </c>
@@ -3203,7 +3215,7 @@
       <c r="F37" s="58"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A38" s="78"/>
+      <c r="A38" s="83"/>
       <c r="B38" s="39" t="s">
         <v>16</v>
       </c>
@@ -3227,10 +3239,10 @@
       <c r="F39" s="57"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A40" s="76" t="s">
+      <c r="A40" s="81" t="s">
         <v>4</v>
       </c>
-      <c r="B40" s="79" t="s">
+      <c r="B40" s="84" t="s">
         <v>35</v>
       </c>
       <c r="C40" s="20" t="s">
@@ -3245,8 +3257,8 @@
       <c r="F40" s="50"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A41" s="83"/>
-      <c r="B41" s="80"/>
+      <c r="A41" s="88"/>
+      <c r="B41" s="85"/>
       <c r="C41" s="22" t="s">
         <v>52</v>
       </c>
@@ -3259,8 +3271,8 @@
       <c r="F41" s="51"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A42" s="83"/>
-      <c r="B42" s="80"/>
+      <c r="A42" s="88"/>
+      <c r="B42" s="85"/>
       <c r="C42" s="22" t="s">
         <v>53</v>
       </c>
@@ -3273,8 +3285,8 @@
       <c r="F42" s="51"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A43" s="83"/>
-      <c r="B43" s="81"/>
+      <c r="A43" s="88"/>
+      <c r="B43" s="86"/>
       <c r="C43" s="7" t="s">
         <v>54</v>
       </c>
@@ -3287,8 +3299,8 @@
       <c r="F43" s="58"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A44" s="83"/>
-      <c r="B44" s="74" t="s">
+      <c r="A44" s="88"/>
+      <c r="B44" s="79" t="s">
         <v>36</v>
       </c>
       <c r="C44" s="27" t="s">
@@ -3303,8 +3315,8 @@
       <c r="F44" s="59"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A45" s="83"/>
-      <c r="B45" s="74"/>
+      <c r="A45" s="88"/>
+      <c r="B45" s="79"/>
       <c r="C45" s="33" t="s">
         <v>55</v>
       </c>
@@ -3317,8 +3329,8 @@
       <c r="F45" s="48"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A46" s="83"/>
-      <c r="B46" s="74"/>
+      <c r="A46" s="88"/>
+      <c r="B46" s="79"/>
       <c r="C46" s="33" t="s">
         <v>56</v>
       </c>
@@ -3331,8 +3343,8 @@
       <c r="F46" s="48"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A47" s="83"/>
-      <c r="B47" s="75"/>
+      <c r="A47" s="88"/>
+      <c r="B47" s="80"/>
       <c r="C47" s="3" t="s">
         <v>57</v>
       </c>
@@ -3345,8 +3357,8 @@
       <c r="F47" s="54"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A48" s="83"/>
-      <c r="B48" s="82" t="s">
+      <c r="A48" s="88"/>
+      <c r="B48" s="87" t="s">
         <v>16</v>
       </c>
       <c r="C48" s="24" t="s">
@@ -3361,8 +3373,8 @@
       <c r="F48" s="52"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A49" s="78"/>
-      <c r="B49" s="82"/>
+      <c r="A49" s="83"/>
+      <c r="B49" s="87"/>
       <c r="C49" s="16" t="s">
         <v>59</v>
       </c>
@@ -3383,10 +3395,10 @@
       <c r="F50" s="57"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A51" s="76" t="s">
+      <c r="A51" s="81" t="s">
         <v>3</v>
       </c>
-      <c r="B51" s="79" t="s">
+      <c r="B51" s="84" t="s">
         <v>35</v>
       </c>
       <c r="C51" s="20" t="s">
@@ -3401,8 +3413,8 @@
       <c r="F51" s="50"/>
     </row>
     <row r="52" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A52" s="83"/>
-      <c r="B52" s="80"/>
+      <c r="A52" s="88"/>
+      <c r="B52" s="85"/>
       <c r="C52" s="43" t="s">
         <v>62</v>
       </c>
@@ -3417,8 +3429,8 @@
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A53" s="83"/>
-      <c r="B53" s="80"/>
+      <c r="A53" s="88"/>
+      <c r="B53" s="85"/>
       <c r="C53" s="22" t="s">
         <v>63</v>
       </c>
@@ -3431,8 +3443,8 @@
       <c r="F53" s="51"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A54" s="83"/>
-      <c r="B54" s="81"/>
+      <c r="A54" s="88"/>
+      <c r="B54" s="86"/>
       <c r="C54" s="7" t="s">
         <v>64</v>
       </c>
@@ -3445,8 +3457,8 @@
       <c r="F54" s="58"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A55" s="83"/>
-      <c r="B55" s="73" t="s">
+      <c r="A55" s="88"/>
+      <c r="B55" s="78" t="s">
         <v>36</v>
       </c>
       <c r="C55" s="31" t="s">
@@ -3461,8 +3473,8 @@
       <c r="F55" s="53"/>
     </row>
     <row r="56" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A56" s="83"/>
-      <c r="B56" s="74"/>
+      <c r="A56" s="88"/>
+      <c r="B56" s="79"/>
       <c r="C56" s="44" t="s">
         <v>65</v>
       </c>
@@ -3477,8 +3489,8 @@
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A57" s="83"/>
-      <c r="B57" s="74"/>
+      <c r="A57" s="88"/>
+      <c r="B57" s="79"/>
       <c r="C57" s="33" t="s">
         <v>66</v>
       </c>
@@ -3491,8 +3503,8 @@
       <c r="F57" s="48"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A58" s="83"/>
-      <c r="B58" s="75"/>
+      <c r="A58" s="88"/>
+      <c r="B58" s="80"/>
       <c r="C58" s="3" t="s">
         <v>67</v>
       </c>
@@ -3505,8 +3517,8 @@
       <c r="F58" s="54"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A59" s="83"/>
-      <c r="B59" s="79" t="s">
+      <c r="A59" s="88"/>
+      <c r="B59" s="84" t="s">
         <v>74</v>
       </c>
       <c r="C59" s="20" t="s">
@@ -3521,8 +3533,8 @@
       <c r="F59" s="50"/>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A60" s="83"/>
-      <c r="B60" s="80"/>
+      <c r="A60" s="88"/>
+      <c r="B60" s="85"/>
       <c r="C60" s="22" t="s">
         <v>69</v>
       </c>
@@ -3535,8 +3547,8 @@
       <c r="F60" s="51"/>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A61" s="83"/>
-      <c r="B61" s="81"/>
+      <c r="A61" s="88"/>
+      <c r="B61" s="86"/>
       <c r="C61" s="7" t="s">
         <v>70</v>
       </c>
@@ -3549,7 +3561,7 @@
       <c r="F61" s="58"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A62" s="83"/>
+      <c r="A62" s="88"/>
       <c r="B62" s="45" t="s">
         <v>16</v>
       </c>
@@ -3575,10 +3587,10 @@
       <c r="F63" s="57"/>
     </row>
     <row r="64" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="76" t="s">
+      <c r="A64" s="81" t="s">
         <v>2</v>
       </c>
-      <c r="B64" s="79" t="s">
+      <c r="B64" s="84" t="s">
         <v>35</v>
       </c>
       <c r="C64" s="20" t="s">
@@ -3595,8 +3607,8 @@
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A65" s="77"/>
-      <c r="B65" s="80"/>
+      <c r="A65" s="82"/>
+      <c r="B65" s="85"/>
       <c r="C65" s="22" t="s">
         <v>79</v>
       </c>
@@ -3611,8 +3623,8 @@
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A66" s="77"/>
-      <c r="B66" s="80"/>
+      <c r="A66" s="82"/>
+      <c r="B66" s="85"/>
       <c r="C66" s="24" t="s">
         <v>80</v>
       </c>
@@ -3625,8 +3637,8 @@
       <c r="F66" s="52"/>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A67" s="77"/>
-      <c r="B67" s="80"/>
+      <c r="A67" s="82"/>
+      <c r="B67" s="85"/>
       <c r="C67" s="24" t="s">
         <v>81</v>
       </c>
@@ -3639,8 +3651,8 @@
       <c r="F67" s="52"/>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A68" s="77"/>
-      <c r="B68" s="80"/>
+      <c r="A68" s="82"/>
+      <c r="B68" s="85"/>
       <c r="C68" s="24" t="s">
         <v>83</v>
       </c>
@@ -3655,8 +3667,8 @@
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A69" s="77"/>
-      <c r="B69" s="80"/>
+      <c r="A69" s="82"/>
+      <c r="B69" s="85"/>
       <c r="C69" s="24" t="s">
         <v>84</v>
       </c>
@@ -3671,8 +3683,8 @@
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A70" s="77"/>
-      <c r="B70" s="80"/>
+      <c r="A70" s="82"/>
+      <c r="B70" s="85"/>
       <c r="C70" s="24" t="s">
         <v>85</v>
       </c>
@@ -3685,8 +3697,8 @@
       <c r="F70" s="52"/>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A71" s="77"/>
-      <c r="B71" s="81"/>
+      <c r="A71" s="82"/>
+      <c r="B71" s="86"/>
       <c r="C71" s="7" t="s">
         <v>82</v>
       </c>
@@ -3699,8 +3711,8 @@
       <c r="F71" s="58"/>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A72" s="77"/>
-      <c r="B72" s="73" t="s">
+      <c r="A72" s="82"/>
+      <c r="B72" s="78" t="s">
         <v>36</v>
       </c>
       <c r="C72" s="31" t="s">
@@ -3717,8 +3729,8 @@
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A73" s="77"/>
-      <c r="B73" s="84"/>
+      <c r="A73" s="82"/>
+      <c r="B73" s="91"/>
       <c r="C73" s="33" t="s">
         <v>87</v>
       </c>
@@ -3733,8 +3745,8 @@
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A74" s="77"/>
-      <c r="B74" s="84"/>
+      <c r="A74" s="82"/>
+      <c r="B74" s="91"/>
       <c r="C74" s="27" t="s">
         <v>88</v>
       </c>
@@ -3747,8 +3759,8 @@
       <c r="F74" s="59"/>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A75" s="77"/>
-      <c r="B75" s="84"/>
+      <c r="A75" s="82"/>
+      <c r="B75" s="91"/>
       <c r="C75" s="33" t="s">
         <v>89</v>
       </c>
@@ -3761,8 +3773,8 @@
       <c r="F75" s="48"/>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A76" s="77"/>
-      <c r="B76" s="84"/>
+      <c r="A76" s="82"/>
+      <c r="B76" s="91"/>
       <c r="C76" s="33" t="s">
         <v>90</v>
       </c>
@@ -3777,8 +3789,8 @@
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A77" s="77"/>
-      <c r="B77" s="84"/>
+      <c r="A77" s="82"/>
+      <c r="B77" s="91"/>
       <c r="C77" s="33" t="s">
         <v>91</v>
       </c>
@@ -3793,8 +3805,8 @@
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A78" s="77"/>
-      <c r="B78" s="84"/>
+      <c r="A78" s="82"/>
+      <c r="B78" s="91"/>
       <c r="C78" s="33" t="s">
         <v>92</v>
       </c>
@@ -3807,8 +3819,8 @@
       <c r="F78" s="48"/>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A79" s="77"/>
-      <c r="B79" s="75"/>
+      <c r="A79" s="82"/>
+      <c r="B79" s="80"/>
       <c r="C79" s="3" t="s">
         <v>93</v>
       </c>
@@ -3821,8 +3833,8 @@
       <c r="F79" s="54"/>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A80" s="77"/>
-      <c r="B80" s="79" t="s">
+      <c r="A80" s="82"/>
+      <c r="B80" s="84" t="s">
         <v>16</v>
       </c>
       <c r="C80" s="20" t="s">
@@ -3837,8 +3849,8 @@
       <c r="F80" s="50"/>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A81" s="77"/>
-      <c r="B81" s="81"/>
+      <c r="A81" s="82"/>
+      <c r="B81" s="86"/>
       <c r="C81" s="6" t="s">
         <v>95</v>
       </c>
@@ -3851,8 +3863,8 @@
       <c r="F81" s="60"/>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A82" s="77"/>
-      <c r="B82" s="73" t="s">
+      <c r="A82" s="82"/>
+      <c r="B82" s="78" t="s">
         <v>107</v>
       </c>
       <c r="C82" s="31" t="s">
@@ -3867,8 +3879,8 @@
       <c r="F82" s="53"/>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A83" s="78"/>
-      <c r="B83" s="75"/>
+      <c r="A83" s="83"/>
+      <c r="B83" s="80"/>
       <c r="C83" s="40" t="s">
         <v>109</v>
       </c>
@@ -3979,8 +3991,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E11F7609-0A7A-46D7-A44A-76050598E181}">
   <dimension ref="A1:J98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3997,10 +4009,10 @@
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
       <c r="B1" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>40</v>
+        <v>127</v>
       </c>
       <c r="D1" s="8"/>
       <c r="E1" s="8"/>
@@ -4010,10 +4022,10 @@
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="7"/>
       <c r="B2" s="9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
@@ -4024,7 +4036,7 @@
     </row>
     <row r="3" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="47" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B3" s="35" t="s">
         <v>6</v>
@@ -4049,10 +4061,10 @@
       <c r="J3" s="67"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="76" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="80" t="s">
+      <c r="A4" s="81" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="85" t="s">
         <v>14</v>
       </c>
       <c r="C4" s="20" t="s">
@@ -4073,8 +4085,8 @@
       <c r="J4" s="67"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="83"/>
-      <c r="B5" s="80"/>
+      <c r="A5" s="88"/>
+      <c r="B5" s="85"/>
       <c r="C5" s="22" t="s">
         <v>8</v>
       </c>
@@ -4093,8 +4105,8 @@
       <c r="J5" s="67"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" s="83"/>
-      <c r="B6" s="80"/>
+      <c r="A6" s="88"/>
+      <c r="B6" s="85"/>
       <c r="C6" s="22" t="s">
         <v>9</v>
       </c>
@@ -4113,8 +4125,8 @@
       <c r="J6" s="67"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" s="83"/>
-      <c r="B7" s="80"/>
+      <c r="A7" s="88"/>
+      <c r="B7" s="85"/>
       <c r="C7" s="22" t="s">
         <v>10</v>
       </c>
@@ -4133,8 +4145,8 @@
       <c r="J7" s="67"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" s="83"/>
-      <c r="B8" s="80"/>
+      <c r="A8" s="88"/>
+      <c r="B8" s="85"/>
       <c r="C8" s="24" t="s">
         <v>11</v>
       </c>
@@ -4153,8 +4165,8 @@
       <c r="J8" s="67"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" s="83"/>
-      <c r="B9" s="80"/>
+      <c r="A9" s="88"/>
+      <c r="B9" s="85"/>
       <c r="C9" s="24" t="s">
         <v>12</v>
       </c>
@@ -4172,8 +4184,8 @@
       <c r="I9" s="69"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" s="83"/>
-      <c r="B10" s="81"/>
+      <c r="A10" s="88"/>
+      <c r="B10" s="86"/>
       <c r="C10" s="29" t="s">
         <v>24</v>
       </c>
@@ -4191,9 +4203,9 @@
       <c r="I10" s="69"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" s="83"/>
-      <c r="B11" s="73" t="s">
-        <v>15</v>
+      <c r="A11" s="88"/>
+      <c r="B11" s="78" t="s">
+        <v>129</v>
       </c>
       <c r="C11" s="31" t="s">
         <v>25</v>
@@ -4212,9 +4224,9 @@
       <c r="I11" s="69"/>
     </row>
     <row r="12" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A12" s="83"/>
-      <c r="B12" s="84"/>
-      <c r="C12" s="90" t="s">
+      <c r="A12" s="88"/>
+      <c r="B12" s="91"/>
+      <c r="C12" s="74" t="s">
         <v>13</v>
       </c>
       <c r="D12" s="34">
@@ -4226,16 +4238,16 @@
       <c r="F12" s="34">
         <v>0</v>
       </c>
-      <c r="G12" s="89" t="s">
-        <v>124</v>
+      <c r="G12" s="73" t="s">
+        <v>123</v>
       </c>
       <c r="H12" s="68"/>
       <c r="I12" s="69"/>
     </row>
     <row r="13" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A13" s="83"/>
-      <c r="B13" s="84"/>
-      <c r="C13" s="90" t="s">
+      <c r="A13" s="88"/>
+      <c r="B13" s="91"/>
+      <c r="C13" s="74" t="s">
         <v>19</v>
       </c>
       <c r="D13" s="34">
@@ -4247,15 +4259,15 @@
       <c r="F13" s="34">
         <v>0</v>
       </c>
-      <c r="G13" s="89" t="s">
-        <v>124</v>
+      <c r="G13" s="73" t="s">
+        <v>123</v>
       </c>
       <c r="I13" s="69"/>
     </row>
     <row r="14" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A14" s="83"/>
-      <c r="B14" s="84"/>
-      <c r="C14" s="90" t="s">
+      <c r="A14" s="88"/>
+      <c r="B14" s="91"/>
+      <c r="C14" s="74" t="s">
         <v>20</v>
       </c>
       <c r="D14" s="34">
@@ -4267,15 +4279,15 @@
       <c r="F14" s="34">
         <v>0</v>
       </c>
-      <c r="G14" s="89" t="s">
-        <v>124</v>
+      <c r="G14" s="73" t="s">
+        <v>123</v>
       </c>
       <c r="I14" s="69"/>
     </row>
     <row r="15" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A15" s="83"/>
-      <c r="B15" s="84"/>
-      <c r="C15" s="90" t="s">
+      <c r="A15" s="88"/>
+      <c r="B15" s="91"/>
+      <c r="C15" s="74" t="s">
         <v>21</v>
       </c>
       <c r="D15" s="34">
@@ -4287,14 +4299,14 @@
       <c r="F15" s="34">
         <v>0</v>
       </c>
-      <c r="G15" s="89" t="s">
-        <v>124</v>
+      <c r="G15" s="73" t="s">
+        <v>123</v>
       </c>
       <c r="I15" s="69"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A16" s="83"/>
-      <c r="B16" s="84"/>
+      <c r="A16" s="88"/>
+      <c r="B16" s="91"/>
       <c r="C16" s="33" t="s">
         <v>23</v>
       </c>
@@ -4311,8 +4323,8 @@
       <c r="I16" s="69"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" s="83"/>
-      <c r="B17" s="84"/>
+      <c r="A17" s="88"/>
+      <c r="B17" s="91"/>
       <c r="C17" s="33" t="s">
         <v>22</v>
       </c>
@@ -4329,8 +4341,8 @@
       <c r="I17" s="69"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" s="83"/>
-      <c r="B18" s="84"/>
+      <c r="A18" s="88"/>
+      <c r="B18" s="91"/>
       <c r="C18" s="27" t="s">
         <v>26</v>
       </c>
@@ -4347,8 +4359,8 @@
       <c r="I18" s="69"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="83"/>
-      <c r="B19" s="75"/>
+      <c r="A19" s="88"/>
+      <c r="B19" s="80"/>
       <c r="C19" s="3" t="s">
         <v>27</v>
       </c>
@@ -4365,8 +4377,8 @@
       <c r="I19" s="69"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A20" s="83"/>
-      <c r="B20" s="79" t="s">
+      <c r="A20" s="88"/>
+      <c r="B20" s="84" t="s">
         <v>28</v>
       </c>
       <c r="C20" s="20" t="s">
@@ -4385,8 +4397,8 @@
       <c r="I20" s="69"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21" s="83"/>
-      <c r="B21" s="82"/>
+      <c r="A21" s="88"/>
+      <c r="B21" s="87"/>
       <c r="C21" s="22" t="s">
         <v>31</v>
       </c>
@@ -4403,8 +4415,8 @@
       <c r="I21" s="69"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A22" s="83"/>
-      <c r="B22" s="81"/>
+      <c r="A22" s="88"/>
+      <c r="B22" s="86"/>
       <c r="C22" s="7" t="s">
         <v>30</v>
       </c>
@@ -4420,7 +4432,7 @@
       <c r="G22" s="58"/>
     </row>
     <row r="23" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A23" s="83"/>
+      <c r="A23" s="88"/>
       <c r="B23" s="4" t="s">
         <v>17</v>
       </c>
@@ -4436,13 +4448,13 @@
       <c r="F23" s="13">
         <v>1</v>
       </c>
-      <c r="G23" s="91" t="s">
-        <v>125</v>
+      <c r="G23" s="75" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A24" s="83"/>
-      <c r="B24" s="79" t="s">
+      <c r="A24" s="88"/>
+      <c r="B24" s="84" t="s">
         <v>16</v>
       </c>
       <c r="C24" s="20" t="s">
@@ -4457,13 +4469,13 @@
       <c r="F24" s="21">
         <v>1</v>
       </c>
-      <c r="G24" s="92" t="s">
-        <v>126</v>
+      <c r="G24" s="76" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A25" s="83"/>
-      <c r="B25" s="82"/>
+      <c r="A25" s="88"/>
+      <c r="B25" s="87"/>
       <c r="C25" s="6" t="s">
         <v>34</v>
       </c>
@@ -4476,8 +4488,8 @@
       <c r="F25" s="12">
         <v>0</v>
       </c>
-      <c r="G25" s="93" t="s">
-        <v>127</v>
+      <c r="G25" s="77" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
@@ -4490,10 +4502,10 @@
       <c r="G26" s="57"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A27" s="76" t="s">
-        <v>1</v>
-      </c>
-      <c r="B27" s="79" t="s">
+      <c r="A27" s="81" t="s">
+        <v>1</v>
+      </c>
+      <c r="B27" s="84" t="s">
         <v>35</v>
       </c>
       <c r="C27" s="20" t="s">
@@ -4512,8 +4524,8 @@
       <c r="I27" s="69"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A28" s="77"/>
-      <c r="B28" s="80"/>
+      <c r="A28" s="82"/>
+      <c r="B28" s="85"/>
       <c r="C28" s="22" t="s">
         <v>50</v>
       </c>
@@ -4532,8 +4544,8 @@
       <c r="I28" s="69"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A29" s="83"/>
-      <c r="B29" s="81"/>
+      <c r="A29" s="88"/>
+      <c r="B29" s="86"/>
       <c r="C29" s="7" t="s">
         <v>37</v>
       </c>
@@ -4550,8 +4562,8 @@
       <c r="I29" s="69"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A30" s="83"/>
-      <c r="B30" s="73" t="s">
+      <c r="A30" s="88"/>
+      <c r="B30" s="78" t="s">
         <v>36</v>
       </c>
       <c r="C30" s="31" t="s">
@@ -4570,8 +4582,8 @@
       <c r="I30" s="69"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A31" s="83"/>
-      <c r="B31" s="74"/>
+      <c r="A31" s="88"/>
+      <c r="B31" s="79"/>
       <c r="C31" s="27" t="s">
         <v>102</v>
       </c>
@@ -4588,8 +4600,8 @@
       <c r="I31" s="69"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A32" s="83"/>
-      <c r="B32" s="75"/>
+      <c r="A32" s="88"/>
+      <c r="B32" s="80"/>
       <c r="C32" s="3" t="s">
         <v>103</v>
       </c>
@@ -4606,8 +4618,8 @@
       <c r="I32" s="69"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A33" s="83"/>
-      <c r="B33" s="82" t="s">
+      <c r="A33" s="88"/>
+      <c r="B33" s="87" t="s">
         <v>16</v>
       </c>
       <c r="C33" s="20" t="s">
@@ -4626,8 +4638,8 @@
       <c r="I33" s="69"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A34" s="83"/>
-      <c r="B34" s="82"/>
+      <c r="A34" s="88"/>
+      <c r="B34" s="87"/>
       <c r="C34" s="22" t="s">
         <v>112</v>
       </c>
@@ -4644,8 +4656,8 @@
       <c r="I34" s="69"/>
     </row>
     <row r="35" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A35" s="78"/>
-      <c r="B35" s="82"/>
+      <c r="A35" s="83"/>
+      <c r="B35" s="87"/>
       <c r="C35" s="15" t="s">
         <v>42</v>
       </c>
@@ -4672,10 +4684,10 @@
       <c r="I36" s="69"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A37" s="85" t="s">
+      <c r="A37" s="89" t="s">
         <v>49</v>
       </c>
-      <c r="B37" s="79" t="s">
+      <c r="B37" s="84" t="s">
         <v>35</v>
       </c>
       <c r="C37" s="20" t="s">
@@ -4694,8 +4706,8 @@
       <c r="I37" s="69"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A38" s="86"/>
-      <c r="B38" s="80"/>
+      <c r="A38" s="90"/>
+      <c r="B38" s="85"/>
       <c r="C38" s="22" t="s">
         <v>43</v>
       </c>
@@ -4712,8 +4724,8 @@
       <c r="I38" s="69"/>
     </row>
     <row r="39" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A39" s="83"/>
-      <c r="B39" s="81"/>
+      <c r="A39" s="88"/>
+      <c r="B39" s="86"/>
       <c r="C39" s="17" t="s">
         <v>44</v>
       </c>
@@ -4730,12 +4742,12 @@
       <c r="I39" s="69"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A40" s="83"/>
-      <c r="B40" s="73" t="s">
-        <v>48</v>
+      <c r="A40" s="88"/>
+      <c r="B40" s="78" t="s">
+        <v>130</v>
       </c>
       <c r="C40" s="38" t="s">
-        <v>60</v>
+        <v>131</v>
       </c>
       <c r="D40" s="18">
         <v>1</v>
@@ -4750,8 +4762,8 @@
       <c r="I40" s="69"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A41" s="83"/>
-      <c r="B41" s="75"/>
+      <c r="A41" s="88"/>
+      <c r="B41" s="80"/>
       <c r="C41" s="2" t="s">
         <v>61</v>
       </c>
@@ -4768,8 +4780,8 @@
       <c r="I41" s="69"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A42" s="83"/>
-      <c r="B42" s="79" t="s">
+      <c r="A42" s="88"/>
+      <c r="B42" s="84" t="s">
         <v>36</v>
       </c>
       <c r="C42" s="20" t="s">
@@ -4788,8 +4800,8 @@
       <c r="I42" s="69"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A43" s="83"/>
-      <c r="B43" s="80"/>
+      <c r="A43" s="88"/>
+      <c r="B43" s="85"/>
       <c r="C43" s="22" t="s">
         <v>45</v>
       </c>
@@ -4806,8 +4818,8 @@
       <c r="I43" s="69"/>
     </row>
     <row r="44" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A44" s="83"/>
-      <c r="B44" s="81"/>
+      <c r="A44" s="88"/>
+      <c r="B44" s="86"/>
       <c r="C44" s="17" t="s">
         <v>46</v>
       </c>
@@ -4824,7 +4836,7 @@
       <c r="I44" s="69"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A45" s="78"/>
+      <c r="A45" s="83"/>
       <c r="B45" s="39" t="s">
         <v>16</v>
       </c>
@@ -4854,10 +4866,10 @@
       <c r="I46" s="69"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A47" s="76" t="s">
+      <c r="A47" s="81" t="s">
         <v>4</v>
       </c>
-      <c r="B47" s="79" t="s">
+      <c r="B47" s="84" t="s">
         <v>35</v>
       </c>
       <c r="C47" s="20" t="s">
@@ -4876,8 +4888,8 @@
       <c r="I47" s="69"/>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A48" s="83"/>
-      <c r="B48" s="80"/>
+      <c r="A48" s="88"/>
+      <c r="B48" s="85"/>
       <c r="C48" s="22" t="s">
         <v>52</v>
       </c>
@@ -4894,8 +4906,8 @@
       <c r="I48" s="69"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A49" s="83"/>
-      <c r="B49" s="80"/>
+      <c r="A49" s="88"/>
+      <c r="B49" s="85"/>
       <c r="C49" s="22" t="s">
         <v>53</v>
       </c>
@@ -4912,8 +4924,8 @@
       <c r="I49" s="69"/>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A50" s="83"/>
-      <c r="B50" s="81"/>
+      <c r="A50" s="88"/>
+      <c r="B50" s="86"/>
       <c r="C50" s="7" t="s">
         <v>54</v>
       </c>
@@ -4930,8 +4942,8 @@
       <c r="I50" s="69"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A51" s="83"/>
-      <c r="B51" s="74" t="s">
+      <c r="A51" s="88"/>
+      <c r="B51" s="79" t="s">
         <v>36</v>
       </c>
       <c r="C51" s="27" t="s">
@@ -4950,8 +4962,8 @@
       <c r="I51" s="69"/>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A52" s="83"/>
-      <c r="B52" s="74"/>
+      <c r="A52" s="88"/>
+      <c r="B52" s="79"/>
       <c r="C52" s="33" t="s">
         <v>55</v>
       </c>
@@ -4968,8 +4980,8 @@
       <c r="I52" s="69"/>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A53" s="83"/>
-      <c r="B53" s="74"/>
+      <c r="A53" s="88"/>
+      <c r="B53" s="79"/>
       <c r="C53" s="33" t="s">
         <v>56</v>
       </c>
@@ -4986,8 +4998,8 @@
       <c r="I53" s="69"/>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A54" s="83"/>
-      <c r="B54" s="75"/>
+      <c r="A54" s="88"/>
+      <c r="B54" s="80"/>
       <c r="C54" s="3" t="s">
         <v>57</v>
       </c>
@@ -5004,8 +5016,8 @@
       <c r="I54" s="69"/>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A55" s="83"/>
-      <c r="B55" s="82" t="s">
+      <c r="A55" s="88"/>
+      <c r="B55" s="87" t="s">
         <v>16</v>
       </c>
       <c r="C55" s="24" t="s">
@@ -5024,8 +5036,8 @@
       <c r="I55" s="69"/>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A56" s="78"/>
-      <c r="B56" s="82"/>
+      <c r="A56" s="83"/>
+      <c r="B56" s="87"/>
       <c r="C56" s="16" t="s">
         <v>59</v>
       </c>
@@ -5052,10 +5064,10 @@
       <c r="I57" s="69"/>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A58" s="76" t="s">
+      <c r="A58" s="81" t="s">
         <v>3</v>
       </c>
-      <c r="B58" s="79" t="s">
+      <c r="B58" s="84" t="s">
         <v>35</v>
       </c>
       <c r="C58" s="20" t="s">
@@ -5074,8 +5086,8 @@
       <c r="I58" s="69"/>
     </row>
     <row r="59" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A59" s="83"/>
-      <c r="B59" s="80"/>
+      <c r="A59" s="88"/>
+      <c r="B59" s="85"/>
       <c r="C59" s="43" t="s">
         <v>62</v>
       </c>
@@ -5094,8 +5106,8 @@
       <c r="I59" s="69"/>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A60" s="83"/>
-      <c r="B60" s="80"/>
+      <c r="A60" s="88"/>
+      <c r="B60" s="85"/>
       <c r="C60" s="22" t="s">
         <v>63</v>
       </c>
@@ -5112,8 +5124,8 @@
       <c r="I60" s="69"/>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A61" s="83"/>
-      <c r="B61" s="81"/>
+      <c r="A61" s="88"/>
+      <c r="B61" s="86"/>
       <c r="C61" s="7" t="s">
         <v>64</v>
       </c>
@@ -5130,8 +5142,8 @@
       <c r="I61" s="69"/>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A62" s="83"/>
-      <c r="B62" s="73" t="s">
+      <c r="A62" s="88"/>
+      <c r="B62" s="78" t="s">
         <v>36</v>
       </c>
       <c r="C62" s="31" t="s">
@@ -5150,8 +5162,8 @@
       <c r="I62" s="69"/>
     </row>
     <row r="63" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A63" s="83"/>
-      <c r="B63" s="74"/>
+      <c r="A63" s="88"/>
+      <c r="B63" s="79"/>
       <c r="C63" s="44" t="s">
         <v>65</v>
       </c>
@@ -5170,8 +5182,8 @@
       <c r="I63" s="69"/>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A64" s="83"/>
-      <c r="B64" s="74"/>
+      <c r="A64" s="88"/>
+      <c r="B64" s="79"/>
       <c r="C64" s="33" t="s">
         <v>66</v>
       </c>
@@ -5188,8 +5200,8 @@
       <c r="I64" s="69"/>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A65" s="83"/>
-      <c r="B65" s="75"/>
+      <c r="A65" s="88"/>
+      <c r="B65" s="80"/>
       <c r="C65" s="3" t="s">
         <v>67</v>
       </c>
@@ -5206,9 +5218,9 @@
       <c r="I65" s="69"/>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A66" s="83"/>
-      <c r="B66" s="87" t="s">
-        <v>121</v>
+      <c r="A66" s="88"/>
+      <c r="B66" s="92" t="s">
+        <v>120</v>
       </c>
       <c r="C66" s="20" t="s">
         <v>68</v>
@@ -5226,8 +5238,8 @@
       <c r="I66" s="69"/>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A67" s="83"/>
-      <c r="B67" s="80"/>
+      <c r="A67" s="88"/>
+      <c r="B67" s="85"/>
       <c r="C67" s="22" t="s">
         <v>69</v>
       </c>
@@ -5244,8 +5256,8 @@
       <c r="I67" s="69"/>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A68" s="83"/>
-      <c r="B68" s="81"/>
+      <c r="A68" s="88"/>
+      <c r="B68" s="86"/>
       <c r="C68" s="7" t="s">
         <v>70</v>
       </c>
@@ -5262,9 +5274,9 @@
       <c r="I68" s="69"/>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A69" s="83"/>
-      <c r="B69" s="88" t="s">
-        <v>122</v>
+      <c r="A69" s="88"/>
+      <c r="B69" s="93" t="s">
+        <v>121</v>
       </c>
       <c r="C69" s="31" t="s">
         <v>71</v>
@@ -5282,8 +5294,8 @@
       <c r="I69" s="69"/>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A70" s="83"/>
-      <c r="B70" s="84"/>
+      <c r="A70" s="88"/>
+      <c r="B70" s="91"/>
       <c r="C70" s="33" t="s">
         <v>72</v>
       </c>
@@ -5300,8 +5312,8 @@
       <c r="I70" s="69"/>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A71" s="83"/>
-      <c r="B71" s="74"/>
+      <c r="A71" s="88"/>
+      <c r="B71" s="79"/>
       <c r="C71" s="40" t="s">
         <v>73</v>
       </c>
@@ -5318,8 +5330,8 @@
       <c r="I71" s="69"/>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A72" s="83"/>
-      <c r="B72" s="79" t="s">
+      <c r="A72" s="88"/>
+      <c r="B72" s="84" t="s">
         <v>16</v>
       </c>
       <c r="C72" s="20" t="s">
@@ -5338,8 +5350,8 @@
       <c r="I72" s="69"/>
     </row>
     <row r="73" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A73" s="83"/>
-      <c r="B73" s="80"/>
+      <c r="A73" s="88"/>
+      <c r="B73" s="85"/>
       <c r="C73" s="43" t="s">
         <v>76</v>
       </c>
@@ -5356,8 +5368,8 @@
       <c r="I73" s="69"/>
     </row>
     <row r="74" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A74" s="78"/>
-      <c r="B74" s="81"/>
+      <c r="A74" s="83"/>
+      <c r="B74" s="86"/>
       <c r="C74" s="17" t="s">
         <v>77</v>
       </c>
@@ -5384,10 +5396,10 @@
       <c r="I75" s="69"/>
     </row>
     <row r="76" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A76" s="76" t="s">
+      <c r="A76" s="81" t="s">
         <v>2</v>
       </c>
-      <c r="B76" s="79" t="s">
+      <c r="B76" s="84" t="s">
         <v>35</v>
       </c>
       <c r="C76" s="20" t="s">
@@ -5408,8 +5420,8 @@
       <c r="I76" s="69"/>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A77" s="77"/>
-      <c r="B77" s="80"/>
+      <c r="A77" s="82"/>
+      <c r="B77" s="85"/>
       <c r="C77" s="22" t="s">
         <v>79</v>
       </c>
@@ -5428,8 +5440,8 @@
       <c r="I77" s="69"/>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A78" s="77"/>
-      <c r="B78" s="80"/>
+      <c r="A78" s="82"/>
+      <c r="B78" s="85"/>
       <c r="C78" s="22" t="s">
         <v>80</v>
       </c>
@@ -5446,8 +5458,8 @@
       <c r="I78" s="69"/>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A79" s="77"/>
-      <c r="B79" s="80"/>
+      <c r="A79" s="82"/>
+      <c r="B79" s="85"/>
       <c r="C79" s="22" t="s">
         <v>81</v>
       </c>
@@ -5464,8 +5476,8 @@
       <c r="I79" s="69"/>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A80" s="77"/>
-      <c r="B80" s="80"/>
+      <c r="A80" s="82"/>
+      <c r="B80" s="85"/>
       <c r="C80" s="22" t="s">
         <v>83</v>
       </c>
@@ -5484,8 +5496,8 @@
       <c r="I80" s="69"/>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A81" s="77"/>
-      <c r="B81" s="80"/>
+      <c r="A81" s="82"/>
+      <c r="B81" s="85"/>
       <c r="C81" s="22" t="s">
         <v>84</v>
       </c>
@@ -5504,8 +5516,8 @@
       <c r="I81" s="69"/>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A82" s="77"/>
-      <c r="B82" s="80"/>
+      <c r="A82" s="82"/>
+      <c r="B82" s="85"/>
       <c r="C82" s="22" t="s">
         <v>85</v>
       </c>
@@ -5522,8 +5534,8 @@
       <c r="I82" s="69"/>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A83" s="77"/>
-      <c r="B83" s="81"/>
+      <c r="A83" s="82"/>
+      <c r="B83" s="86"/>
       <c r="C83" s="7" t="s">
         <v>82</v>
       </c>
@@ -5540,8 +5552,8 @@
       <c r="I83" s="69"/>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A84" s="77"/>
-      <c r="B84" s="73" t="s">
+      <c r="A84" s="82"/>
+      <c r="B84" s="78" t="s">
         <v>36</v>
       </c>
       <c r="C84" s="31" t="s">
@@ -5562,8 +5574,8 @@
       <c r="I84" s="69"/>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A85" s="77"/>
-      <c r="B85" s="84"/>
+      <c r="A85" s="82"/>
+      <c r="B85" s="91"/>
       <c r="C85" s="27" t="s">
         <v>87</v>
       </c>
@@ -5582,8 +5594,8 @@
       <c r="I85" s="69"/>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A86" s="77"/>
-      <c r="B86" s="84"/>
+      <c r="A86" s="82"/>
+      <c r="B86" s="91"/>
       <c r="C86" s="27" t="s">
         <v>88</v>
       </c>
@@ -5600,8 +5612,8 @@
       <c r="I86" s="69"/>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A87" s="77"/>
-      <c r="B87" s="84"/>
+      <c r="A87" s="82"/>
+      <c r="B87" s="91"/>
       <c r="C87" s="27" t="s">
         <v>89</v>
       </c>
@@ -5618,8 +5630,8 @@
       <c r="I87" s="69"/>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A88" s="77"/>
-      <c r="B88" s="84"/>
+      <c r="A88" s="82"/>
+      <c r="B88" s="91"/>
       <c r="C88" s="27" t="s">
         <v>90</v>
       </c>
@@ -5638,8 +5650,8 @@
       <c r="I88" s="69"/>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A89" s="77"/>
-      <c r="B89" s="84"/>
+      <c r="A89" s="82"/>
+      <c r="B89" s="91"/>
       <c r="C89" s="27" t="s">
         <v>91</v>
       </c>
@@ -5658,8 +5670,8 @@
       <c r="I89" s="69"/>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A90" s="77"/>
-      <c r="B90" s="84"/>
+      <c r="A90" s="82"/>
+      <c r="B90" s="91"/>
       <c r="C90" s="27" t="s">
         <v>92</v>
       </c>
@@ -5676,8 +5688,8 @@
       <c r="I90" s="69"/>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A91" s="77"/>
-      <c r="B91" s="75"/>
+      <c r="A91" s="82"/>
+      <c r="B91" s="80"/>
       <c r="C91" s="3" t="s">
         <v>93</v>
       </c>
@@ -5694,8 +5706,8 @@
       <c r="I91" s="67"/>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A92" s="77"/>
-      <c r="B92" s="79" t="s">
+      <c r="A92" s="82"/>
+      <c r="B92" s="84" t="s">
         <v>16</v>
       </c>
       <c r="C92" s="20" t="s">
@@ -5714,8 +5726,8 @@
       <c r="I92" s="67"/>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A93" s="77"/>
-      <c r="B93" s="81"/>
+      <c r="A93" s="82"/>
+      <c r="B93" s="86"/>
       <c r="C93" s="6" t="s">
         <v>95</v>
       </c>
@@ -5732,8 +5744,8 @@
       <c r="I93" s="67"/>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A94" s="77"/>
-      <c r="B94" s="73" t="s">
+      <c r="A94" s="82"/>
+      <c r="B94" s="78" t="s">
         <v>107</v>
       </c>
       <c r="C94" s="31" t="s">
@@ -5752,8 +5764,8 @@
       <c r="I94" s="67"/>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A95" s="77"/>
-      <c r="B95" s="74"/>
+      <c r="A95" s="82"/>
+      <c r="B95" s="79"/>
       <c r="C95" s="33" t="s">
         <v>113</v>
       </c>
@@ -5770,8 +5782,8 @@
       <c r="I95" s="67"/>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A96" s="77"/>
-      <c r="B96" s="74"/>
+      <c r="A96" s="82"/>
+      <c r="B96" s="79"/>
       <c r="C96" s="33" t="s">
         <v>109</v>
       </c>
@@ -5787,8 +5799,8 @@
       <c r="G96" s="48"/>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A97" s="78"/>
-      <c r="B97" s="75"/>
+      <c r="A97" s="83"/>
+      <c r="B97" s="80"/>
       <c r="C97" s="40" t="s">
         <v>114</v>
       </c>

</xml_diff>

<commit_message>
relecture et corrections du fichier de tests ainsi que quelques corrections du rapport
</commit_message>
<xml_diff>
--- a/Doc/Tests/liste_de_tests.xlsx
+++ b/Doc/Tests/liste_de_tests.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F558BB1-DE3E-4D19-8FB8-56DB2DB74271}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68444C54-8F59-4AF8-8F46-42876DB14766}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="600" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PostgreSQL" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="139">
   <si>
     <t>Client</t>
   </si>
@@ -400,18 +400,10 @@
 budget</t>
   </si>
   <si>
-    <t>Clients du budget
- partagé</t>
-  </si>
-  <si>
     <t>Entité à 
 tester</t>
   </si>
   <si>
-    <t>Erreur de connexion toujours 
-présente si déconnexion du client</t>
-  </si>
-  <si>
     <t>Champs de la partie connexion
 plus accessibles avec le curseur</t>
   </si>
@@ -437,6 +429,37 @@
   </si>
   <si>
     <t>Le résumé du compte par défaut s'affiche sur le tableau de bord</t>
+  </si>
+  <si>
+    <t>Message d'erreur toujours 
+présent si déconnexion du client</t>
+  </si>
+  <si>
+    <t>Accès au tableau de bord à la connexion d'un compte activé</t>
+  </si>
+  <si>
+    <t>Connexion avec client supprimé</t>
+  </si>
+  <si>
+    <t>Si aucun compte par défaut n'existe, le tableau de bord ne se remplit pas</t>
+  </si>
+  <si>
+    <t>Accès au tableau de bord et activation du compte à la saisie du bon code</t>
+  </si>
+  <si>
+    <t>La modification d'un compte bancaire en compte par défaut, retire l'attribut "par défaut" du compte par défaut s'il existe</t>
+  </si>
+  <si>
+    <t>Clients du budget
+partagé</t>
+  </si>
+  <si>
+    <t>Modification d'une dette avec un ou plusieurs champs obligatoires 
+manquants</t>
+  </si>
+  <si>
+    <t>Modification d'une créance avec un ou plusieurs champs obligatoires 
+manquants</t>
   </si>
 </sst>
 </file>
@@ -577,7 +600,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="94">
+  <cellXfs count="103">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -766,6 +789,24 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -775,44 +816,51 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1128,16 +1176,16 @@
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.77734375" customWidth="1"/>
-    <col min="2" max="2" width="22.77734375" customWidth="1"/>
-    <col min="3" max="3" width="65.77734375" customWidth="1"/>
-    <col min="4" max="5" width="7.77734375" style="19" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="32.33203125" style="64" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" customWidth="1"/>
+    <col min="3" max="3" width="65.7109375" customWidth="1"/>
+    <col min="4" max="5" width="7.7109375" style="19" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="32.28515625" style="64" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -1157,11 +1205,11 @@
         <v>104</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="81" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="85" t="s">
+      <c r="B2" s="79" t="s">
         <v>14</v>
       </c>
       <c r="C2" s="20" t="s">
@@ -1175,9 +1223,9 @@
       </c>
       <c r="F2" s="50"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="88"/>
-      <c r="B3" s="85"/>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="82"/>
+      <c r="B3" s="79"/>
       <c r="C3" s="22" t="s">
         <v>8</v>
       </c>
@@ -1195,9 +1243,9 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="88"/>
-      <c r="B4" s="85"/>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="82"/>
+      <c r="B4" s="79"/>
       <c r="C4" s="22" t="s">
         <v>9</v>
       </c>
@@ -1215,9 +1263,9 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="88"/>
-      <c r="B5" s="85"/>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="82"/>
+      <c r="B5" s="79"/>
       <c r="C5" s="22" t="s">
         <v>10</v>
       </c>
@@ -1229,9 +1277,9 @@
       </c>
       <c r="F5" s="51"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="88"/>
-      <c r="B6" s="85"/>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="82"/>
+      <c r="B6" s="79"/>
       <c r="C6" s="24" t="s">
         <v>11</v>
       </c>
@@ -1243,9 +1291,9 @@
       </c>
       <c r="F6" s="52"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="88"/>
-      <c r="B7" s="85"/>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="82"/>
+      <c r="B7" s="79"/>
       <c r="C7" s="24" t="s">
         <v>12</v>
       </c>
@@ -1257,9 +1305,9 @@
       </c>
       <c r="F7" s="52"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="88"/>
-      <c r="B8" s="86"/>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="82"/>
+      <c r="B8" s="80"/>
       <c r="C8" s="29" t="s">
         <v>24</v>
       </c>
@@ -1271,9 +1319,9 @@
       </c>
       <c r="F8" s="66"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="88"/>
-      <c r="B9" s="78" t="s">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="82"/>
+      <c r="B9" s="84" t="s">
         <v>15</v>
       </c>
       <c r="C9" s="31" t="s">
@@ -1287,9 +1335,9 @@
       </c>
       <c r="F9" s="53"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="88"/>
-      <c r="B10" s="91"/>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="82"/>
+      <c r="B10" s="87"/>
       <c r="C10" s="33" t="s">
         <v>13</v>
       </c>
@@ -1301,9 +1349,9 @@
       </c>
       <c r="F10" s="48"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="88"/>
-      <c r="B11" s="91"/>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="82"/>
+      <c r="B11" s="87"/>
       <c r="C11" s="33" t="s">
         <v>19</v>
       </c>
@@ -1315,9 +1363,9 @@
       </c>
       <c r="F11" s="48"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="88"/>
-      <c r="B12" s="91"/>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="82"/>
+      <c r="B12" s="87"/>
       <c r="C12" s="33" t="s">
         <v>20</v>
       </c>
@@ -1329,9 +1377,9 @@
       </c>
       <c r="F12" s="48"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="88"/>
-      <c r="B13" s="91"/>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="82"/>
+      <c r="B13" s="87"/>
       <c r="C13" s="33" t="s">
         <v>21</v>
       </c>
@@ -1343,9 +1391,9 @@
       </c>
       <c r="F13" s="48"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="88"/>
-      <c r="B14" s="91"/>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="82"/>
+      <c r="B14" s="87"/>
       <c r="C14" s="33" t="s">
         <v>23</v>
       </c>
@@ -1357,9 +1405,9 @@
       </c>
       <c r="F14" s="48"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="88"/>
-      <c r="B15" s="91"/>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="82"/>
+      <c r="B15" s="87"/>
       <c r="C15" s="33" t="s">
         <v>22</v>
       </c>
@@ -1371,9 +1419,9 @@
       </c>
       <c r="F15" s="48"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="88"/>
-      <c r="B16" s="91"/>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="82"/>
+      <c r="B16" s="87"/>
       <c r="C16" s="27" t="s">
         <v>26</v>
       </c>
@@ -1385,9 +1433,9 @@
       </c>
       <c r="F16" s="59"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="88"/>
-      <c r="B17" s="80"/>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="82"/>
+      <c r="B17" s="86"/>
       <c r="C17" s="3" t="s">
         <v>27</v>
       </c>
@@ -1399,9 +1447,9 @@
       </c>
       <c r="F17" s="54"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="88"/>
-      <c r="B18" s="84" t="s">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="82"/>
+      <c r="B18" s="78" t="s">
         <v>28</v>
       </c>
       <c r="C18" s="20" t="s">
@@ -1415,9 +1463,9 @@
       </c>
       <c r="F18" s="50"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" s="88"/>
-      <c r="B19" s="87"/>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="82"/>
+      <c r="B19" s="88"/>
       <c r="C19" s="22" t="s">
         <v>31</v>
       </c>
@@ -1429,9 +1477,9 @@
       </c>
       <c r="F19" s="51"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="88"/>
-      <c r="B20" s="86"/>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="82"/>
+      <c r="B20" s="80"/>
       <c r="C20" s="7" t="s">
         <v>30</v>
       </c>
@@ -1443,8 +1491,8 @@
       </c>
       <c r="F20" s="58"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" s="88"/>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="82"/>
       <c r="B21" s="4" t="s">
         <v>17</v>
       </c>
@@ -1461,9 +1509,9 @@
         <v>116</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" s="88"/>
-      <c r="B22" s="84" t="s">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="82"/>
+      <c r="B22" s="78" t="s">
         <v>16</v>
       </c>
       <c r="C22" s="20" t="s">
@@ -1479,9 +1527,9 @@
         <v>110</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23" s="88"/>
-      <c r="B23" s="87"/>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="82"/>
+      <c r="B23" s="88"/>
       <c r="C23" s="6" t="s">
         <v>34</v>
       </c>
@@ -1495,7 +1543,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="14"/>
       <c r="B24" s="14"/>
       <c r="C24" s="14"/>
@@ -1503,11 +1551,11 @@
       <c r="E24" s="36"/>
       <c r="F24" s="57"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="81" t="s">
         <v>1</v>
       </c>
-      <c r="B25" s="84" t="s">
+      <c r="B25" s="78" t="s">
         <v>35</v>
       </c>
       <c r="C25" s="20" t="s">
@@ -1521,9 +1569,9 @@
       </c>
       <c r="F25" s="50"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26" s="82"/>
-      <c r="B26" s="85"/>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="89"/>
+      <c r="B26" s="79"/>
       <c r="C26" s="22" t="s">
         <v>50</v>
       </c>
@@ -1535,9 +1583,9 @@
       </c>
       <c r="F26" s="51"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A27" s="88"/>
-      <c r="B27" s="86"/>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="82"/>
+      <c r="B27" s="80"/>
       <c r="C27" s="7" t="s">
         <v>37</v>
       </c>
@@ -1549,9 +1597,9 @@
       </c>
       <c r="F27" s="58"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A28" s="88"/>
-      <c r="B28" s="78" t="s">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="82"/>
+      <c r="B28" s="84" t="s">
         <v>36</v>
       </c>
       <c r="C28" s="31" t="s">
@@ -1565,9 +1613,9 @@
       </c>
       <c r="F28" s="53"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A29" s="88"/>
-      <c r="B29" s="79"/>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="82"/>
+      <c r="B29" s="85"/>
       <c r="C29" s="27" t="s">
         <v>102</v>
       </c>
@@ -1579,9 +1627,9 @@
       </c>
       <c r="F29" s="59"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A30" s="88"/>
-      <c r="B30" s="80"/>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="82"/>
+      <c r="B30" s="86"/>
       <c r="C30" s="3" t="s">
         <v>103</v>
       </c>
@@ -1593,9 +1641,9 @@
       </c>
       <c r="F30" s="54"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A31" s="88"/>
-      <c r="B31" s="87" t="s">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="82"/>
+      <c r="B31" s="88" t="s">
         <v>16</v>
       </c>
       <c r="C31" s="20" t="s">
@@ -1609,9 +1657,9 @@
       </c>
       <c r="F31" s="50"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A32" s="88"/>
-      <c r="B32" s="87"/>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="82"/>
+      <c r="B32" s="88"/>
       <c r="C32" s="22" t="s">
         <v>112</v>
       </c>
@@ -1623,9 +1671,9 @@
       </c>
       <c r="F32" s="51"/>
     </row>
-    <row r="33" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="83"/>
-      <c r="B33" s="87"/>
+      <c r="B33" s="88"/>
       <c r="C33" s="15" t="s">
         <v>42</v>
       </c>
@@ -1637,7 +1685,7 @@
       </c>
       <c r="F33" s="60"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="14"/>
       <c r="B34" s="14"/>
       <c r="C34" s="14"/>
@@ -1645,11 +1693,11 @@
       <c r="E34" s="36"/>
       <c r="F34" s="57"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A35" s="89" t="s">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="90" t="s">
         <v>49</v>
       </c>
-      <c r="B35" s="84" t="s">
+      <c r="B35" s="78" t="s">
         <v>35</v>
       </c>
       <c r="C35" s="20" t="s">
@@ -1663,9 +1711,9 @@
       </c>
       <c r="F35" s="50"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A36" s="90"/>
-      <c r="B36" s="85"/>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="91"/>
+      <c r="B36" s="79"/>
       <c r="C36" s="22" t="s">
         <v>43</v>
       </c>
@@ -1677,9 +1725,9 @@
       </c>
       <c r="F36" s="51"/>
     </row>
-    <row r="37" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A37" s="88"/>
-      <c r="B37" s="86"/>
+    <row r="37" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A37" s="82"/>
+      <c r="B37" s="80"/>
       <c r="C37" s="17" t="s">
         <v>44</v>
       </c>
@@ -1691,9 +1739,9 @@
       </c>
       <c r="F37" s="58"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A38" s="88"/>
-      <c r="B38" s="78" t="s">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="82"/>
+      <c r="B38" s="84" t="s">
         <v>48</v>
       </c>
       <c r="C38" s="38" t="s">
@@ -1707,9 +1755,9 @@
       </c>
       <c r="F38" s="61"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A39" s="88"/>
-      <c r="B39" s="80"/>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="82"/>
+      <c r="B39" s="86"/>
       <c r="C39" s="2" t="s">
         <v>61</v>
       </c>
@@ -1721,9 +1769,9 @@
       </c>
       <c r="F39" s="61"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A40" s="88"/>
-      <c r="B40" s="84" t="s">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="82"/>
+      <c r="B40" s="78" t="s">
         <v>36</v>
       </c>
       <c r="C40" s="20" t="s">
@@ -1737,9 +1785,9 @@
       </c>
       <c r="F40" s="50"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A41" s="88"/>
-      <c r="B41" s="85"/>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="82"/>
+      <c r="B41" s="79"/>
       <c r="C41" s="22" t="s">
         <v>45</v>
       </c>
@@ -1751,9 +1799,9 @@
       </c>
       <c r="F41" s="51"/>
     </row>
-    <row r="42" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A42" s="88"/>
-      <c r="B42" s="86"/>
+    <row r="42" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A42" s="82"/>
+      <c r="B42" s="80"/>
       <c r="C42" s="17" t="s">
         <v>46</v>
       </c>
@@ -1765,7 +1813,7 @@
       </c>
       <c r="F42" s="58"/>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="83"/>
       <c r="B43" s="39" t="s">
         <v>16</v>
@@ -1781,7 +1829,7 @@
       </c>
       <c r="F43" s="56"/>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="14"/>
       <c r="B44" s="14"/>
       <c r="C44" s="14"/>
@@ -1789,11 +1837,11 @@
       <c r="E44" s="36"/>
       <c r="F44" s="57"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="81" t="s">
         <v>4</v>
       </c>
-      <c r="B45" s="84" t="s">
+      <c r="B45" s="78" t="s">
         <v>35</v>
       </c>
       <c r="C45" s="20" t="s">
@@ -1807,9 +1855,9 @@
       </c>
       <c r="F45" s="50"/>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A46" s="88"/>
-      <c r="B46" s="85"/>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="82"/>
+      <c r="B46" s="79"/>
       <c r="C46" s="22" t="s">
         <v>52</v>
       </c>
@@ -1821,9 +1869,9 @@
       </c>
       <c r="F46" s="51"/>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A47" s="88"/>
-      <c r="B47" s="85"/>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="82"/>
+      <c r="B47" s="79"/>
       <c r="C47" s="22" t="s">
         <v>53</v>
       </c>
@@ -1835,9 +1883,9 @@
       </c>
       <c r="F47" s="51"/>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A48" s="88"/>
-      <c r="B48" s="86"/>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="82"/>
+      <c r="B48" s="80"/>
       <c r="C48" s="7" t="s">
         <v>54</v>
       </c>
@@ -1849,9 +1897,9 @@
       </c>
       <c r="F48" s="58"/>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A49" s="88"/>
-      <c r="B49" s="79" t="s">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="82"/>
+      <c r="B49" s="85" t="s">
         <v>36</v>
       </c>
       <c r="C49" s="27" t="s">
@@ -1865,9 +1913,9 @@
       </c>
       <c r="F49" s="59"/>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A50" s="88"/>
-      <c r="B50" s="79"/>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="82"/>
+      <c r="B50" s="85"/>
       <c r="C50" s="33" t="s">
         <v>55</v>
       </c>
@@ -1879,9 +1927,9 @@
       </c>
       <c r="F50" s="48"/>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A51" s="88"/>
-      <c r="B51" s="79"/>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="82"/>
+      <c r="B51" s="85"/>
       <c r="C51" s="33" t="s">
         <v>56</v>
       </c>
@@ -1893,9 +1941,9 @@
       </c>
       <c r="F51" s="48"/>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A52" s="88"/>
-      <c r="B52" s="80"/>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="82"/>
+      <c r="B52" s="86"/>
       <c r="C52" s="3" t="s">
         <v>57</v>
       </c>
@@ -1907,9 +1955,9 @@
       </c>
       <c r="F52" s="54"/>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A53" s="88"/>
-      <c r="B53" s="87" t="s">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="82"/>
+      <c r="B53" s="88" t="s">
         <v>16</v>
       </c>
       <c r="C53" s="24" t="s">
@@ -1923,9 +1971,9 @@
       </c>
       <c r="F53" s="52"/>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="83"/>
-      <c r="B54" s="87"/>
+      <c r="B54" s="88"/>
       <c r="C54" s="16" t="s">
         <v>59</v>
       </c>
@@ -1937,7 +1985,7 @@
       </c>
       <c r="F54" s="60"/>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="14"/>
       <c r="B55" s="14"/>
       <c r="C55" s="14"/>
@@ -1945,11 +1993,11 @@
       <c r="E55" s="36"/>
       <c r="F55" s="57"/>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="81" t="s">
         <v>3</v>
       </c>
-      <c r="B56" s="84" t="s">
+      <c r="B56" s="78" t="s">
         <v>35</v>
       </c>
       <c r="C56" s="20" t="s">
@@ -1963,9 +2011,9 @@
       </c>
       <c r="F56" s="50"/>
     </row>
-    <row r="57" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A57" s="88"/>
-      <c r="B57" s="85"/>
+    <row r="57" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A57" s="82"/>
+      <c r="B57" s="79"/>
       <c r="C57" s="43" t="s">
         <v>62</v>
       </c>
@@ -1979,9 +2027,9 @@
         <v>101</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A58" s="88"/>
-      <c r="B58" s="85"/>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" s="82"/>
+      <c r="B58" s="79"/>
       <c r="C58" s="22" t="s">
         <v>63</v>
       </c>
@@ -1993,9 +2041,9 @@
       </c>
       <c r="F58" s="51"/>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A59" s="88"/>
-      <c r="B59" s="86"/>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" s="82"/>
+      <c r="B59" s="80"/>
       <c r="C59" s="7" t="s">
         <v>64</v>
       </c>
@@ -2007,9 +2055,9 @@
       </c>
       <c r="F59" s="58"/>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A60" s="88"/>
-      <c r="B60" s="78" t="s">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" s="82"/>
+      <c r="B60" s="84" t="s">
         <v>36</v>
       </c>
       <c r="C60" s="31" t="s">
@@ -2023,9 +2071,9 @@
       </c>
       <c r="F60" s="53"/>
     </row>
-    <row r="61" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A61" s="88"/>
-      <c r="B61" s="79"/>
+    <row r="61" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A61" s="82"/>
+      <c r="B61" s="85"/>
       <c r="C61" s="44" t="s">
         <v>65</v>
       </c>
@@ -2039,9 +2087,9 @@
         <v>101</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A62" s="88"/>
-      <c r="B62" s="79"/>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" s="82"/>
+      <c r="B62" s="85"/>
       <c r="C62" s="33" t="s">
         <v>66</v>
       </c>
@@ -2053,9 +2101,9 @@
       </c>
       <c r="F62" s="48"/>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A63" s="88"/>
-      <c r="B63" s="80"/>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" s="82"/>
+      <c r="B63" s="86"/>
       <c r="C63" s="3" t="s">
         <v>67</v>
       </c>
@@ -2067,9 +2115,9 @@
       </c>
       <c r="F63" s="54"/>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A64" s="88"/>
-      <c r="B64" s="84" t="s">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" s="82"/>
+      <c r="B64" s="78" t="s">
         <v>74</v>
       </c>
       <c r="C64" s="20" t="s">
@@ -2083,9 +2131,9 @@
       </c>
       <c r="F64" s="50"/>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A65" s="88"/>
-      <c r="B65" s="85"/>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" s="82"/>
+      <c r="B65" s="79"/>
       <c r="C65" s="22" t="s">
         <v>69</v>
       </c>
@@ -2097,9 +2145,9 @@
       </c>
       <c r="F65" s="51"/>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A66" s="88"/>
-      <c r="B66" s="86"/>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" s="82"/>
+      <c r="B66" s="80"/>
       <c r="C66" s="7" t="s">
         <v>70</v>
       </c>
@@ -2111,9 +2159,9 @@
       </c>
       <c r="F66" s="58"/>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A67" s="88"/>
-      <c r="B67" s="78" t="s">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67" s="82"/>
+      <c r="B67" s="84" t="s">
         <v>96</v>
       </c>
       <c r="C67" s="31" t="s">
@@ -2127,9 +2175,9 @@
       </c>
       <c r="F67" s="53"/>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A68" s="88"/>
-      <c r="B68" s="91"/>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68" s="82"/>
+      <c r="B68" s="87"/>
       <c r="C68" s="33" t="s">
         <v>72</v>
       </c>
@@ -2141,9 +2189,9 @@
       </c>
       <c r="F68" s="48"/>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A69" s="88"/>
-      <c r="B69" s="79"/>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69" s="82"/>
+      <c r="B69" s="85"/>
       <c r="C69" s="40" t="s">
         <v>73</v>
       </c>
@@ -2155,9 +2203,9 @@
       </c>
       <c r="F69" s="61"/>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A70" s="88"/>
-      <c r="B70" s="84" t="s">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70" s="82"/>
+      <c r="B70" s="78" t="s">
         <v>16</v>
       </c>
       <c r="C70" s="20" t="s">
@@ -2171,9 +2219,9 @@
       </c>
       <c r="F70" s="50"/>
     </row>
-    <row r="71" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A71" s="88"/>
-      <c r="B71" s="85"/>
+    <row r="71" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A71" s="82"/>
+      <c r="B71" s="79"/>
       <c r="C71" s="43" t="s">
         <v>76</v>
       </c>
@@ -2185,9 +2233,9 @@
       </c>
       <c r="F71" s="51"/>
     </row>
-    <row r="72" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A72" s="83"/>
-      <c r="B72" s="86"/>
+      <c r="B72" s="80"/>
       <c r="C72" s="17" t="s">
         <v>77</v>
       </c>
@@ -2199,7 +2247,7 @@
       </c>
       <c r="F72" s="58"/>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="14"/>
       <c r="B73" s="14"/>
       <c r="C73" s="14"/>
@@ -2207,11 +2255,11 @@
       <c r="E73" s="36"/>
       <c r="F73" s="57"/>
     </row>
-    <row r="74" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="81" t="s">
         <v>2</v>
       </c>
-      <c r="B74" s="84" t="s">
+      <c r="B74" s="78" t="s">
         <v>35</v>
       </c>
       <c r="C74" s="20" t="s">
@@ -2227,9 +2275,9 @@
         <v>115</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A75" s="82"/>
-      <c r="B75" s="85"/>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A75" s="89"/>
+      <c r="B75" s="79"/>
       <c r="C75" s="22" t="s">
         <v>79</v>
       </c>
@@ -2243,9 +2291,9 @@
         <v>115</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A76" s="82"/>
-      <c r="B76" s="85"/>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A76" s="89"/>
+      <c r="B76" s="79"/>
       <c r="C76" s="22" t="s">
         <v>80</v>
       </c>
@@ -2257,9 +2305,9 @@
       </c>
       <c r="F76" s="51"/>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A77" s="82"/>
-      <c r="B77" s="85"/>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A77" s="89"/>
+      <c r="B77" s="79"/>
       <c r="C77" s="22" t="s">
         <v>81</v>
       </c>
@@ -2271,9 +2319,9 @@
       </c>
       <c r="F77" s="51"/>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A78" s="82"/>
-      <c r="B78" s="85"/>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A78" s="89"/>
+      <c r="B78" s="79"/>
       <c r="C78" s="22" t="s">
         <v>83</v>
       </c>
@@ -2287,9 +2335,9 @@
         <v>115</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A79" s="82"/>
-      <c r="B79" s="85"/>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A79" s="89"/>
+      <c r="B79" s="79"/>
       <c r="C79" s="22" t="s">
         <v>84</v>
       </c>
@@ -2303,9 +2351,9 @@
         <v>115</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A80" s="82"/>
-      <c r="B80" s="85"/>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A80" s="89"/>
+      <c r="B80" s="79"/>
       <c r="C80" s="22" t="s">
         <v>85</v>
       </c>
@@ -2317,9 +2365,9 @@
       </c>
       <c r="F80" s="51"/>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A81" s="82"/>
-      <c r="B81" s="86"/>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A81" s="89"/>
+      <c r="B81" s="80"/>
       <c r="C81" s="7" t="s">
         <v>82</v>
       </c>
@@ -2331,9 +2379,9 @@
       </c>
       <c r="F81" s="58"/>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A82" s="82"/>
-      <c r="B82" s="78" t="s">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A82" s="89"/>
+      <c r="B82" s="84" t="s">
         <v>36</v>
       </c>
       <c r="C82" s="31" t="s">
@@ -2349,9 +2397,9 @@
         <v>115</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A83" s="82"/>
-      <c r="B83" s="91"/>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A83" s="89"/>
+      <c r="B83" s="87"/>
       <c r="C83" s="27" t="s">
         <v>87</v>
       </c>
@@ -2365,9 +2413,9 @@
         <v>115</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A84" s="82"/>
-      <c r="B84" s="91"/>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A84" s="89"/>
+      <c r="B84" s="87"/>
       <c r="C84" s="27" t="s">
         <v>88</v>
       </c>
@@ -2379,9 +2427,9 @@
       </c>
       <c r="F84" s="59"/>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A85" s="82"/>
-      <c r="B85" s="91"/>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A85" s="89"/>
+      <c r="B85" s="87"/>
       <c r="C85" s="27" t="s">
         <v>89</v>
       </c>
@@ -2393,9 +2441,9 @@
       </c>
       <c r="F85" s="59"/>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A86" s="82"/>
-      <c r="B86" s="91"/>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A86" s="89"/>
+      <c r="B86" s="87"/>
       <c r="C86" s="27" t="s">
         <v>90</v>
       </c>
@@ -2409,9 +2457,9 @@
         <v>115</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A87" s="82"/>
-      <c r="B87" s="91"/>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A87" s="89"/>
+      <c r="B87" s="87"/>
       <c r="C87" s="27" t="s">
         <v>91</v>
       </c>
@@ -2425,9 +2473,9 @@
         <v>115</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A88" s="82"/>
-      <c r="B88" s="91"/>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A88" s="89"/>
+      <c r="B88" s="87"/>
       <c r="C88" s="27" t="s">
         <v>92</v>
       </c>
@@ -2439,9 +2487,9 @@
       </c>
       <c r="F88" s="59"/>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A89" s="82"/>
-      <c r="B89" s="80"/>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A89" s="89"/>
+      <c r="B89" s="86"/>
       <c r="C89" s="3" t="s">
         <v>93</v>
       </c>
@@ -2453,9 +2501,9 @@
       </c>
       <c r="F89" s="54"/>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A90" s="82"/>
-      <c r="B90" s="84" t="s">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A90" s="89"/>
+      <c r="B90" s="78" t="s">
         <v>16</v>
       </c>
       <c r="C90" s="20" t="s">
@@ -2469,9 +2517,9 @@
       </c>
       <c r="F90" s="50"/>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A91" s="82"/>
-      <c r="B91" s="86"/>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A91" s="89"/>
+      <c r="B91" s="80"/>
       <c r="C91" s="6" t="s">
         <v>95</v>
       </c>
@@ -2483,9 +2531,9 @@
       </c>
       <c r="F91" s="60"/>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A92" s="82"/>
-      <c r="B92" s="78" t="s">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A92" s="89"/>
+      <c r="B92" s="84" t="s">
         <v>107</v>
       </c>
       <c r="C92" s="31" t="s">
@@ -2499,9 +2547,9 @@
       </c>
       <c r="F92" s="53"/>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A93" s="82"/>
-      <c r="B93" s="79"/>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A93" s="89"/>
+      <c r="B93" s="85"/>
       <c r="C93" s="33" t="s">
         <v>113</v>
       </c>
@@ -2513,9 +2561,9 @@
       </c>
       <c r="F93" s="48"/>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A94" s="82"/>
-      <c r="B94" s="79"/>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A94" s="89"/>
+      <c r="B94" s="85"/>
       <c r="C94" s="33" t="s">
         <v>109</v>
       </c>
@@ -2527,9 +2575,9 @@
       </c>
       <c r="F94" s="48"/>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" s="83"/>
-      <c r="B95" s="80"/>
+      <c r="B95" s="86"/>
       <c r="C95" s="40" t="s">
         <v>114</v>
       </c>
@@ -2541,7 +2589,7 @@
       </c>
       <c r="F95" s="61"/>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" s="14"/>
       <c r="B96" s="14"/>
       <c r="C96" s="14"/>
@@ -2551,18 +2599,6 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="B45:B48"/>
-    <mergeCell ref="A56:A72"/>
-    <mergeCell ref="B56:B59"/>
-    <mergeCell ref="B60:B63"/>
-    <mergeCell ref="B64:B66"/>
-    <mergeCell ref="B67:B69"/>
-    <mergeCell ref="B70:B72"/>
-    <mergeCell ref="B2:B8"/>
-    <mergeCell ref="B9:B17"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="A2:A23"/>
     <mergeCell ref="B92:B95"/>
     <mergeCell ref="A74:A95"/>
     <mergeCell ref="B25:B27"/>
@@ -2579,6 +2615,18 @@
     <mergeCell ref="B49:B52"/>
     <mergeCell ref="B53:B54"/>
     <mergeCell ref="A45:A54"/>
+    <mergeCell ref="B2:B8"/>
+    <mergeCell ref="B9:B17"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="A2:A23"/>
+    <mergeCell ref="B45:B48"/>
+    <mergeCell ref="A56:A72"/>
+    <mergeCell ref="B56:B59"/>
+    <mergeCell ref="B60:B63"/>
+    <mergeCell ref="B64:B66"/>
+    <mergeCell ref="B67:B69"/>
+    <mergeCell ref="B70:B72"/>
   </mergeCells>
   <conditionalFormatting sqref="D97:E1048576 D56:E72 D1:E54 D74:E91">
     <cfRule type="iconSet" priority="12">
@@ -2647,16 +2695,16 @@
       <selection activeCell="E2" sqref="E2:E83"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.77734375" customWidth="1"/>
-    <col min="2" max="2" width="22.77734375" customWidth="1"/>
-    <col min="3" max="3" width="70.33203125" customWidth="1"/>
-    <col min="4" max="5" width="7.77734375" style="19" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="32.33203125" style="64" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" customWidth="1"/>
+    <col min="3" max="3" width="70.28515625" customWidth="1"/>
+    <col min="4" max="5" width="7.7109375" style="19" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="32.28515625" style="64" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -2676,11 +2724,11 @@
         <v>104</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="81" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="85" t="s">
+      <c r="B2" s="79" t="s">
         <v>14</v>
       </c>
       <c r="C2" s="20" t="s">
@@ -2694,9 +2742,9 @@
       </c>
       <c r="F2" s="50"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="88"/>
-      <c r="B3" s="85"/>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="82"/>
+      <c r="B3" s="79"/>
       <c r="C3" s="22" t="s">
         <v>8</v>
       </c>
@@ -2714,9 +2762,9 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="88"/>
-      <c r="B4" s="85"/>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="82"/>
+      <c r="B4" s="79"/>
       <c r="C4" s="22" t="s">
         <v>9</v>
       </c>
@@ -2734,9 +2782,9 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="88"/>
-      <c r="B5" s="85"/>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="82"/>
+      <c r="B5" s="79"/>
       <c r="C5" s="22" t="s">
         <v>10</v>
       </c>
@@ -2748,9 +2796,9 @@
       </c>
       <c r="F5" s="51"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="88"/>
-      <c r="B6" s="85"/>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="82"/>
+      <c r="B6" s="79"/>
       <c r="C6" s="24" t="s">
         <v>11</v>
       </c>
@@ -2762,9 +2810,9 @@
       </c>
       <c r="F6" s="52"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="88"/>
-      <c r="B7" s="85"/>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="82"/>
+      <c r="B7" s="79"/>
       <c r="C7" s="24" t="s">
         <v>12</v>
       </c>
@@ -2776,9 +2824,9 @@
       </c>
       <c r="F7" s="52"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="88"/>
-      <c r="B8" s="78" t="s">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="82"/>
+      <c r="B8" s="84" t="s">
         <v>15</v>
       </c>
       <c r="C8" s="31" t="s">
@@ -2792,9 +2840,9 @@
       </c>
       <c r="F8" s="53"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="88"/>
-      <c r="B9" s="91"/>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="82"/>
+      <c r="B9" s="87"/>
       <c r="C9" s="33" t="s">
         <v>13</v>
       </c>
@@ -2806,9 +2854,9 @@
       </c>
       <c r="F9" s="48"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="88"/>
-      <c r="B10" s="91"/>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="82"/>
+      <c r="B10" s="87"/>
       <c r="C10" s="33" t="s">
         <v>19</v>
       </c>
@@ -2822,9 +2870,9 @@
         <v>99</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="88"/>
-      <c r="B11" s="91"/>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="82"/>
+      <c r="B11" s="87"/>
       <c r="C11" s="33" t="s">
         <v>20</v>
       </c>
@@ -2836,9 +2884,9 @@
       </c>
       <c r="F11" s="48"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="88"/>
-      <c r="B12" s="91"/>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="82"/>
+      <c r="B12" s="87"/>
       <c r="C12" s="33" t="s">
         <v>21</v>
       </c>
@@ -2850,9 +2898,9 @@
       </c>
       <c r="F12" s="48"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="88"/>
-      <c r="B13" s="91"/>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="82"/>
+      <c r="B13" s="87"/>
       <c r="C13" s="33" t="s">
         <v>23</v>
       </c>
@@ -2864,9 +2912,9 @@
       </c>
       <c r="F13" s="48"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="88"/>
-      <c r="B14" s="91"/>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="82"/>
+      <c r="B14" s="87"/>
       <c r="C14" s="33" t="s">
         <v>22</v>
       </c>
@@ -2878,9 +2926,9 @@
       </c>
       <c r="F14" s="48"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="88"/>
-      <c r="B15" s="80"/>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="82"/>
+      <c r="B15" s="86"/>
       <c r="C15" s="3" t="s">
         <v>100</v>
       </c>
@@ -2892,8 +2940,8 @@
       </c>
       <c r="F15" s="54"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="88"/>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="82"/>
       <c r="B16" s="41" t="s">
         <v>17</v>
       </c>
@@ -2908,9 +2956,9 @@
       </c>
       <c r="F16" s="55"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="88"/>
-      <c r="B17" s="78" t="s">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="82"/>
+      <c r="B17" s="84" t="s">
         <v>16</v>
       </c>
       <c r="C17" s="31" t="s">
@@ -2924,9 +2972,9 @@
       </c>
       <c r="F17" s="53"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="88"/>
-      <c r="B18" s="91"/>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="82"/>
+      <c r="B18" s="87"/>
       <c r="C18" s="40" t="s">
         <v>34</v>
       </c>
@@ -2940,7 +2988,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="14"/>
       <c r="B19" s="14"/>
       <c r="C19" s="14"/>
@@ -2948,11 +2996,11 @@
       <c r="E19" s="36"/>
       <c r="F19" s="57"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="81" t="s">
         <v>1</v>
       </c>
-      <c r="B20" s="84" t="s">
+      <c r="B20" s="78" t="s">
         <v>35</v>
       </c>
       <c r="C20" s="20" t="s">
@@ -2966,9 +3014,9 @@
       </c>
       <c r="F20" s="50"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" s="82"/>
-      <c r="B21" s="85"/>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="89"/>
+      <c r="B21" s="79"/>
       <c r="C21" s="22" t="s">
         <v>50</v>
       </c>
@@ -2982,9 +3030,9 @@
         <v>101</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" s="88"/>
-      <c r="B22" s="86"/>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="82"/>
+      <c r="B22" s="80"/>
       <c r="C22" s="7" t="s">
         <v>37</v>
       </c>
@@ -2996,9 +3044,9 @@
       </c>
       <c r="F22" s="58"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23" s="88"/>
-      <c r="B23" s="78" t="s">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="82"/>
+      <c r="B23" s="84" t="s">
         <v>36</v>
       </c>
       <c r="C23" s="31" t="s">
@@ -3014,9 +3062,9 @@
         <v>101</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24" s="88"/>
-      <c r="B24" s="79"/>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="82"/>
+      <c r="B24" s="85"/>
       <c r="C24" s="27" t="s">
         <v>102</v>
       </c>
@@ -3028,9 +3076,9 @@
       </c>
       <c r="F24" s="59"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25" s="88"/>
-      <c r="B25" s="80"/>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="82"/>
+      <c r="B25" s="86"/>
       <c r="C25" s="3" t="s">
         <v>103</v>
       </c>
@@ -3042,9 +3090,9 @@
       </c>
       <c r="F25" s="54"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26" s="88"/>
-      <c r="B26" s="87" t="s">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="82"/>
+      <c r="B26" s="88" t="s">
         <v>16</v>
       </c>
       <c r="C26" s="20" t="s">
@@ -3058,9 +3106,9 @@
       </c>
       <c r="F26" s="50"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A27" s="88"/>
-      <c r="B27" s="87"/>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="82"/>
+      <c r="B27" s="88"/>
       <c r="C27" s="22" t="s">
         <v>112</v>
       </c>
@@ -3072,9 +3120,9 @@
       </c>
       <c r="F27" s="51"/>
     </row>
-    <row r="28" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="83"/>
-      <c r="B28" s="87"/>
+      <c r="B28" s="88"/>
       <c r="C28" s="15" t="s">
         <v>42</v>
       </c>
@@ -3086,7 +3134,7 @@
       </c>
       <c r="F28" s="60"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="14"/>
       <c r="B29" s="14"/>
       <c r="C29" s="14"/>
@@ -3094,11 +3142,11 @@
       <c r="E29" s="36"/>
       <c r="F29" s="57"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A30" s="89" t="s">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="90" t="s">
         <v>49</v>
       </c>
-      <c r="B30" s="84" t="s">
+      <c r="B30" s="78" t="s">
         <v>35</v>
       </c>
       <c r="C30" s="20" t="s">
@@ -3112,9 +3160,9 @@
       </c>
       <c r="F30" s="50"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A31" s="90"/>
-      <c r="B31" s="85"/>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="91"/>
+      <c r="B31" s="79"/>
       <c r="C31" s="22" t="s">
         <v>43</v>
       </c>
@@ -3126,9 +3174,9 @@
       </c>
       <c r="F31" s="51"/>
     </row>
-    <row r="32" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A32" s="88"/>
-      <c r="B32" s="86"/>
+    <row r="32" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" s="82"/>
+      <c r="B32" s="80"/>
       <c r="C32" s="17" t="s">
         <v>44</v>
       </c>
@@ -3140,9 +3188,9 @@
       </c>
       <c r="F32" s="58"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A33" s="88"/>
-      <c r="B33" s="78" t="s">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="82"/>
+      <c r="B33" s="84" t="s">
         <v>48</v>
       </c>
       <c r="C33" s="38" t="s">
@@ -3156,9 +3204,9 @@
       </c>
       <c r="F33" s="61"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A34" s="88"/>
-      <c r="B34" s="80"/>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="82"/>
+      <c r="B34" s="86"/>
       <c r="C34" s="2" t="s">
         <v>61</v>
       </c>
@@ -3170,9 +3218,9 @@
       </c>
       <c r="F34" s="61"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A35" s="88"/>
-      <c r="B35" s="84" t="s">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="82"/>
+      <c r="B35" s="78" t="s">
         <v>36</v>
       </c>
       <c r="C35" s="20" t="s">
@@ -3186,9 +3234,9 @@
       </c>
       <c r="F35" s="50"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A36" s="88"/>
-      <c r="B36" s="85"/>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="82"/>
+      <c r="B36" s="79"/>
       <c r="C36" s="22" t="s">
         <v>45</v>
       </c>
@@ -3200,9 +3248,9 @@
       </c>
       <c r="F36" s="51"/>
     </row>
-    <row r="37" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A37" s="88"/>
-      <c r="B37" s="86"/>
+    <row r="37" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A37" s="82"/>
+      <c r="B37" s="80"/>
       <c r="C37" s="17" t="s">
         <v>46</v>
       </c>
@@ -3214,7 +3262,7 @@
       </c>
       <c r="F37" s="58"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="83"/>
       <c r="B38" s="39" t="s">
         <v>16</v>
@@ -3230,7 +3278,7 @@
       </c>
       <c r="F38" s="56"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="14"/>
       <c r="B39" s="14"/>
       <c r="C39" s="14"/>
@@ -3238,11 +3286,11 @@
       <c r="E39" s="36"/>
       <c r="F39" s="57"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="81" t="s">
         <v>4</v>
       </c>
-      <c r="B40" s="84" t="s">
+      <c r="B40" s="78" t="s">
         <v>35</v>
       </c>
       <c r="C40" s="20" t="s">
@@ -3256,9 +3304,9 @@
       </c>
       <c r="F40" s="50"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A41" s="88"/>
-      <c r="B41" s="85"/>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="82"/>
+      <c r="B41" s="79"/>
       <c r="C41" s="22" t="s">
         <v>52</v>
       </c>
@@ -3270,9 +3318,9 @@
       </c>
       <c r="F41" s="51"/>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A42" s="88"/>
-      <c r="B42" s="85"/>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="82"/>
+      <c r="B42" s="79"/>
       <c r="C42" s="22" t="s">
         <v>53</v>
       </c>
@@ -3284,9 +3332,9 @@
       </c>
       <c r="F42" s="51"/>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A43" s="88"/>
-      <c r="B43" s="86"/>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="82"/>
+      <c r="B43" s="80"/>
       <c r="C43" s="7" t="s">
         <v>54</v>
       </c>
@@ -3298,9 +3346,9 @@
       </c>
       <c r="F43" s="58"/>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A44" s="88"/>
-      <c r="B44" s="79" t="s">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="82"/>
+      <c r="B44" s="85" t="s">
         <v>36</v>
       </c>
       <c r="C44" s="27" t="s">
@@ -3314,9 +3362,9 @@
       </c>
       <c r="F44" s="59"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A45" s="88"/>
-      <c r="B45" s="79"/>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="82"/>
+      <c r="B45" s="85"/>
       <c r="C45" s="33" t="s">
         <v>55</v>
       </c>
@@ -3328,9 +3376,9 @@
       </c>
       <c r="F45" s="48"/>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A46" s="88"/>
-      <c r="B46" s="79"/>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="82"/>
+      <c r="B46" s="85"/>
       <c r="C46" s="33" t="s">
         <v>56</v>
       </c>
@@ -3342,9 +3390,9 @@
       </c>
       <c r="F46" s="48"/>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A47" s="88"/>
-      <c r="B47" s="80"/>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="82"/>
+      <c r="B47" s="86"/>
       <c r="C47" s="3" t="s">
         <v>57</v>
       </c>
@@ -3356,9 +3404,9 @@
       </c>
       <c r="F47" s="54"/>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A48" s="88"/>
-      <c r="B48" s="87" t="s">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="82"/>
+      <c r="B48" s="88" t="s">
         <v>16</v>
       </c>
       <c r="C48" s="24" t="s">
@@ -3372,9 +3420,9 @@
       </c>
       <c r="F48" s="52"/>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="83"/>
-      <c r="B49" s="87"/>
+      <c r="B49" s="88"/>
       <c r="C49" s="16" t="s">
         <v>59</v>
       </c>
@@ -3386,7 +3434,7 @@
       </c>
       <c r="F49" s="60"/>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="14"/>
       <c r="B50" s="14"/>
       <c r="C50" s="14"/>
@@ -3394,11 +3442,11 @@
       <c r="E50" s="36"/>
       <c r="F50" s="57"/>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="81" t="s">
         <v>3</v>
       </c>
-      <c r="B51" s="84" t="s">
+      <c r="B51" s="78" t="s">
         <v>35</v>
       </c>
       <c r="C51" s="20" t="s">
@@ -3412,9 +3460,9 @@
       </c>
       <c r="F51" s="50"/>
     </row>
-    <row r="52" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A52" s="88"/>
-      <c r="B52" s="85"/>
+    <row r="52" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A52" s="82"/>
+      <c r="B52" s="79"/>
       <c r="C52" s="43" t="s">
         <v>62</v>
       </c>
@@ -3428,9 +3476,9 @@
         <v>101</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A53" s="88"/>
-      <c r="B53" s="85"/>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="82"/>
+      <c r="B53" s="79"/>
       <c r="C53" s="22" t="s">
         <v>63</v>
       </c>
@@ -3442,9 +3490,9 @@
       </c>
       <c r="F53" s="51"/>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A54" s="88"/>
-      <c r="B54" s="86"/>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" s="82"/>
+      <c r="B54" s="80"/>
       <c r="C54" s="7" t="s">
         <v>64</v>
       </c>
@@ -3456,9 +3504,9 @@
       </c>
       <c r="F54" s="58"/>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A55" s="88"/>
-      <c r="B55" s="78" t="s">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" s="82"/>
+      <c r="B55" s="84" t="s">
         <v>36</v>
       </c>
       <c r="C55" s="31" t="s">
@@ -3472,9 +3520,9 @@
       </c>
       <c r="F55" s="53"/>
     </row>
-    <row r="56" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A56" s="88"/>
-      <c r="B56" s="79"/>
+    <row r="56" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A56" s="82"/>
+      <c r="B56" s="85"/>
       <c r="C56" s="44" t="s">
         <v>65</v>
       </c>
@@ -3488,9 +3536,9 @@
         <v>101</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A57" s="88"/>
-      <c r="B57" s="79"/>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" s="82"/>
+      <c r="B57" s="85"/>
       <c r="C57" s="33" t="s">
         <v>66</v>
       </c>
@@ -3502,9 +3550,9 @@
       </c>
       <c r="F57" s="48"/>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A58" s="88"/>
-      <c r="B58" s="80"/>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" s="82"/>
+      <c r="B58" s="86"/>
       <c r="C58" s="3" t="s">
         <v>67</v>
       </c>
@@ -3516,9 +3564,9 @@
       </c>
       <c r="F58" s="54"/>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A59" s="88"/>
-      <c r="B59" s="84" t="s">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" s="82"/>
+      <c r="B59" s="78" t="s">
         <v>74</v>
       </c>
       <c r="C59" s="20" t="s">
@@ -3532,9 +3580,9 @@
       </c>
       <c r="F59" s="50"/>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A60" s="88"/>
-      <c r="B60" s="85"/>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" s="82"/>
+      <c r="B60" s="79"/>
       <c r="C60" s="22" t="s">
         <v>69</v>
       </c>
@@ -3546,9 +3594,9 @@
       </c>
       <c r="F60" s="51"/>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A61" s="88"/>
-      <c r="B61" s="86"/>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" s="82"/>
+      <c r="B61" s="80"/>
       <c r="C61" s="7" t="s">
         <v>70</v>
       </c>
@@ -3560,8 +3608,8 @@
       </c>
       <c r="F61" s="58"/>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A62" s="88"/>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" s="82"/>
       <c r="B62" s="45" t="s">
         <v>16</v>
       </c>
@@ -3578,7 +3626,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="14"/>
       <c r="B63" s="14"/>
       <c r="C63" s="14"/>
@@ -3586,11 +3634,11 @@
       <c r="E63" s="36"/>
       <c r="F63" s="57"/>
     </row>
-    <row r="64" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="81" t="s">
         <v>2</v>
       </c>
-      <c r="B64" s="84" t="s">
+      <c r="B64" s="78" t="s">
         <v>35</v>
       </c>
       <c r="C64" s="20" t="s">
@@ -3606,9 +3654,9 @@
         <v>115</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A65" s="82"/>
-      <c r="B65" s="85"/>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" s="89"/>
+      <c r="B65" s="79"/>
       <c r="C65" s="22" t="s">
         <v>79</v>
       </c>
@@ -3622,9 +3670,9 @@
         <v>115</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A66" s="82"/>
-      <c r="B66" s="85"/>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" s="89"/>
+      <c r="B66" s="79"/>
       <c r="C66" s="24" t="s">
         <v>80</v>
       </c>
@@ -3636,9 +3684,9 @@
       </c>
       <c r="F66" s="52"/>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A67" s="82"/>
-      <c r="B67" s="85"/>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67" s="89"/>
+      <c r="B67" s="79"/>
       <c r="C67" s="24" t="s">
         <v>81</v>
       </c>
@@ -3650,9 +3698,9 @@
       </c>
       <c r="F67" s="52"/>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A68" s="82"/>
-      <c r="B68" s="85"/>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68" s="89"/>
+      <c r="B68" s="79"/>
       <c r="C68" s="24" t="s">
         <v>83</v>
       </c>
@@ -3666,9 +3714,9 @@
         <v>115</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A69" s="82"/>
-      <c r="B69" s="85"/>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69" s="89"/>
+      <c r="B69" s="79"/>
       <c r="C69" s="24" t="s">
         <v>84</v>
       </c>
@@ -3682,9 +3730,9 @@
         <v>115</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A70" s="82"/>
-      <c r="B70" s="85"/>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70" s="89"/>
+      <c r="B70" s="79"/>
       <c r="C70" s="24" t="s">
         <v>85</v>
       </c>
@@ -3696,9 +3744,9 @@
       </c>
       <c r="F70" s="52"/>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A71" s="82"/>
-      <c r="B71" s="86"/>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A71" s="89"/>
+      <c r="B71" s="80"/>
       <c r="C71" s="7" t="s">
         <v>82</v>
       </c>
@@ -3710,9 +3758,9 @@
       </c>
       <c r="F71" s="58"/>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A72" s="82"/>
-      <c r="B72" s="78" t="s">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A72" s="89"/>
+      <c r="B72" s="84" t="s">
         <v>36</v>
       </c>
       <c r="C72" s="31" t="s">
@@ -3728,9 +3776,9 @@
         <v>115</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A73" s="82"/>
-      <c r="B73" s="91"/>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A73" s="89"/>
+      <c r="B73" s="87"/>
       <c r="C73" s="33" t="s">
         <v>87</v>
       </c>
@@ -3744,9 +3792,9 @@
         <v>115</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A74" s="82"/>
-      <c r="B74" s="91"/>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A74" s="89"/>
+      <c r="B74" s="87"/>
       <c r="C74" s="27" t="s">
         <v>88</v>
       </c>
@@ -3758,9 +3806,9 @@
       </c>
       <c r="F74" s="59"/>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A75" s="82"/>
-      <c r="B75" s="91"/>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A75" s="89"/>
+      <c r="B75" s="87"/>
       <c r="C75" s="33" t="s">
         <v>89</v>
       </c>
@@ -3772,9 +3820,9 @@
       </c>
       <c r="F75" s="48"/>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A76" s="82"/>
-      <c r="B76" s="91"/>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A76" s="89"/>
+      <c r="B76" s="87"/>
       <c r="C76" s="33" t="s">
         <v>90</v>
       </c>
@@ -3788,9 +3836,9 @@
         <v>115</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A77" s="82"/>
-      <c r="B77" s="91"/>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A77" s="89"/>
+      <c r="B77" s="87"/>
       <c r="C77" s="33" t="s">
         <v>91</v>
       </c>
@@ -3804,9 +3852,9 @@
         <v>115</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A78" s="82"/>
-      <c r="B78" s="91"/>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A78" s="89"/>
+      <c r="B78" s="87"/>
       <c r="C78" s="33" t="s">
         <v>92</v>
       </c>
@@ -3818,9 +3866,9 @@
       </c>
       <c r="F78" s="48"/>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A79" s="82"/>
-      <c r="B79" s="80"/>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A79" s="89"/>
+      <c r="B79" s="86"/>
       <c r="C79" s="3" t="s">
         <v>93</v>
       </c>
@@ -3832,9 +3880,9 @@
       </c>
       <c r="F79" s="54"/>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A80" s="82"/>
-      <c r="B80" s="84" t="s">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A80" s="89"/>
+      <c r="B80" s="78" t="s">
         <v>16</v>
       </c>
       <c r="C80" s="20" t="s">
@@ -3848,9 +3896,9 @@
       </c>
       <c r="F80" s="50"/>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A81" s="82"/>
-      <c r="B81" s="86"/>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A81" s="89"/>
+      <c r="B81" s="80"/>
       <c r="C81" s="6" t="s">
         <v>95</v>
       </c>
@@ -3862,9 +3910,9 @@
       </c>
       <c r="F81" s="60"/>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A82" s="82"/>
-      <c r="B82" s="78" t="s">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A82" s="89"/>
+      <c r="B82" s="84" t="s">
         <v>107</v>
       </c>
       <c r="C82" s="31" t="s">
@@ -3878,9 +3926,9 @@
       </c>
       <c r="F82" s="53"/>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="83"/>
-      <c r="B83" s="80"/>
+      <c r="B83" s="86"/>
       <c r="C83" s="40" t="s">
         <v>109</v>
       </c>
@@ -3892,7 +3940,7 @@
       </c>
       <c r="F83" s="61"/>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="65"/>
       <c r="B84" s="14"/>
       <c r="C84" s="14"/>
@@ -3902,14 +3950,11 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="A2:A18"/>
-    <mergeCell ref="B2:B7"/>
-    <mergeCell ref="B8:B15"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="A20:A28"/>
-    <mergeCell ref="B20:B22"/>
-    <mergeCell ref="B23:B25"/>
-    <mergeCell ref="B26:B28"/>
+    <mergeCell ref="B64:B71"/>
+    <mergeCell ref="B72:B79"/>
+    <mergeCell ref="B80:B81"/>
+    <mergeCell ref="A64:A83"/>
+    <mergeCell ref="B82:B83"/>
     <mergeCell ref="A51:A62"/>
     <mergeCell ref="B51:B54"/>
     <mergeCell ref="B55:B58"/>
@@ -3922,11 +3967,14 @@
     <mergeCell ref="B40:B43"/>
     <mergeCell ref="B44:B47"/>
     <mergeCell ref="B48:B49"/>
-    <mergeCell ref="B64:B71"/>
-    <mergeCell ref="B72:B79"/>
-    <mergeCell ref="B80:B81"/>
-    <mergeCell ref="A64:A83"/>
-    <mergeCell ref="B82:B83"/>
+    <mergeCell ref="A2:A18"/>
+    <mergeCell ref="B2:B7"/>
+    <mergeCell ref="B8:B15"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="A20:A28"/>
+    <mergeCell ref="B20:B22"/>
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="B26:B28"/>
   </mergeCells>
   <conditionalFormatting sqref="D85:E1048576 D64:E81 D51:E62 D1:E49">
     <cfRule type="iconSet" priority="7">
@@ -3991,41 +4039,41 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E11F7609-0A7A-46D7-A44A-76050598E181}">
   <dimension ref="A1:J98"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView tabSelected="1" zoomScale="325" zoomScaleNormal="325" workbookViewId="0">
+      <selection activeCell="C97" sqref="C97"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.109375" customWidth="1"/>
-    <col min="2" max="2" width="17.33203125" customWidth="1"/>
-    <col min="3" max="3" width="65.77734375" customWidth="1"/>
-    <col min="4" max="4" width="8.5546875" style="19" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" customWidth="1"/>
+    <col min="3" max="3" width="65.7109375" customWidth="1"/>
+    <col min="4" max="4" width="8.5703125" style="19" customWidth="1"/>
     <col min="5" max="6" width="9" style="19" customWidth="1"/>
-    <col min="7" max="7" width="31.5546875" style="64" customWidth="1"/>
-    <col min="9" max="9" width="9.33203125" customWidth="1"/>
+    <col min="7" max="7" width="31.5703125" style="64" customWidth="1"/>
+    <col min="9" max="9" width="9.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="6"/>
       <c r="B1" s="8">
         <v>1</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D1" s="8"/>
       <c r="E1" s="8"/>
       <c r="F1" s="8"/>
       <c r="G1" s="63"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="7"/>
       <c r="B2" s="9">
         <v>0</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
@@ -4034,9 +4082,9 @@
       <c r="H2" s="68"/>
       <c r="I2" s="68"/>
     </row>
-    <row r="3" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="47" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B3" s="35" t="s">
         <v>6</v>
@@ -4060,11 +4108,11 @@
       <c r="I3" s="67"/>
       <c r="J3" s="67"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="81" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="85" t="s">
+      <c r="B4" s="79" t="s">
         <v>14</v>
       </c>
       <c r="C4" s="20" t="s">
@@ -4084,9 +4132,9 @@
       <c r="I4" s="72"/>
       <c r="J4" s="67"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="88"/>
-      <c r="B5" s="85"/>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="82"/>
+      <c r="B5" s="79"/>
       <c r="C5" s="22" t="s">
         <v>8</v>
       </c>
@@ -4104,9 +4152,9 @@
       <c r="I5" s="71"/>
       <c r="J5" s="67"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" s="88"/>
-      <c r="B6" s="85"/>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="82"/>
+      <c r="B6" s="79"/>
       <c r="C6" s="22" t="s">
         <v>9</v>
       </c>
@@ -4124,9 +4172,9 @@
       <c r="I6" s="71"/>
       <c r="J6" s="67"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" s="88"/>
-      <c r="B7" s="85"/>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="82"/>
+      <c r="B7" s="79"/>
       <c r="C7" s="22" t="s">
         <v>10</v>
       </c>
@@ -4144,9 +4192,9 @@
       <c r="I7" s="71"/>
       <c r="J7" s="67"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" s="88"/>
-      <c r="B8" s="85"/>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="82"/>
+      <c r="B8" s="79"/>
       <c r="C8" s="24" t="s">
         <v>11</v>
       </c>
@@ -4164,9 +4212,9 @@
       <c r="I8" s="70"/>
       <c r="J8" s="67"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" s="88"/>
-      <c r="B9" s="85"/>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="82"/>
+      <c r="B9" s="79"/>
       <c r="C9" s="24" t="s">
         <v>12</v>
       </c>
@@ -4183,9 +4231,9 @@
       <c r="H9" s="68"/>
       <c r="I9" s="69"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" s="88"/>
-      <c r="B10" s="86"/>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="82"/>
+      <c r="B10" s="80"/>
       <c r="C10" s="29" t="s">
         <v>24</v>
       </c>
@@ -4202,10 +4250,10 @@
       <c r="H10" s="68"/>
       <c r="I10" s="69"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" s="88"/>
-      <c r="B11" s="78" t="s">
-        <v>129</v>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="82"/>
+      <c r="B11" s="84" t="s">
+        <v>127</v>
       </c>
       <c r="C11" s="31" t="s">
         <v>25</v>
@@ -4223,9 +4271,9 @@
       <c r="H11" s="68"/>
       <c r="I11" s="69"/>
     </row>
-    <row r="12" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A12" s="88"/>
-      <c r="B12" s="91"/>
+    <row r="12" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="82"/>
+      <c r="B12" s="87"/>
       <c r="C12" s="74" t="s">
         <v>13</v>
       </c>
@@ -4239,14 +4287,14 @@
         <v>0</v>
       </c>
       <c r="G12" s="73" t="s">
-        <v>123</v>
+        <v>130</v>
       </c>
       <c r="H12" s="68"/>
       <c r="I12" s="69"/>
     </row>
-    <row r="13" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A13" s="88"/>
-      <c r="B13" s="91"/>
+    <row r="13" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="82"/>
+      <c r="B13" s="87"/>
       <c r="C13" s="74" t="s">
         <v>19</v>
       </c>
@@ -4260,13 +4308,13 @@
         <v>0</v>
       </c>
       <c r="G13" s="73" t="s">
-        <v>123</v>
+        <v>130</v>
       </c>
       <c r="I13" s="69"/>
     </row>
-    <row r="14" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A14" s="88"/>
-      <c r="B14" s="91"/>
+    <row r="14" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="82"/>
+      <c r="B14" s="87"/>
       <c r="C14" s="74" t="s">
         <v>20</v>
       </c>
@@ -4280,13 +4328,13 @@
         <v>0</v>
       </c>
       <c r="G14" s="73" t="s">
-        <v>123</v>
+        <v>130</v>
       </c>
       <c r="I14" s="69"/>
     </row>
-    <row r="15" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A15" s="88"/>
-      <c r="B15" s="91"/>
+    <row r="15" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="82"/>
+      <c r="B15" s="87"/>
       <c r="C15" s="74" t="s">
         <v>21</v>
       </c>
@@ -4300,13 +4348,13 @@
         <v>0</v>
       </c>
       <c r="G15" s="73" t="s">
-        <v>123</v>
+        <v>130</v>
       </c>
       <c r="I15" s="69"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A16" s="88"/>
-      <c r="B16" s="91"/>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="82"/>
+      <c r="B16" s="87"/>
       <c r="C16" s="33" t="s">
         <v>23</v>
       </c>
@@ -4322,9 +4370,9 @@
       <c r="G16" s="48"/>
       <c r="I16" s="69"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" s="88"/>
-      <c r="B17" s="91"/>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="82"/>
+      <c r="B17" s="87"/>
       <c r="C17" s="33" t="s">
         <v>22</v>
       </c>
@@ -4340,9 +4388,9 @@
       <c r="G17" s="48"/>
       <c r="I17" s="69"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" s="88"/>
-      <c r="B18" s="91"/>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="82"/>
+      <c r="B18" s="87"/>
       <c r="C18" s="27" t="s">
         <v>26</v>
       </c>
@@ -4358,11 +4406,11 @@
       <c r="G18" s="59"/>
       <c r="I18" s="69"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="88"/>
-      <c r="B19" s="80"/>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="82"/>
+      <c r="B19" s="86"/>
       <c r="C19" s="3" t="s">
-        <v>27</v>
+        <v>131</v>
       </c>
       <c r="D19" s="11">
         <v>1</v>
@@ -4376,9 +4424,9 @@
       <c r="G19" s="54"/>
       <c r="I19" s="69"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A20" s="88"/>
-      <c r="B20" s="84" t="s">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="82"/>
+      <c r="B20" s="78" t="s">
         <v>28</v>
       </c>
       <c r="C20" s="20" t="s">
@@ -4396,9 +4444,9 @@
       <c r="G20" s="50"/>
       <c r="I20" s="69"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21" s="88"/>
-      <c r="B21" s="87"/>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="82"/>
+      <c r="B21" s="88"/>
       <c r="C21" s="22" t="s">
         <v>31</v>
       </c>
@@ -4414,11 +4462,11 @@
       <c r="G21" s="51"/>
       <c r="I21" s="69"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A22" s="88"/>
-      <c r="B22" s="86"/>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="82"/>
+      <c r="B22" s="80"/>
       <c r="C22" s="7" t="s">
-        <v>30</v>
+        <v>134</v>
       </c>
       <c r="D22" s="9">
         <v>1</v>
@@ -4431,8 +4479,8 @@
       </c>
       <c r="G22" s="58"/>
     </row>
-    <row r="23" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A23" s="88"/>
+    <row r="23" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="82"/>
       <c r="B23" s="4" t="s">
         <v>17</v>
       </c>
@@ -4449,12 +4497,12 @@
         <v>1</v>
       </c>
       <c r="G23" s="75" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A24" s="88"/>
-      <c r="B24" s="84" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="82"/>
+      <c r="B24" s="78" t="s">
         <v>16</v>
       </c>
       <c r="C24" s="20" t="s">
@@ -4470,14 +4518,14 @@
         <v>1</v>
       </c>
       <c r="G24" s="76" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A25" s="88"/>
-      <c r="B25" s="87"/>
+        <v>123</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A25" s="82"/>
+      <c r="B25" s="88"/>
       <c r="C25" s="6" t="s">
-        <v>34</v>
+        <v>132</v>
       </c>
       <c r="D25" s="12">
         <v>0</v>
@@ -4489,10 +4537,10 @@
         <v>0</v>
       </c>
       <c r="G25" s="77" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="14"/>
       <c r="B26" s="14"/>
       <c r="C26" s="14"/>
@@ -4501,11 +4549,11 @@
       <c r="F26" s="36"/>
       <c r="G26" s="57"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="81" t="s">
         <v>1</v>
       </c>
-      <c r="B27" s="84" t="s">
+      <c r="B27" s="78" t="s">
         <v>35</v>
       </c>
       <c r="C27" s="20" t="s">
@@ -4523,9 +4571,9 @@
       <c r="G27" s="50"/>
       <c r="I27" s="69"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A28" s="82"/>
-      <c r="B28" s="85"/>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="89"/>
+      <c r="B28" s="79"/>
       <c r="C28" s="22" t="s">
         <v>50</v>
       </c>
@@ -4543,9 +4591,9 @@
       </c>
       <c r="I28" s="69"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A29" s="88"/>
-      <c r="B29" s="86"/>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="82"/>
+      <c r="B29" s="80"/>
       <c r="C29" s="7" t="s">
         <v>37</v>
       </c>
@@ -4561,9 +4609,9 @@
       <c r="G29" s="58"/>
       <c r="I29" s="69"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A30" s="88"/>
-      <c r="B30" s="78" t="s">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="82"/>
+      <c r="B30" s="84" t="s">
         <v>36</v>
       </c>
       <c r="C30" s="31" t="s">
@@ -4578,12 +4626,14 @@
       <c r="F30" s="32">
         <v>1</v>
       </c>
-      <c r="G30" s="53"/>
+      <c r="G30" s="53" t="s">
+        <v>101</v>
+      </c>
       <c r="I30" s="69"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A31" s="88"/>
-      <c r="B31" s="79"/>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="82"/>
+      <c r="B31" s="85"/>
       <c r="C31" s="27" t="s">
         <v>102</v>
       </c>
@@ -4599,9 +4649,9 @@
       <c r="G31" s="59"/>
       <c r="I31" s="69"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A32" s="88"/>
-      <c r="B32" s="80"/>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="82"/>
+      <c r="B32" s="86"/>
       <c r="C32" s="3" t="s">
         <v>103</v>
       </c>
@@ -4617,9 +4667,9 @@
       <c r="G32" s="54"/>
       <c r="I32" s="69"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A33" s="88"/>
-      <c r="B33" s="87" t="s">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="82"/>
+      <c r="B33" s="88" t="s">
         <v>16</v>
       </c>
       <c r="C33" s="20" t="s">
@@ -4637,9 +4687,9 @@
       <c r="G33" s="50"/>
       <c r="I33" s="69"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A34" s="88"/>
-      <c r="B34" s="87"/>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="82"/>
+      <c r="B34" s="88"/>
       <c r="C34" s="22" t="s">
         <v>112</v>
       </c>
@@ -4655,9 +4705,9 @@
       <c r="G34" s="51"/>
       <c r="I34" s="69"/>
     </row>
-    <row r="35" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="83"/>
-      <c r="B35" s="87"/>
+      <c r="B35" s="88"/>
       <c r="C35" s="15" t="s">
         <v>42</v>
       </c>
@@ -4673,7 +4723,7 @@
       <c r="G35" s="60"/>
       <c r="I35" s="69"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="14"/>
       <c r="B36" s="14"/>
       <c r="C36" s="14"/>
@@ -4683,11 +4733,11 @@
       <c r="G36" s="57"/>
       <c r="I36" s="69"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A37" s="89" t="s">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" s="90" t="s">
         <v>49</v>
       </c>
-      <c r="B37" s="84" t="s">
+      <c r="B37" s="78" t="s">
         <v>35</v>
       </c>
       <c r="C37" s="20" t="s">
@@ -4705,9 +4755,9 @@
       <c r="G37" s="50"/>
       <c r="I37" s="69"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A38" s="90"/>
-      <c r="B38" s="85"/>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" s="91"/>
+      <c r="B38" s="79"/>
       <c r="C38" s="22" t="s">
         <v>43</v>
       </c>
@@ -4723,9 +4773,9 @@
       <c r="G38" s="51"/>
       <c r="I38" s="69"/>
     </row>
-    <row r="39" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A39" s="88"/>
-      <c r="B39" s="86"/>
+    <row r="39" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A39" s="82"/>
+      <c r="B39" s="80"/>
       <c r="C39" s="17" t="s">
         <v>44</v>
       </c>
@@ -4741,13 +4791,13 @@
       <c r="G39" s="58"/>
       <c r="I39" s="69"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A40" s="88"/>
-      <c r="B40" s="78" t="s">
-        <v>130</v>
+    <row r="40" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="82"/>
+      <c r="B40" s="84" t="s">
+        <v>128</v>
       </c>
       <c r="C40" s="38" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D40" s="18">
         <v>1</v>
@@ -4761,27 +4811,27 @@
       <c r="G40" s="61"/>
       <c r="I40" s="69"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A41" s="88"/>
-      <c r="B41" s="80"/>
-      <c r="C41" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="D41" s="18">
-        <v>1</v>
-      </c>
-      <c r="E41" s="18">
-        <v>1</v>
-      </c>
-      <c r="F41" s="18">
-        <v>1</v>
-      </c>
-      <c r="G41" s="61"/>
-      <c r="I41" s="69"/>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A42" s="88"/>
-      <c r="B42" s="84" t="s">
+    <row r="41" spans="1:9" s="98" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="82"/>
+      <c r="B41" s="86"/>
+      <c r="C41" s="94" t="s">
+        <v>133</v>
+      </c>
+      <c r="D41" s="96">
+        <v>1</v>
+      </c>
+      <c r="E41" s="96">
+        <v>1</v>
+      </c>
+      <c r="F41" s="96">
+        <v>1</v>
+      </c>
+      <c r="G41" s="97"/>
+      <c r="I41" s="99"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" s="82"/>
+      <c r="B42" s="78" t="s">
         <v>36</v>
       </c>
       <c r="C42" s="20" t="s">
@@ -4799,9 +4849,9 @@
       <c r="G42" s="50"/>
       <c r="I42" s="69"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A43" s="88"/>
-      <c r="B43" s="85"/>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" s="82"/>
+      <c r="B43" s="79"/>
       <c r="C43" s="22" t="s">
         <v>45</v>
       </c>
@@ -4817,11 +4867,11 @@
       <c r="G43" s="51"/>
       <c r="I43" s="69"/>
     </row>
-    <row r="44" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A44" s="88"/>
-      <c r="B44" s="86"/>
+    <row r="44" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A44" s="82"/>
+      <c r="B44" s="80"/>
       <c r="C44" s="17" t="s">
-        <v>46</v>
+        <v>135</v>
       </c>
       <c r="D44" s="9">
         <v>1</v>
@@ -4835,7 +4885,7 @@
       <c r="G44" s="58"/>
       <c r="I44" s="69"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="83"/>
       <c r="B45" s="39" t="s">
         <v>16</v>
@@ -4855,7 +4905,7 @@
       <c r="G45" s="56"/>
       <c r="I45" s="69"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="14"/>
       <c r="B46" s="14"/>
       <c r="C46" s="14"/>
@@ -4865,11 +4915,11 @@
       <c r="G46" s="57"/>
       <c r="I46" s="69"/>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="81" t="s">
         <v>4</v>
       </c>
-      <c r="B47" s="84" t="s">
+      <c r="B47" s="78" t="s">
         <v>35</v>
       </c>
       <c r="C47" s="20" t="s">
@@ -4887,9 +4937,9 @@
       <c r="G47" s="50"/>
       <c r="I47" s="69"/>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A48" s="88"/>
-      <c r="B48" s="85"/>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" s="82"/>
+      <c r="B48" s="79"/>
       <c r="C48" s="22" t="s">
         <v>52</v>
       </c>
@@ -4905,9 +4955,9 @@
       <c r="G48" s="51"/>
       <c r="I48" s="69"/>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A49" s="88"/>
-      <c r="B49" s="85"/>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49" s="82"/>
+      <c r="B49" s="79"/>
       <c r="C49" s="22" t="s">
         <v>53</v>
       </c>
@@ -4923,9 +4973,9 @@
       <c r="G49" s="51"/>
       <c r="I49" s="69"/>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A50" s="88"/>
-      <c r="B50" s="86"/>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50" s="82"/>
+      <c r="B50" s="80"/>
       <c r="C50" s="7" t="s">
         <v>54</v>
       </c>
@@ -4941,9 +4991,9 @@
       <c r="G50" s="58"/>
       <c r="I50" s="69"/>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A51" s="88"/>
-      <c r="B51" s="79" t="s">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51" s="82"/>
+      <c r="B51" s="85" t="s">
         <v>36</v>
       </c>
       <c r="C51" s="27" t="s">
@@ -4961,9 +5011,9 @@
       <c r="G51" s="59"/>
       <c r="I51" s="69"/>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A52" s="88"/>
-      <c r="B52" s="79"/>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52" s="82"/>
+      <c r="B52" s="85"/>
       <c r="C52" s="33" t="s">
         <v>55</v>
       </c>
@@ -4979,9 +5029,9 @@
       <c r="G52" s="48"/>
       <c r="I52" s="69"/>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A53" s="88"/>
-      <c r="B53" s="79"/>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A53" s="82"/>
+      <c r="B53" s="85"/>
       <c r="C53" s="33" t="s">
         <v>56</v>
       </c>
@@ -4997,9 +5047,9 @@
       <c r="G53" s="48"/>
       <c r="I53" s="69"/>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A54" s="88"/>
-      <c r="B54" s="80"/>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A54" s="82"/>
+      <c r="B54" s="86"/>
       <c r="C54" s="3" t="s">
         <v>57</v>
       </c>
@@ -5015,9 +5065,9 @@
       <c r="G54" s="54"/>
       <c r="I54" s="69"/>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A55" s="88"/>
-      <c r="B55" s="87" t="s">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A55" s="82"/>
+      <c r="B55" s="88" t="s">
         <v>16</v>
       </c>
       <c r="C55" s="24" t="s">
@@ -5035,9 +5085,9 @@
       <c r="G55" s="52"/>
       <c r="I55" s="69"/>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="83"/>
-      <c r="B56" s="87"/>
+      <c r="B56" s="88"/>
       <c r="C56" s="16" t="s">
         <v>59</v>
       </c>
@@ -5053,7 +5103,7 @@
       <c r="G56" s="60"/>
       <c r="I56" s="69"/>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="14"/>
       <c r="B57" s="14"/>
       <c r="C57" s="14"/>
@@ -5063,11 +5113,11 @@
       <c r="G57" s="57"/>
       <c r="I57" s="69"/>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="81" t="s">
         <v>3</v>
       </c>
-      <c r="B58" s="84" t="s">
+      <c r="B58" s="78" t="s">
         <v>35</v>
       </c>
       <c r="C58" s="20" t="s">
@@ -5085,10 +5135,10 @@
       <c r="G58" s="50"/>
       <c r="I58" s="69"/>
     </row>
-    <row r="59" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A59" s="88"/>
-      <c r="B59" s="85"/>
-      <c r="C59" s="43" t="s">
+    <row r="59" spans="1:9" s="95" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="82"/>
+      <c r="B59" s="79"/>
+      <c r="C59" s="100" t="s">
         <v>62</v>
       </c>
       <c r="D59" s="23">
@@ -5105,9 +5155,9 @@
       </c>
       <c r="I59" s="69"/>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A60" s="88"/>
-      <c r="B60" s="85"/>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A60" s="82"/>
+      <c r="B60" s="79"/>
       <c r="C60" s="22" t="s">
         <v>63</v>
       </c>
@@ -5123,9 +5173,9 @@
       <c r="G60" s="51"/>
       <c r="I60" s="69"/>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A61" s="88"/>
-      <c r="B61" s="86"/>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A61" s="82"/>
+      <c r="B61" s="80"/>
       <c r="C61" s="7" t="s">
         <v>64</v>
       </c>
@@ -5141,9 +5191,9 @@
       <c r="G61" s="58"/>
       <c r="I61" s="69"/>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A62" s="88"/>
-      <c r="B62" s="78" t="s">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A62" s="82"/>
+      <c r="B62" s="84" t="s">
         <v>36</v>
       </c>
       <c r="C62" s="31" t="s">
@@ -5161,9 +5211,9 @@
       <c r="G62" s="53"/>
       <c r="I62" s="69"/>
     </row>
-    <row r="63" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A63" s="88"/>
-      <c r="B63" s="79"/>
+    <row r="63" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A63" s="82"/>
+      <c r="B63" s="85"/>
       <c r="C63" s="44" t="s">
         <v>65</v>
       </c>
@@ -5181,9 +5231,9 @@
       </c>
       <c r="I63" s="69"/>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A64" s="88"/>
-      <c r="B64" s="79"/>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A64" s="82"/>
+      <c r="B64" s="85"/>
       <c r="C64" s="33" t="s">
         <v>66</v>
       </c>
@@ -5199,9 +5249,9 @@
       <c r="G64" s="48"/>
       <c r="I64" s="69"/>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A65" s="88"/>
-      <c r="B65" s="80"/>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A65" s="82"/>
+      <c r="B65" s="86"/>
       <c r="C65" s="3" t="s">
         <v>67</v>
       </c>
@@ -5217,8 +5267,8 @@
       <c r="G65" s="54"/>
       <c r="I65" s="69"/>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A66" s="88"/>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A66" s="82"/>
       <c r="B66" s="92" t="s">
         <v>120</v>
       </c>
@@ -5237,9 +5287,9 @@
       <c r="G66" s="50"/>
       <c r="I66" s="69"/>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A67" s="88"/>
-      <c r="B67" s="85"/>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A67" s="82"/>
+      <c r="B67" s="79"/>
       <c r="C67" s="22" t="s">
         <v>69</v>
       </c>
@@ -5255,9 +5305,9 @@
       <c r="G67" s="51"/>
       <c r="I67" s="69"/>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A68" s="88"/>
-      <c r="B68" s="86"/>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A68" s="82"/>
+      <c r="B68" s="80"/>
       <c r="C68" s="7" t="s">
         <v>70</v>
       </c>
@@ -5273,10 +5323,10 @@
       <c r="G68" s="58"/>
       <c r="I68" s="69"/>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A69" s="88"/>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A69" s="82"/>
       <c r="B69" s="93" t="s">
-        <v>121</v>
+        <v>136</v>
       </c>
       <c r="C69" s="31" t="s">
         <v>71</v>
@@ -5293,9 +5343,9 @@
       <c r="G69" s="53"/>
       <c r="I69" s="69"/>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A70" s="88"/>
-      <c r="B70" s="91"/>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A70" s="82"/>
+      <c r="B70" s="87"/>
       <c r="C70" s="33" t="s">
         <v>72</v>
       </c>
@@ -5311,9 +5361,9 @@
       <c r="G70" s="48"/>
       <c r="I70" s="69"/>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A71" s="88"/>
-      <c r="B71" s="79"/>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A71" s="82"/>
+      <c r="B71" s="85"/>
       <c r="C71" s="40" t="s">
         <v>73</v>
       </c>
@@ -5329,9 +5379,9 @@
       <c r="G71" s="61"/>
       <c r="I71" s="69"/>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A72" s="88"/>
-      <c r="B72" s="84" t="s">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A72" s="82"/>
+      <c r="B72" s="78" t="s">
         <v>16</v>
       </c>
       <c r="C72" s="20" t="s">
@@ -5349,10 +5399,10 @@
       <c r="G72" s="50"/>
       <c r="I72" s="69"/>
     </row>
-    <row r="73" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A73" s="88"/>
-      <c r="B73" s="85"/>
-      <c r="C73" s="43" t="s">
+    <row r="73" spans="1:9" s="95" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="82"/>
+      <c r="B73" s="79"/>
+      <c r="C73" s="100" t="s">
         <v>76</v>
       </c>
       <c r="D73" s="23">
@@ -5367,10 +5417,10 @@
       <c r="G73" s="51"/>
       <c r="I73" s="69"/>
     </row>
-    <row r="74" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:9" s="95" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="83"/>
-      <c r="B74" s="86"/>
-      <c r="C74" s="17" t="s">
+      <c r="B74" s="80"/>
+      <c r="C74" s="101" t="s">
         <v>77</v>
       </c>
       <c r="D74" s="9">
@@ -5385,7 +5435,7 @@
       <c r="G74" s="58"/>
       <c r="I74" s="69"/>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" s="14"/>
       <c r="B75" s="14"/>
       <c r="C75" s="14"/>
@@ -5395,11 +5445,11 @@
       <c r="G75" s="57"/>
       <c r="I75" s="69"/>
     </row>
-    <row r="76" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="81" t="s">
         <v>2</v>
       </c>
-      <c r="B76" s="84" t="s">
+      <c r="B76" s="78" t="s">
         <v>35</v>
       </c>
       <c r="C76" s="20" t="s">
@@ -5419,9 +5469,9 @@
       </c>
       <c r="I76" s="69"/>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A77" s="82"/>
-      <c r="B77" s="85"/>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A77" s="89"/>
+      <c r="B77" s="79"/>
       <c r="C77" s="22" t="s">
         <v>79</v>
       </c>
@@ -5439,9 +5489,9 @@
       </c>
       <c r="I77" s="69"/>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A78" s="82"/>
-      <c r="B78" s="85"/>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A78" s="89"/>
+      <c r="B78" s="79"/>
       <c r="C78" s="22" t="s">
         <v>80</v>
       </c>
@@ -5457,9 +5507,9 @@
       <c r="G78" s="51"/>
       <c r="I78" s="69"/>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A79" s="82"/>
-      <c r="B79" s="85"/>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A79" s="89"/>
+      <c r="B79" s="79"/>
       <c r="C79" s="22" t="s">
         <v>81</v>
       </c>
@@ -5475,9 +5525,9 @@
       <c r="G79" s="51"/>
       <c r="I79" s="69"/>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A80" s="82"/>
-      <c r="B80" s="85"/>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A80" s="89"/>
+      <c r="B80" s="79"/>
       <c r="C80" s="22" t="s">
         <v>83</v>
       </c>
@@ -5495,9 +5545,9 @@
       </c>
       <c r="I80" s="69"/>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A81" s="82"/>
-      <c r="B81" s="85"/>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A81" s="89"/>
+      <c r="B81" s="79"/>
       <c r="C81" s="22" t="s">
         <v>84</v>
       </c>
@@ -5515,9 +5565,9 @@
       </c>
       <c r="I81" s="69"/>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A82" s="82"/>
-      <c r="B82" s="85"/>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A82" s="89"/>
+      <c r="B82" s="79"/>
       <c r="C82" s="22" t="s">
         <v>85</v>
       </c>
@@ -5533,9 +5583,9 @@
       <c r="G82" s="51"/>
       <c r="I82" s="69"/>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A83" s="82"/>
-      <c r="B83" s="86"/>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A83" s="89"/>
+      <c r="B83" s="80"/>
       <c r="C83" s="7" t="s">
         <v>82</v>
       </c>
@@ -5551,9 +5601,9 @@
       <c r="G83" s="58"/>
       <c r="I83" s="69"/>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A84" s="82"/>
-      <c r="B84" s="78" t="s">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A84" s="89"/>
+      <c r="B84" s="84" t="s">
         <v>36</v>
       </c>
       <c r="C84" s="31" t="s">
@@ -5573,11 +5623,11 @@
       </c>
       <c r="I84" s="69"/>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A85" s="82"/>
-      <c r="B85" s="91"/>
-      <c r="C85" s="27" t="s">
-        <v>87</v>
+    <row r="85" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A85" s="89"/>
+      <c r="B85" s="87"/>
+      <c r="C85" s="102" t="s">
+        <v>137</v>
       </c>
       <c r="D85" s="28">
         <v>0</v>
@@ -5593,9 +5643,9 @@
       </c>
       <c r="I85" s="69"/>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A86" s="82"/>
-      <c r="B86" s="91"/>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A86" s="89"/>
+      <c r="B86" s="87"/>
       <c r="C86" s="27" t="s">
         <v>88</v>
       </c>
@@ -5611,9 +5661,9 @@
       <c r="G86" s="59"/>
       <c r="I86" s="69"/>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A87" s="82"/>
-      <c r="B87" s="91"/>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A87" s="89"/>
+      <c r="B87" s="87"/>
       <c r="C87" s="27" t="s">
         <v>89</v>
       </c>
@@ -5629,9 +5679,9 @@
       <c r="G87" s="59"/>
       <c r="I87" s="69"/>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A88" s="82"/>
-      <c r="B88" s="91"/>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A88" s="89"/>
+      <c r="B88" s="87"/>
       <c r="C88" s="27" t="s">
         <v>90</v>
       </c>
@@ -5649,11 +5699,11 @@
       </c>
       <c r="I88" s="69"/>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A89" s="82"/>
-      <c r="B89" s="91"/>
-      <c r="C89" s="27" t="s">
-        <v>91</v>
+    <row r="89" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A89" s="89"/>
+      <c r="B89" s="87"/>
+      <c r="C89" s="102" t="s">
+        <v>138</v>
       </c>
       <c r="D89" s="28">
         <v>0</v>
@@ -5669,9 +5719,9 @@
       </c>
       <c r="I89" s="69"/>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A90" s="82"/>
-      <c r="B90" s="91"/>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A90" s="89"/>
+      <c r="B90" s="87"/>
       <c r="C90" s="27" t="s">
         <v>92</v>
       </c>
@@ -5687,9 +5737,9 @@
       <c r="G90" s="59"/>
       <c r="I90" s="69"/>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A91" s="82"/>
-      <c r="B91" s="80"/>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A91" s="89"/>
+      <c r="B91" s="86"/>
       <c r="C91" s="3" t="s">
         <v>93</v>
       </c>
@@ -5705,9 +5755,9 @@
       <c r="G91" s="54"/>
       <c r="I91" s="67"/>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A92" s="82"/>
-      <c r="B92" s="84" t="s">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A92" s="89"/>
+      <c r="B92" s="78" t="s">
         <v>16</v>
       </c>
       <c r="C92" s="20" t="s">
@@ -5725,9 +5775,9 @@
       <c r="G92" s="50"/>
       <c r="I92" s="67"/>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A93" s="82"/>
-      <c r="B93" s="86"/>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A93" s="89"/>
+      <c r="B93" s="80"/>
       <c r="C93" s="6" t="s">
         <v>95</v>
       </c>
@@ -5743,9 +5793,9 @@
       <c r="G93" s="60"/>
       <c r="I93" s="67"/>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A94" s="82"/>
-      <c r="B94" s="78" t="s">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A94" s="89"/>
+      <c r="B94" s="84" t="s">
         <v>107</v>
       </c>
       <c r="C94" s="31" t="s">
@@ -5763,9 +5813,9 @@
       <c r="G94" s="53"/>
       <c r="I94" s="67"/>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A95" s="82"/>
-      <c r="B95" s="79"/>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A95" s="89"/>
+      <c r="B95" s="85"/>
       <c r="C95" s="33" t="s">
         <v>113</v>
       </c>
@@ -5781,9 +5831,9 @@
       <c r="G95" s="48"/>
       <c r="I95" s="67"/>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A96" s="82"/>
-      <c r="B96" s="79"/>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A96" s="89"/>
+      <c r="B96" s="85"/>
       <c r="C96" s="33" t="s">
         <v>109</v>
       </c>
@@ -5798,9 +5848,9 @@
       </c>
       <c r="G96" s="48"/>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" s="83"/>
-      <c r="B97" s="80"/>
+      <c r="B97" s="86"/>
       <c r="C97" s="40" t="s">
         <v>114</v>
       </c>
@@ -5815,7 +5865,7 @@
       </c>
       <c r="G97" s="61"/>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" s="14"/>
       <c r="B98" s="14"/>
       <c r="C98" s="14"/>
@@ -5826,6 +5876,25 @@
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="A76:A97"/>
+    <mergeCell ref="B76:B83"/>
+    <mergeCell ref="B84:B91"/>
+    <mergeCell ref="B92:B93"/>
+    <mergeCell ref="B94:B97"/>
+    <mergeCell ref="A58:A74"/>
+    <mergeCell ref="B58:B61"/>
+    <mergeCell ref="B62:B65"/>
+    <mergeCell ref="B66:B68"/>
+    <mergeCell ref="B69:B71"/>
+    <mergeCell ref="B72:B74"/>
+    <mergeCell ref="A37:A45"/>
+    <mergeCell ref="B37:B39"/>
+    <mergeCell ref="B40:B41"/>
+    <mergeCell ref="B42:B44"/>
+    <mergeCell ref="A47:A56"/>
+    <mergeCell ref="B47:B50"/>
+    <mergeCell ref="B51:B54"/>
+    <mergeCell ref="B55:B56"/>
     <mergeCell ref="A27:A35"/>
     <mergeCell ref="B27:B29"/>
     <mergeCell ref="B30:B32"/>
@@ -5835,25 +5904,6 @@
     <mergeCell ref="B11:B19"/>
     <mergeCell ref="B20:B22"/>
     <mergeCell ref="B24:B25"/>
-    <mergeCell ref="A37:A45"/>
-    <mergeCell ref="B37:B39"/>
-    <mergeCell ref="B40:B41"/>
-    <mergeCell ref="B42:B44"/>
-    <mergeCell ref="A47:A56"/>
-    <mergeCell ref="B47:B50"/>
-    <mergeCell ref="B51:B54"/>
-    <mergeCell ref="B55:B56"/>
-    <mergeCell ref="A58:A74"/>
-    <mergeCell ref="B58:B61"/>
-    <mergeCell ref="B62:B65"/>
-    <mergeCell ref="B66:B68"/>
-    <mergeCell ref="B69:B71"/>
-    <mergeCell ref="B72:B74"/>
-    <mergeCell ref="A76:A97"/>
-    <mergeCell ref="B76:B83"/>
-    <mergeCell ref="B84:B91"/>
-    <mergeCell ref="B92:B93"/>
-    <mergeCell ref="B94:B97"/>
   </mergeCells>
   <conditionalFormatting sqref="D99:F1048576 D69:F74 D3:F3 D76:E93 D10:F10 D4:E9 D18:F26 D11:E17 D36:F36 D27:E35 D46:F46 D37:E45 D47:E56 D58:E68">
     <cfRule type="iconSet" priority="17">

</xml_diff>